<commit_message>
Introduced modification to intentionally trigger Toolbox-Test
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -136,7 +136,7 @@
     <t xml:space="preserve">ESG Ziele</t>
   </si>
   <si>
-    <t xml:space="preserve">Existenz von ESG-Zielen</t>
+    <t xml:space="preserve">Existenz von Unternehmensspezifischen ESG-Zielen</t>
   </si>
   <si>
     <t xml:space="preserve">Hat das Unternehmen spezifische ESG-Ziele / Engagements? Werden bspw. spezifische Ziele / Maßnahmen ergriffen, um das 1,5 Grad Ziel zu erreichen?</t>
@@ -1827,48 +1827,48 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2314,7 +2314,7 @@
   <dimension ref="A1:M121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2331,7 +2331,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="12.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -2388,21 +2388,21 @@
       <c r="E2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -2411,194 +2411,194 @@
       <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="21" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="21"/>
-    </row>
-    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="12"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="21" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="15"/>
-    </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -2607,29 +2607,29 @@
       <c r="E9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -2638,204 +2638,204 @@
       <c r="E10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="21"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="13" t="s">
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="12" t="s">
         <v>66</v>
       </c>
       <c r="K12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="13" t="s">
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="12" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="13" t="s">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="12" t="s">
         <v>66</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>76</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="13" t="s">
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="12" t="s">
         <v>66</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -2844,351 +2844,351 @@
       <c r="E16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>60</v>
       </c>
       <c r="H16" s="10"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="21"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="20"/>
       <c r="K16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="21"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>87</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="16" t="s">
         <v>60</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="21"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="21"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
         <v>94</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="17"/>
-    </row>
-    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
         <v>98</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="21"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L21" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>103</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L22" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="21" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L23" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="21" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
       <c r="K24" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="15"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
         <v>111</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="21" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="15"/>
-    </row>
-    <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L26" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D27" s="10" t="s">
@@ -3197,33 +3197,33 @@
       <c r="E27" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H27" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L27" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="15"/>
-    </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L27" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
         <v>123</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -3232,95 +3232,95 @@
       <c r="E28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H28" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L28" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="15"/>
-    </row>
-    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="14"/>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>128</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="21" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
       <c r="K29" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L29" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="15"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
         <v>131</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="21" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="15"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
       <c r="K30" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L30" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="15"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
         <v>134</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>128</v>
       </c>
       <c r="D31" s="10" t="s">
@@ -3329,95 +3329,95 @@
       <c r="E31" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="21" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="15"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
       <c r="K31" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="L31" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="15"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>139</v>
       </c>
       <c r="E32" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="15"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="L32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="15"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
         <v>142</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="21" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="15"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
       <c r="K33" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L33" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="15"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L33" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
         <v>145</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>128</v>
       </c>
       <c r="D34" s="10" t="s">
@@ -3426,95 +3426,95 @@
       <c r="E34" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="21" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I34" s="14"/>
-      <c r="J34" s="15"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
       <c r="K34" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="L34" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="15"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
         <v>148</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>149</v>
       </c>
       <c r="E35" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="15"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
       <c r="K35" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="L35" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" s="15"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L35" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="21" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="15"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
       <c r="K36" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L36" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="15"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L36" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
         <v>153</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>128</v>
       </c>
       <c r="D37" s="10" t="s">
@@ -3523,252 +3523,252 @@
       <c r="E37" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="21" t="s">
+      <c r="F37" s="10"/>
+      <c r="G37" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="15"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
       <c r="K37" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="L37" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="15"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L37" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E38" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="15"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="14"/>
       <c r="K38" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="L38" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" s="15"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
         <v>158</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="21" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="15"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="14"/>
       <c r="K39" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L39" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M39" s="15"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
         <v>162</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="21" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="15"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="14"/>
       <c r="K40" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" s="15"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L40" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="21" t="s">
+      <c r="F41" s="10"/>
+      <c r="G41" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="21"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="20"/>
       <c r="K41" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L41" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" s="15"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L41" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="s">
         <v>169</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="21" t="s">
+      <c r="F42" s="10"/>
+      <c r="G42" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="21" t="s">
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="20" t="s">
         <v>66</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L42" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M42" s="15"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L42" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
         <v>172</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="21" t="s">
         <v>159</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="21" t="s">
+      <c r="F43" s="10"/>
+      <c r="G43" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="15"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
       <c r="K43" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L43" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M43" s="15"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L43" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
         <v>175</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="21" t="s">
         <v>176</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="F44" s="12"/>
-      <c r="G44" s="21" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="15"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="14"/>
       <c r="K44" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L44" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M44" s="15"/>
-    </row>
-    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L44" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="14"/>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="21" t="s">
         <v>176</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -3777,62 +3777,62 @@
       <c r="E45" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G45" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="15"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
       <c r="K45" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="L45" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L45" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="21" t="s">
         <v>176</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="21" t="s">
+      <c r="F46" s="10"/>
+      <c r="G46" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="15"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="14"/>
       <c r="K46" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="15"/>
-    </row>
-    <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L46" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
         <v>187</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="21" t="s">
         <v>176</v>
       </c>
       <c r="D47" s="10" t="s">
@@ -3841,31 +3841,31 @@
       <c r="E47" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G47" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="15"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
       <c r="K47" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="L47" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M47" s="15"/>
-    </row>
-    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
         <v>190</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="21" t="s">
         <v>191</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -3874,55 +3874,55 @@
       <c r="E48" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="15"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="14"/>
       <c r="K48" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L48" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M48" s="15"/>
-    </row>
-    <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
         <v>195</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>191</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="21" t="s">
+      <c r="F49" s="10"/>
+      <c r="G49" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="15"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="14"/>
       <c r="K49" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L49" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M49" s="15"/>
-    </row>
-    <row r="50" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L49" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
         <v>198</v>
       </c>
@@ -3938,24 +3938,24 @@
       <c r="E50" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="G50" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="15"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="14"/>
       <c r="K50" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L50" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M50" s="15"/>
-    </row>
-    <row r="51" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L50" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
         <v>205</v>
       </c>
@@ -3965,28 +3965,28 @@
       <c r="C51" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="21" t="s">
+      <c r="F51" s="10"/>
+      <c r="G51" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="15"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="14"/>
       <c r="K51" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L51" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M51" s="15"/>
-    </row>
-    <row r="52" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L51" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
         <v>208</v>
       </c>
@@ -3999,120 +3999,120 @@
       <c r="D52" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="15"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="14"/>
       <c r="K52" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L52" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M52" s="15"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L52" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
         <v>212</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>213</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="21" t="s">
+      <c r="F53" s="10"/>
+      <c r="G53" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="15"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="14"/>
       <c r="K53" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L53" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="15"/>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L53" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="s">
         <v>216</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="21" t="s">
         <v>213</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="G54" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="15"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="14"/>
       <c r="K54" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="L54" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="15"/>
-    </row>
-    <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L54" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="14"/>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="s">
         <v>220</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>213</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="21" t="s">
+      <c r="F55" s="10"/>
+      <c r="G55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="15"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="14"/>
       <c r="K55" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L55" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="15"/>
+      <c r="L55" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="28" t="s">
@@ -4130,24 +4130,24 @@
       <c r="E56" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="G56" s="13" t="s">
+      <c r="G56" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="15"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="14"/>
       <c r="K56" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L56" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="15"/>
-    </row>
-    <row r="57" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
         <v>228</v>
       </c>
@@ -4157,28 +4157,28 @@
       <c r="C57" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>229</v>
       </c>
       <c r="E57" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="15"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="14"/>
       <c r="K57" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L57" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M57" s="15"/>
+      <c r="L57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
@@ -4196,24 +4196,24 @@
       <c r="E58" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G58" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="15"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="14"/>
       <c r="K58" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L58" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L58" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="14"/>
+    </row>
+    <row r="59" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
         <v>237</v>
       </c>
@@ -4229,24 +4229,24 @@
       <c r="E59" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="15"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="14"/>
       <c r="K59" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L59" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="15"/>
-    </row>
-    <row r="60" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L59" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="14"/>
+    </row>
+    <row r="60" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
         <v>239</v>
       </c>
@@ -4262,24 +4262,24 @@
       <c r="E60" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="G60" s="13" t="s">
+      <c r="G60" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="15"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="14"/>
       <c r="K60" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L60" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M60" s="15"/>
-    </row>
-    <row r="61" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L60" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="14"/>
+    </row>
+    <row r="61" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
         <v>244</v>
       </c>
@@ -4295,24 +4295,24 @@
       <c r="E61" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="15"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="14"/>
       <c r="K61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L61" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M61" s="15"/>
-    </row>
-    <row r="62" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L61" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M61" s="14"/>
+    </row>
+    <row r="62" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
         <v>246</v>
       </c>
@@ -4328,24 +4328,24 @@
       <c r="E62" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G62" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="15"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="14"/>
       <c r="K62" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L62" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M62" s="15"/>
-    </row>
-    <row r="63" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L62" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62" s="14"/>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
         <v>251</v>
       </c>
@@ -4361,24 +4361,24 @@
       <c r="E63" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="15"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="14"/>
       <c r="K63" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L63" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M63" s="15"/>
-    </row>
-    <row r="64" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L63" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
         <v>253</v>
       </c>
@@ -4394,24 +4394,24 @@
       <c r="E64" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G64" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="15"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="14"/>
       <c r="K64" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L64" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M64" s="15"/>
-    </row>
-    <row r="65" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L64" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="14"/>
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
         <v>257</v>
       </c>
@@ -4424,56 +4424,56 @@
       <c r="D65" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="F65" s="12"/>
-      <c r="G65" s="21" t="s">
+      <c r="F65" s="10"/>
+      <c r="G65" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="15"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="14"/>
       <c r="K65" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L65" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M65" s="15"/>
-    </row>
-    <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L65" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="16" t="s">
         <v>261</v>
       </c>
       <c r="D66" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="F66" s="12"/>
-      <c r="G66" s="21" t="s">
+      <c r="F66" s="10"/>
+      <c r="G66" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="15"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="14"/>
       <c r="K66" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L66" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M66" s="15"/>
-    </row>
-    <row r="67" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L66" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
         <v>264</v>
       </c>
@@ -4486,58 +4486,58 @@
       <c r="D67" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="G67" s="21" t="s">
+      <c r="G67" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="15"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="14"/>
       <c r="K67" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="L67" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M67" s="15"/>
-    </row>
-    <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L67" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="16" t="s">
         <v>261</v>
       </c>
       <c r="D68" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="F68" s="12"/>
-      <c r="G68" s="21" t="s">
+      <c r="F68" s="10"/>
+      <c r="G68" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="15"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="14"/>
       <c r="K68" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L68" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M68" s="15"/>
-    </row>
-    <row r="69" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L68" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" s="14"/>
+    </row>
+    <row r="69" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="s">
         <v>271</v>
       </c>
@@ -4550,27 +4550,27 @@
       <c r="D69" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="G69" s="21" t="s">
+      <c r="G69" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="15"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="14"/>
       <c r="K69" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="L69" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M69" s="15"/>
-    </row>
-    <row r="70" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L69" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M69" s="14"/>
+    </row>
+    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="s">
         <v>275</v>
       </c>
@@ -4583,25 +4583,25 @@
       <c r="D70" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="F70" s="12"/>
-      <c r="G70" s="21" t="s">
+      <c r="F70" s="10"/>
+      <c r="G70" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="15"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="14"/>
       <c r="K70" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L70" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M70" s="15"/>
-    </row>
-    <row r="71" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L70" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M70" s="14"/>
+    </row>
+    <row r="71" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
         <v>279</v>
       </c>
@@ -4617,24 +4617,24 @@
       <c r="E71" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G71" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="15"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="14"/>
       <c r="K71" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="L71" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M71" s="15"/>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L71" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
         <v>283</v>
       </c>
@@ -4650,24 +4650,24 @@
       <c r="E72" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="F72" s="12"/>
-      <c r="G72" s="21" t="s">
+      <c r="F72" s="10"/>
+      <c r="G72" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H72" s="21" t="s">
+      <c r="H72" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="I72" s="14"/>
-      <c r="J72" s="15"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="14"/>
       <c r="K72" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L72" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M72" s="15"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L72" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
         <v>288</v>
       </c>
@@ -4680,25 +4680,25 @@
       <c r="D73" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="F73" s="12"/>
-      <c r="G73" s="21" t="s">
+      <c r="F73" s="10"/>
+      <c r="G73" s="20" t="s">
         <v>291</v>
       </c>
       <c r="H73" s="10"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="15"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="14"/>
       <c r="K73" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L73" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M73" s="15"/>
-    </row>
-    <row r="74" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L73" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
         <v>292</v>
       </c>
@@ -4714,24 +4714,24 @@
       <c r="E74" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="G74" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="15"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="14"/>
       <c r="K74" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L74" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M74" s="15"/>
-    </row>
-    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L74" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
         <v>296</v>
       </c>
@@ -4744,230 +4744,230 @@
       <c r="D75" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="21" t="s">
+      <c r="F75" s="10"/>
+      <c r="G75" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="15"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="14"/>
       <c r="K75" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L75" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M75" s="15"/>
-    </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L75" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="s">
         <v>301</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="22" t="s">
+      <c r="C76" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="G76" s="21" t="s">
+      <c r="G76" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="15"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="14"/>
       <c r="K76" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L76" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M76" s="15"/>
-    </row>
-    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L76" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
         <v>306</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C77" s="22" t="s">
+      <c r="C77" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="G77" s="21" t="s">
+      <c r="G77" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="15"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="14"/>
       <c r="K77" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L77" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M77" s="15"/>
-    </row>
-    <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L77" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
         <v>310</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C78" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="G78" s="21" t="s">
+      <c r="G78" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="15"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="14"/>
       <c r="K78" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L78" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M78" s="15"/>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L78" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
         <v>314</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C79" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E79" s="12" t="s">
+      <c r="E79" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="G79" s="21" t="s">
+      <c r="G79" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="15"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="14"/>
       <c r="K79" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L79" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M79" s="15"/>
-    </row>
-    <row r="80" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L79" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
         <v>318</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E80" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="G80" s="21" t="s">
+      <c r="G80" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="15"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="14"/>
       <c r="K80" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L80" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M80" s="15"/>
-    </row>
-    <row r="81" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L80" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
         <v>322</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D81" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="E81" s="12" t="s">
+      <c r="E81" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="F81" s="12" t="s">
+      <c r="F81" s="22" t="s">
         <v>325</v>
       </c>
-      <c r="G81" s="21" t="s">
+      <c r="G81" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="15"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="14"/>
       <c r="K81" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L81" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M81" s="15"/>
-    </row>
-    <row r="82" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L81" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="s">
         <v>326</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C82" s="21" t="s">
         <v>298</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -4976,24 +4976,24 @@
       <c r="E82" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="G82" s="13" t="s">
+      <c r="G82" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="15"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="14"/>
       <c r="K82" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L82" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M82" s="15"/>
-    </row>
-    <row r="83" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L82" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="s">
         <v>331</v>
       </c>
@@ -5006,29 +5006,29 @@
       <c r="D83" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E83" s="12" t="s">
+      <c r="E83" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="F83" s="12"/>
-      <c r="G83" s="21" t="s">
+      <c r="F83" s="10"/>
+      <c r="G83" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="15"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="14"/>
       <c r="K83" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L83" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M83" s="15"/>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L83" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="16" t="s">
         <v>297</v>
       </c>
       <c r="C84" s="47" t="s">
@@ -5040,22 +5040,22 @@
       <c r="E84" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="F84" s="12"/>
-      <c r="G84" s="13" t="s">
+      <c r="F84" s="10"/>
+      <c r="G84" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="15"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="14"/>
       <c r="K84" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L84" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M84" s="15"/>
-    </row>
-    <row r="85" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L84" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
         <v>338</v>
       </c>
@@ -5071,24 +5071,24 @@
       <c r="E85" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="G85" s="13" t="s">
+      <c r="G85" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="15"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="14"/>
       <c r="K85" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L85" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M85" s="15"/>
-    </row>
-    <row r="86" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L85" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M85" s="14"/>
+    </row>
+    <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
         <v>342</v>
       </c>
@@ -5104,24 +5104,24 @@
       <c r="E86" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="G86" s="13" t="s">
+      <c r="G86" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="15"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="14"/>
       <c r="K86" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L86" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M86" s="15"/>
-    </row>
-    <row r="87" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L86" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M86" s="14"/>
+    </row>
+    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
         <v>347</v>
       </c>
@@ -5134,25 +5134,25 @@
       <c r="D87" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="E87" s="12" t="s">
+      <c r="E87" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="F87" s="12"/>
-      <c r="G87" s="21" t="s">
+      <c r="F87" s="10"/>
+      <c r="G87" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="15"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="14"/>
       <c r="K87" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L87" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M87" s="15"/>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L87" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M87" s="14"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
         <v>350</v>
       </c>
@@ -5168,24 +5168,24 @@
       <c r="E88" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G88" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="15"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="14"/>
       <c r="K88" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L88" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M88" s="15"/>
-    </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L88" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M88" s="14"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
         <v>355</v>
       </c>
@@ -5201,24 +5201,24 @@
       <c r="E89" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G89" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="15"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="14"/>
       <c r="K89" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L89" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L89" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M89" s="14"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="50" t="s">
         <v>359</v>
       </c>
@@ -5234,24 +5234,24 @@
       <c r="E90" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="G90" s="13" t="s">
+      <c r="G90" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="15"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="14"/>
       <c r="K90" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L90" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M90" s="15"/>
-    </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L90" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M90" s="14"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="50" t="s">
         <v>363</v>
       </c>
@@ -5267,24 +5267,24 @@
       <c r="E91" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="F91" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="G91" s="13" t="s">
+      <c r="G91" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="15"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="14"/>
       <c r="K91" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L91" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M91" s="15"/>
-    </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L91" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M91" s="14"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="50" t="s">
         <v>367</v>
       </c>
@@ -5297,27 +5297,27 @@
       <c r="D92" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E92" s="12" t="s">
+      <c r="E92" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F92" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="G92" s="21" t="s">
+      <c r="G92" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="15"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="14"/>
       <c r="K92" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L92" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M92" s="15"/>
-    </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L92" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M92" s="14"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="50" t="s">
         <v>371</v>
       </c>
@@ -5333,22 +5333,22 @@
       <c r="E93" s="46" t="s">
         <v>373</v>
       </c>
-      <c r="F93" s="12"/>
-      <c r="G93" s="21" t="s">
+      <c r="F93" s="10"/>
+      <c r="G93" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="15"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="14"/>
       <c r="K93" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L93" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M93" s="15"/>
-    </row>
-    <row r="94" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L93" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M93" s="14"/>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="50" t="s">
         <v>374</v>
       </c>
@@ -5361,25 +5361,25 @@
       <c r="D94" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="E94" s="12" t="s">
+      <c r="E94" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="F94" s="12"/>
-      <c r="G94" s="21" t="s">
+      <c r="F94" s="10"/>
+      <c r="G94" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H94" s="14"/>
-      <c r="I94" s="14"/>
-      <c r="J94" s="15"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="14"/>
       <c r="K94" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L94" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M94" s="15"/>
-    </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L94" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="50" t="s">
         <v>378</v>
       </c>
@@ -5395,24 +5395,24 @@
       <c r="E95" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="F95" s="12"/>
-      <c r="G95" s="21" t="s">
+      <c r="F95" s="10"/>
+      <c r="G95" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H95" s="52" t="s">
         <v>381</v>
       </c>
-      <c r="I95" s="14"/>
-      <c r="J95" s="15"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="14"/>
       <c r="K95" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="L95" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M95" s="15"/>
-    </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L95" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M95" s="14"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="50" t="s">
         <v>382</v>
       </c>
@@ -5428,24 +5428,24 @@
       <c r="E96" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="G96" s="21" t="s">
+      <c r="G96" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H96" s="14"/>
-      <c r="I96" s="14"/>
-      <c r="J96" s="15"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="14"/>
       <c r="K96" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="L96" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M96" s="15"/>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L96" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="50" t="s">
         <v>386</v>
       </c>
@@ -5461,22 +5461,22 @@
       <c r="E97" s="54" t="s">
         <v>390</v>
       </c>
-      <c r="F97" s="12"/>
-      <c r="G97" s="21" t="s">
+      <c r="F97" s="10"/>
+      <c r="G97" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H97" s="14"/>
-      <c r="I97" s="14"/>
-      <c r="J97" s="15"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="14"/>
       <c r="K97" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L97" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M97" s="15"/>
-    </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L97" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="50" t="s">
         <v>391</v>
       </c>
@@ -5492,22 +5492,22 @@
       <c r="E98" s="55" t="s">
         <v>393</v>
       </c>
-      <c r="F98" s="12"/>
-      <c r="G98" s="21" t="s">
+      <c r="F98" s="10"/>
+      <c r="G98" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="15"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="14"/>
       <c r="K98" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L98" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M98" s="15"/>
-    </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L98" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M98" s="14"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="50" t="s">
         <v>394</v>
       </c>
@@ -5523,22 +5523,22 @@
       <c r="E99" s="54" t="s">
         <v>396</v>
       </c>
-      <c r="F99" s="12"/>
-      <c r="G99" s="21" t="s">
+      <c r="F99" s="10"/>
+      <c r="G99" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H99" s="14"/>
-      <c r="I99" s="14"/>
-      <c r="J99" s="15"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="14"/>
       <c r="K99" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L99" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M99" s="15"/>
-    </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L99" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M99" s="14"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="50" t="s">
         <v>397</v>
       </c>
@@ -5554,22 +5554,22 @@
       <c r="E100" s="54" t="s">
         <v>400</v>
       </c>
-      <c r="F100" s="12"/>
-      <c r="G100" s="21" t="s">
+      <c r="F100" s="10"/>
+      <c r="G100" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H100" s="14"/>
-      <c r="I100" s="14"/>
-      <c r="J100" s="15"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="14"/>
       <c r="K100" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L100" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M100" s="15"/>
-    </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L100" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M100" s="14"/>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="50" t="s">
         <v>401</v>
       </c>
@@ -5585,22 +5585,22 @@
       <c r="E101" s="54" t="s">
         <v>403</v>
       </c>
-      <c r="F101" s="12"/>
-      <c r="G101" s="21" t="s">
+      <c r="F101" s="10"/>
+      <c r="G101" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="15"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="14"/>
       <c r="K101" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L101" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M101" s="15"/>
-    </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L101" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M101" s="14"/>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="50" t="s">
         <v>404</v>
       </c>
@@ -5616,22 +5616,22 @@
       <c r="E102" s="54" t="s">
         <v>406</v>
       </c>
-      <c r="F102" s="12"/>
-      <c r="G102" s="21" t="s">
+      <c r="F102" s="10"/>
+      <c r="G102" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H102" s="14"/>
-      <c r="I102" s="14"/>
-      <c r="J102" s="15"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="14"/>
       <c r="K102" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L102" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M102" s="15"/>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L102" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M102" s="14"/>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="50" t="s">
         <v>407</v>
       </c>
@@ -5647,22 +5647,22 @@
       <c r="E103" s="55" t="s">
         <v>410</v>
       </c>
-      <c r="F103" s="12"/>
-      <c r="G103" s="21" t="s">
+      <c r="F103" s="10"/>
+      <c r="G103" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="15"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="14"/>
       <c r="K103" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L103" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M103" s="15"/>
-    </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L103" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M103" s="14"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="50" t="s">
         <v>411</v>
       </c>
@@ -5678,22 +5678,22 @@
       <c r="E104" s="55" t="s">
         <v>413</v>
       </c>
-      <c r="F104" s="12"/>
-      <c r="G104" s="21" t="s">
+      <c r="F104" s="10"/>
+      <c r="G104" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="15"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="14"/>
       <c r="K104" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L104" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M104" s="15"/>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L104" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M104" s="14"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="50" t="s">
         <v>414</v>
       </c>
@@ -5709,22 +5709,22 @@
       <c r="E105" s="55" t="s">
         <v>415</v>
       </c>
-      <c r="F105" s="12"/>
-      <c r="G105" s="21" t="s">
+      <c r="F105" s="10"/>
+      <c r="G105" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="15"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="14"/>
       <c r="K105" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L105" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M105" s="15"/>
-    </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L105" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M105" s="14"/>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="50" t="s">
         <v>416</v>
       </c>
@@ -5740,22 +5740,22 @@
       <c r="E106" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="F106" s="12"/>
-      <c r="G106" s="21" t="s">
+      <c r="F106" s="10"/>
+      <c r="G106" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="15"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="14"/>
       <c r="K106" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L106" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M106" s="15"/>
-    </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L106" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M106" s="14"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="50" t="s">
         <v>420</v>
       </c>
@@ -5771,22 +5771,22 @@
       <c r="E107" s="55" t="s">
         <v>422</v>
       </c>
-      <c r="F107" s="12"/>
-      <c r="G107" s="21" t="s">
+      <c r="F107" s="10"/>
+      <c r="G107" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
-      <c r="J107" s="15"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="14"/>
       <c r="K107" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L107" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M107" s="15"/>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L107" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M107" s="14"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="50" t="s">
         <v>423</v>
       </c>
@@ -5802,22 +5802,22 @@
       <c r="E108" s="55" t="s">
         <v>425</v>
       </c>
-      <c r="F108" s="12"/>
-      <c r="G108" s="21" t="s">
+      <c r="F108" s="10"/>
+      <c r="G108" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
-      <c r="J108" s="15"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="14"/>
       <c r="K108" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L108" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M108" s="15"/>
-    </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L108" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M108" s="14"/>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="50" t="s">
         <v>426</v>
       </c>
@@ -5833,22 +5833,22 @@
       <c r="E109" s="55" t="s">
         <v>429</v>
       </c>
-      <c r="F109" s="12"/>
-      <c r="G109" s="21" t="s">
+      <c r="F109" s="10"/>
+      <c r="G109" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
-      <c r="J109" s="15"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="14"/>
       <c r="K109" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L109" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M109" s="15"/>
-    </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L109" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M109" s="14"/>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="50" t="s">
         <v>430</v>
       </c>
@@ -5864,22 +5864,22 @@
       <c r="E110" s="55" t="s">
         <v>432</v>
       </c>
-      <c r="F110" s="12"/>
-      <c r="G110" s="13" t="s">
+      <c r="F110" s="10"/>
+      <c r="G110" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="H110" s="14"/>
-      <c r="I110" s="14"/>
-      <c r="J110" s="15"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="14"/>
       <c r="K110" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L110" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M110" s="15"/>
-    </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L110" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M110" s="14"/>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="50" t="s">
         <v>433</v>
       </c>
@@ -5895,22 +5895,22 @@
       <c r="E111" s="55" t="s">
         <v>435</v>
       </c>
-      <c r="F111" s="12"/>
+      <c r="F111" s="10"/>
       <c r="G111" s="56" t="s">
         <v>305</v>
       </c>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="15"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="14"/>
       <c r="K111" s="53" t="s">
         <v>13</v>
       </c>
       <c r="L111" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="M111" s="15"/>
-    </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M111" s="14"/>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="50" t="s">
         <v>436</v>
       </c>
@@ -5924,22 +5924,22 @@
         <v>437</v>
       </c>
       <c r="E112" s="55"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="21" t="s">
+      <c r="F112" s="10"/>
+      <c r="G112" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
-      <c r="J112" s="15"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="14"/>
       <c r="K112" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L112" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M112" s="15"/>
-    </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L112" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M112" s="14"/>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="50" t="s">
         <v>438</v>
       </c>
@@ -5955,22 +5955,22 @@
       <c r="E113" s="55" t="s">
         <v>440</v>
       </c>
-      <c r="F113" s="12"/>
-      <c r="G113" s="21" t="s">
+      <c r="F113" s="10"/>
+      <c r="G113" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
-      <c r="J113" s="15"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="14"/>
       <c r="K113" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="L113" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M113" s="15"/>
-    </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L113" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M113" s="14"/>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="50" t="s">
         <v>441</v>
       </c>
@@ -5986,24 +5986,24 @@
       <c r="E114" s="55" t="s">
         <v>443</v>
       </c>
-      <c r="F114" s="12"/>
-      <c r="G114" s="21" t="s">
+      <c r="F114" s="10"/>
+      <c r="G114" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14" t="s">
+      <c r="H114" s="13"/>
+      <c r="I114" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="J114" s="15"/>
+      <c r="J114" s="14"/>
       <c r="K114" s="53" t="s">
         <v>438</v>
       </c>
-      <c r="L114" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M114" s="15"/>
-    </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L114" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M114" s="14"/>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="50" t="s">
         <v>445</v>
       </c>
@@ -6019,22 +6019,22 @@
       <c r="E115" s="55" t="s">
         <v>448</v>
       </c>
-      <c r="F115" s="12"/>
-      <c r="G115" s="21" t="s">
+      <c r="F115" s="10"/>
+      <c r="G115" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="15"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="14"/>
       <c r="K115" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="L115" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M115" s="15"/>
-    </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L115" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M115" s="14"/>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="50" t="s">
         <v>449</v>
       </c>
@@ -6050,24 +6050,24 @@
       <c r="E116" s="55" t="s">
         <v>451</v>
       </c>
-      <c r="F116" s="12" t="s">
+      <c r="F116" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="G116" s="21" t="s">
+      <c r="G116" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H116" s="14"/>
-      <c r="I116" s="14"/>
-      <c r="J116" s="15"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="14"/>
       <c r="K116" s="53" t="s">
         <v>445</v>
       </c>
-      <c r="L116" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M116" s="15"/>
-    </row>
-    <row r="117" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L116" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M116" s="14"/>
+    </row>
+    <row r="117" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="50" t="s">
         <v>453</v>
       </c>
@@ -6080,27 +6080,27 @@
       <c r="D117" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="E117" s="12" t="s">
+      <c r="E117" s="22" t="s">
         <v>455</v>
       </c>
-      <c r="F117" s="12" t="s">
+      <c r="F117" s="22" t="s">
         <v>456</v>
       </c>
-      <c r="G117" s="21" t="s">
+      <c r="G117" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
-      <c r="J117" s="15"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="14"/>
       <c r="K117" s="53" t="s">
         <v>445</v>
       </c>
-      <c r="L117" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M117" s="15"/>
-    </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L117" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M117" s="14"/>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="50" t="s">
         <v>457</v>
       </c>
@@ -6116,24 +6116,24 @@
       <c r="E118" s="58" t="s">
         <v>460</v>
       </c>
-      <c r="F118" s="12"/>
-      <c r="G118" s="13" t="s">
+      <c r="F118" s="10"/>
+      <c r="G118" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H118" s="13" t="s">
+      <c r="H118" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="I118" s="14"/>
-      <c r="J118" s="15"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="14"/>
       <c r="K118" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L118" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M118" s="15"/>
-    </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L118" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M118" s="14"/>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="50" t="s">
         <v>462</v>
       </c>
@@ -6149,14 +6149,14 @@
       <c r="E119" s="58" t="s">
         <v>464</v>
       </c>
-      <c r="F119" s="12" t="s">
+      <c r="F119" s="22" t="s">
         <v>465</v>
       </c>
       <c r="G119" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="H119" s="13"/>
-      <c r="I119" s="14"/>
+      <c r="H119" s="12"/>
+      <c r="I119" s="13"/>
       <c r="J119" s="60"/>
       <c r="K119" s="61" t="s">
         <v>13</v>
@@ -6164,9 +6164,9 @@
       <c r="L119" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="M119" s="15"/>
-    </row>
-    <row r="120" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M119" s="14"/>
+    </row>
+    <row r="120" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="50" t="s">
         <v>466</v>
       </c>
@@ -6179,25 +6179,25 @@
       <c r="D120" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="E120" s="12" t="s">
+      <c r="E120" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="F120" s="12"/>
-      <c r="G120" s="21" t="s">
+      <c r="F120" s="10"/>
+      <c r="G120" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
       <c r="J120" s="27"/>
       <c r="K120" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L120" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M120" s="15"/>
-    </row>
-    <row r="121" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L120" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M120" s="14"/>
+    </row>
+    <row r="121" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="63" t="s">
         <v>470</v>
       </c>
@@ -6210,16 +6210,16 @@
       <c r="D121" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E121" s="12" t="s">
+      <c r="E121" s="22" t="s">
         <v>472</v>
       </c>
-      <c r="F121" s="12" t="s">
+      <c r="F121" s="22" t="s">
         <v>473</v>
       </c>
-      <c r="G121" s="21" t="s">
+      <c r="G121" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H121" s="14"/>
+      <c r="H121" s="13"/>
       <c r="K121" s="63" t="s">
         <v>466</v>
       </c>

</xml_diff>

<commit_message>
Revert "Introduced modification to intentionally trigger Toolbox-Test"
This reverts commit e7d9999014b116692a621651518e6fbdaa0977ed.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -136,7 +136,7 @@
     <t xml:space="preserve">ESG Ziele</t>
   </si>
   <si>
-    <t xml:space="preserve">Existenz von Unternehmensspezifischen ESG-Zielen</t>
+    <t xml:space="preserve">Existenz von ESG-Zielen</t>
   </si>
   <si>
     <t xml:space="preserve">Hat das Unternehmen spezifische ESG-Ziele / Engagements? Werden bspw. spezifische Ziele / Maßnahmen ergriffen, um das 1,5 Grad Ziel zu erreichen?</t>
@@ -1827,6 +1827,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -1865,10 +1869,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2314,7 +2314,7 @@
   <dimension ref="A1:M121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2331,7 +2331,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="12.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -2388,21 +2388,21 @@
       <c r="E2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -2411,194 +2411,194 @@
       <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="20"/>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="13"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="21"/>
+    </row>
+    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="20" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="19" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -2607,29 +2607,29 @@
       <c r="E9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="18" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -2638,204 +2638,204 @@
       <c r="E10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="20"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="12" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="13" t="s">
         <v>66</v>
       </c>
       <c r="K12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="12" t="s">
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="13" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="12" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="13" t="s">
         <v>66</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>76</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="12" t="s">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="13" t="s">
         <v>66</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -2844,351 +2844,351 @@
       <c r="E16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="17" t="s">
         <v>60</v>
       </c>
       <c r="H16" s="10"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="20"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>84</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="12" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="20"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>87</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="17" t="s">
         <v>60</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="20"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="13" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="20"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L19" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
         <v>94</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="12" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
         <v>98</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="20"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L21" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>105</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="20" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
       <c r="K23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="15"/>
+    </row>
+    <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>105</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="20" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="14"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
         <v>111</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="22" t="s">
         <v>105</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="14"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>115</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="20" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="14"/>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>115</v>
       </c>
       <c r="D27" s="10" t="s">
@@ -3197,33 +3197,33 @@
       <c r="E27" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H27" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L27" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
         <v>123</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="22" t="s">
         <v>115</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -3232,95 +3232,95 @@
       <c r="E28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H28" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
       <c r="K28" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L28" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L28" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="15"/>
+    </row>
+    <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="22" t="s">
         <v>128</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="20" t="s">
+      <c r="F29" s="12"/>
+      <c r="G29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="15"/>
       <c r="K29" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L29" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="15"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
         <v>131</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="20" t="s">
+      <c r="F30" s="12"/>
+      <c r="G30" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
       <c r="K30" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="15"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
         <v>134</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>128</v>
       </c>
       <c r="D31" s="10" t="s">
@@ -3329,95 +3329,95 @@
       <c r="E31" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="20" t="s">
+      <c r="F31" s="12"/>
+      <c r="G31" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="L31" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="15"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>139</v>
       </c>
       <c r="E32" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="15"/>
       <c r="K32" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="L32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="15"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
         <v>142</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="20" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L33" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="14"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L33" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
         <v>145</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="22" t="s">
         <v>128</v>
       </c>
       <c r="D34" s="10" t="s">
@@ -3426,95 +3426,95 @@
       <c r="E34" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="20" t="s">
+      <c r="F34" s="12"/>
+      <c r="G34" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="15"/>
       <c r="K34" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="14"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
         <v>148</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>149</v>
       </c>
       <c r="E35" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="15"/>
       <c r="K35" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="L35" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="15"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="20" t="s">
+      <c r="F36" s="12"/>
+      <c r="G36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="15"/>
       <c r="K36" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="L36" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="14"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L36" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="15"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
         <v>153</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="22" t="s">
         <v>128</v>
       </c>
       <c r="D37" s="10" t="s">
@@ -3523,252 +3523,252 @@
       <c r="E37" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="20" t="s">
+      <c r="F37" s="12"/>
+      <c r="G37" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I37" s="13"/>
-      <c r="J37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="L37" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L37" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="15"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>157</v>
       </c>
       <c r="E38" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="15"/>
       <c r="K38" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="L38" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" s="14"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="15"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
         <v>158</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="22" t="s">
         <v>159</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="20" t="s">
+      <c r="F39" s="12"/>
+      <c r="G39" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L39" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M39" s="14"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="15"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
         <v>162</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="22" t="s">
         <v>159</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="20" t="s">
+      <c r="F40" s="12"/>
+      <c r="G40" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L40" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" s="14"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L40" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="15"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="22" t="s">
         <v>159</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="20" t="s">
+      <c r="F41" s="12"/>
+      <c r="G41" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="20"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="21"/>
       <c r="K41" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L41" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" s="14"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="15"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="s">
         <v>169</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="22" t="s">
         <v>159</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="20" t="s">
+      <c r="F42" s="12"/>
+      <c r="G42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="20" t="s">
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="21" t="s">
         <v>66</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L42" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M42" s="14"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="15"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
         <v>172</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="22" t="s">
         <v>159</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="20" t="s">
+      <c r="F43" s="12"/>
+      <c r="G43" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="15"/>
       <c r="K43" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L43" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M43" s="14"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="15"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
         <v>175</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="22" t="s">
         <v>176</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E44" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="20" t="s">
+      <c r="F44" s="12"/>
+      <c r="G44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="15"/>
       <c r="K44" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L44" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M44" s="14"/>
-    </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="15"/>
+    </row>
+    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="22" t="s">
         <v>176</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -3777,62 +3777,62 @@
       <c r="E45" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G45" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="15"/>
       <c r="K45" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="L45" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="14"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="15"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
         <v>184</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="22" t="s">
         <v>176</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E46" s="22" t="s">
+      <c r="E46" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="20" t="s">
+      <c r="F46" s="12"/>
+      <c r="G46" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
       <c r="K46" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="14"/>
-    </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="15"/>
+    </row>
+    <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
         <v>187</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="22" t="s">
         <v>176</v>
       </c>
       <c r="D47" s="10" t="s">
@@ -3841,31 +3841,31 @@
       <c r="E47" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G47" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="15"/>
       <c r="K47" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="L47" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M47" s="14"/>
-    </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="15"/>
+    </row>
+    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
         <v>190</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -3874,55 +3874,55 @@
       <c r="E48" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="15"/>
       <c r="K48" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L48" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M48" s="14"/>
-    </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="15"/>
+    </row>
+    <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
         <v>195</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="F49" s="10"/>
-      <c r="G49" s="20" t="s">
+      <c r="F49" s="12"/>
+      <c r="G49" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="15"/>
       <c r="K49" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L49" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M49" s="14"/>
-    </row>
-    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="15"/>
+    </row>
+    <row r="50" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
         <v>198</v>
       </c>
@@ -3938,24 +3938,24 @@
       <c r="E50" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G50" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="15"/>
       <c r="K50" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L50" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M50" s="14"/>
-    </row>
-    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
         <v>205</v>
       </c>
@@ -3965,28 +3965,28 @@
       <c r="C51" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="F51" s="10"/>
-      <c r="G51" s="20" t="s">
+      <c r="F51" s="12"/>
+      <c r="G51" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="15"/>
       <c r="K51" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L51" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M51" s="14"/>
-    </row>
-    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="15"/>
+    </row>
+    <row r="52" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
         <v>208</v>
       </c>
@@ -3999,120 +3999,120 @@
       <c r="D52" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="22" t="s">
+      <c r="E52" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="F52" s="22" t="s">
+      <c r="F52" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="15"/>
       <c r="K52" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L52" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M52" s="14"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="15"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
         <v>212</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="22" t="s">
         <v>213</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="E53" s="22" t="s">
+      <c r="E53" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="20" t="s">
+      <c r="F53" s="12"/>
+      <c r="G53" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="15"/>
       <c r="K53" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L53" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="14"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L53" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M53" s="15"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="s">
         <v>216</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="22" t="s">
         <v>213</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="E54" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="15"/>
       <c r="K54" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="L54" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="14"/>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L54" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="15"/>
+    </row>
+    <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="s">
         <v>220</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="22" t="s">
         <v>213</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="E55" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="F55" s="10"/>
-      <c r="G55" s="20" t="s">
+      <c r="F55" s="12"/>
+      <c r="G55" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="15"/>
       <c r="K55" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L55" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="14"/>
+      <c r="L55" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="28" t="s">
@@ -4130,24 +4130,24 @@
       <c r="E56" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F56" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="G56" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="15"/>
       <c r="K56" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L56" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="14"/>
-    </row>
-    <row r="57" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="15"/>
+    </row>
+    <row r="57" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
         <v>228</v>
       </c>
@@ -4157,28 +4157,28 @@
       <c r="C57" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="13" t="s">
         <v>229</v>
       </c>
       <c r="E57" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="15"/>
       <c r="K57" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L57" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M57" s="14"/>
+      <c r="L57" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
@@ -4196,24 +4196,24 @@
       <c r="E58" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="G58" s="12" t="s">
+      <c r="G58" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="15"/>
       <c r="K58" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L58" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M58" s="14"/>
-    </row>
-    <row r="59" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L58" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="15"/>
+    </row>
+    <row r="59" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
         <v>237</v>
       </c>
@@ -4229,24 +4229,24 @@
       <c r="E59" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="15"/>
       <c r="K59" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L59" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="14"/>
-    </row>
-    <row r="60" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L59" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
         <v>239</v>
       </c>
@@ -4262,24 +4262,24 @@
       <c r="E60" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="F60" s="22" t="s">
+      <c r="F60" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G60" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="15"/>
       <c r="K60" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L60" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M60" s="14"/>
-    </row>
-    <row r="61" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L60" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
         <v>244</v>
       </c>
@@ -4295,24 +4295,24 @@
       <c r="E61" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="F61" s="22" t="s">
+      <c r="F61" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="15"/>
       <c r="K61" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L61" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M61" s="14"/>
-    </row>
-    <row r="62" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M61" s="15"/>
+    </row>
+    <row r="62" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
         <v>246</v>
       </c>
@@ -4328,24 +4328,24 @@
       <c r="E62" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="F62" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="G62" s="12" t="s">
+      <c r="G62" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="15"/>
       <c r="K62" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L62" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M62" s="14"/>
-    </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L62" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62" s="15"/>
+    </row>
+    <row r="63" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
         <v>251</v>
       </c>
@@ -4361,24 +4361,24 @@
       <c r="E63" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="15"/>
       <c r="K63" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L63" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M63" s="14"/>
-    </row>
-    <row r="64" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" s="15"/>
+    </row>
+    <row r="64" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
         <v>253</v>
       </c>
@@ -4394,24 +4394,24 @@
       <c r="E64" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="F64" s="22" t="s">
+      <c r="F64" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="G64" s="12" t="s">
+      <c r="G64" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="15"/>
       <c r="K64" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L64" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M64" s="14"/>
-    </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L64" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="15"/>
+    </row>
+    <row r="65" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
         <v>257</v>
       </c>
@@ -4424,56 +4424,56 @@
       <c r="D65" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="E65" s="22" t="s">
+      <c r="E65" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="F65" s="10"/>
-      <c r="G65" s="20" t="s">
+      <c r="F65" s="12"/>
+      <c r="G65" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="15"/>
       <c r="K65" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L65" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="15"/>
+    </row>
+    <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="17" t="s">
         <v>261</v>
       </c>
       <c r="D66" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="22" t="s">
+      <c r="E66" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="F66" s="10"/>
-      <c r="G66" s="20" t="s">
+      <c r="F66" s="12"/>
+      <c r="G66" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="15"/>
       <c r="K66" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L66" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M66" s="14"/>
-    </row>
-    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L66" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" s="15"/>
+    </row>
+    <row r="67" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
         <v>264</v>
       </c>
@@ -4486,58 +4486,58 @@
       <c r="D67" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="E67" s="22" t="s">
+      <c r="E67" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="F67" s="22" t="s">
+      <c r="F67" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="15"/>
       <c r="K67" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="L67" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M67" s="14"/>
-    </row>
-    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L67" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="17" t="s">
         <v>261</v>
       </c>
       <c r="D68" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="E68" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="F68" s="10"/>
-      <c r="G68" s="20" t="s">
+      <c r="F68" s="12"/>
+      <c r="G68" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="15"/>
       <c r="K68" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L68" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M68" s="14"/>
-    </row>
-    <row r="69" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L68" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" s="15"/>
+    </row>
+    <row r="69" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="s">
         <v>271</v>
       </c>
@@ -4550,27 +4550,27 @@
       <c r="D69" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="E69" s="22" t="s">
+      <c r="E69" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="F69" s="22" t="s">
+      <c r="F69" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="G69" s="20" t="s">
+      <c r="G69" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="15"/>
       <c r="K69" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="L69" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M69" s="14"/>
-    </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L69" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M69" s="15"/>
+    </row>
+    <row r="70" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="s">
         <v>275</v>
       </c>
@@ -4583,25 +4583,25 @@
       <c r="D70" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E70" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="20" t="s">
+      <c r="F70" s="12"/>
+      <c r="G70" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="15"/>
       <c r="K70" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L70" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M70" s="14"/>
-    </row>
-    <row r="71" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L70" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M70" s="15"/>
+    </row>
+    <row r="71" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
         <v>279</v>
       </c>
@@ -4617,24 +4617,24 @@
       <c r="E71" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="F71" s="22" t="s">
+      <c r="F71" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="G71" s="12" t="s">
+      <c r="G71" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="15"/>
       <c r="K71" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="L71" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M71" s="14"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L71" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="15"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
         <v>283</v>
       </c>
@@ -4650,24 +4650,24 @@
       <c r="E72" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="F72" s="10"/>
-      <c r="G72" s="20" t="s">
+      <c r="F72" s="12"/>
+      <c r="G72" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H72" s="20" t="s">
+      <c r="H72" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="I72" s="13"/>
-      <c r="J72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="15"/>
       <c r="K72" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L72" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M72" s="14"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L72" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M72" s="15"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
         <v>288</v>
       </c>
@@ -4680,25 +4680,25 @@
       <c r="D73" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="F73" s="10"/>
-      <c r="G73" s="20" t="s">
+      <c r="F73" s="12"/>
+      <c r="G73" s="21" t="s">
         <v>291</v>
       </c>
       <c r="H73" s="10"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="15"/>
       <c r="K73" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L73" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M73" s="14"/>
-    </row>
-    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L73" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M73" s="15"/>
+    </row>
+    <row r="74" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
         <v>292</v>
       </c>
@@ -4714,24 +4714,24 @@
       <c r="E74" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="F74" s="22" t="s">
+      <c r="F74" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="G74" s="12" t="s">
+      <c r="G74" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="15"/>
       <c r="K74" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L74" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M74" s="14"/>
-    </row>
-    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L74" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M74" s="15"/>
+    </row>
+    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
         <v>296</v>
       </c>
@@ -4744,230 +4744,230 @@
       <c r="D75" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="E75" s="22" t="s">
+      <c r="E75" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="20" t="s">
+      <c r="F75" s="12"/>
+      <c r="G75" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="15"/>
       <c r="K75" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L75" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M75" s="14"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L75" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M75" s="15"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="s">
         <v>301</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="E76" s="22" t="s">
+      <c r="E76" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="F76" s="22" t="s">
+      <c r="F76" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="G76" s="20" t="s">
+      <c r="G76" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="15"/>
       <c r="K76" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L76" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M76" s="14"/>
-    </row>
-    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M76" s="15"/>
+    </row>
+    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
         <v>306</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="E77" s="22" t="s">
+      <c r="E77" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F77" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="G77" s="20" t="s">
+      <c r="G77" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="15"/>
       <c r="K77" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L77" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M77" s="14"/>
-    </row>
-    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L77" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M77" s="15"/>
+    </row>
+    <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
         <v>310</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C78" s="21" t="s">
+      <c r="C78" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="E78" s="22" t="s">
+      <c r="E78" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="F78" s="22" t="s">
+      <c r="F78" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="G78" s="20" t="s">
+      <c r="G78" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="15"/>
       <c r="K78" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L78" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M78" s="14"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L78" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M78" s="15"/>
+    </row>
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
         <v>314</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="C79" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E79" s="22" t="s">
+      <c r="E79" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="F79" s="22" t="s">
+      <c r="F79" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="G79" s="20" t="s">
+      <c r="G79" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="15"/>
       <c r="K79" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L79" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M79" s="14"/>
-    </row>
-    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L79" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M79" s="15"/>
+    </row>
+    <row r="80" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
         <v>318</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C80" s="21" t="s">
+      <c r="C80" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E80" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="F80" s="22" t="s">
+      <c r="F80" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="G80" s="20" t="s">
+      <c r="G80" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="15"/>
       <c r="K80" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L80" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M80" s="14"/>
-    </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L80" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M80" s="15"/>
+    </row>
+    <row r="81" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
         <v>322</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D81" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="E81" s="22" t="s">
+      <c r="E81" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="F81" s="22" t="s">
+      <c r="F81" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="G81" s="20" t="s">
+      <c r="G81" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="15"/>
       <c r="K81" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L81" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M81" s="14"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L81" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M81" s="15"/>
+    </row>
+    <row r="82" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="s">
         <v>326</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="22" t="s">
         <v>298</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -4976,24 +4976,24 @@
       <c r="E82" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="F82" s="22" t="s">
+      <c r="F82" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="G82" s="12" t="s">
+      <c r="G82" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="15"/>
       <c r="K82" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="L82" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M82" s="14"/>
-    </row>
-    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L82" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M82" s="15"/>
+    </row>
+    <row r="83" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="s">
         <v>331</v>
       </c>
@@ -5006,29 +5006,29 @@
       <c r="D83" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E83" s="22" t="s">
+      <c r="E83" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="F83" s="10"/>
-      <c r="G83" s="20" t="s">
+      <c r="F83" s="12"/>
+      <c r="G83" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="15"/>
       <c r="K83" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L83" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M83" s="14"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L83" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M83" s="15"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="17" t="s">
         <v>297</v>
       </c>
       <c r="C84" s="47" t="s">
@@ -5040,22 +5040,22 @@
       <c r="E84" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="F84" s="10"/>
-      <c r="G84" s="12" t="s">
+      <c r="F84" s="12"/>
+      <c r="G84" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="15"/>
       <c r="K84" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L84" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M84" s="14"/>
-    </row>
-    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L84" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M84" s="15"/>
+    </row>
+    <row r="85" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
         <v>338</v>
       </c>
@@ -5071,24 +5071,24 @@
       <c r="E85" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F85" s="22" t="s">
+      <c r="F85" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="G85" s="12" t="s">
+      <c r="G85" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="15"/>
       <c r="K85" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L85" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M85" s="14"/>
-    </row>
-    <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L85" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M85" s="15"/>
+    </row>
+    <row r="86" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
         <v>342</v>
       </c>
@@ -5104,24 +5104,24 @@
       <c r="E86" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="F86" s="22" t="s">
+      <c r="F86" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="G86" s="12" t="s">
+      <c r="G86" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="15"/>
       <c r="K86" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L86" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M86" s="14"/>
-    </row>
-    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L86" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M86" s="15"/>
+    </row>
+    <row r="87" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
         <v>347</v>
       </c>
@@ -5134,25 +5134,25 @@
       <c r="D87" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="E87" s="22" t="s">
+      <c r="E87" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="F87" s="10"/>
-      <c r="G87" s="20" t="s">
+      <c r="F87" s="12"/>
+      <c r="G87" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="15"/>
       <c r="K87" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L87" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M87" s="14"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L87" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M87" s="15"/>
+    </row>
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
         <v>350</v>
       </c>
@@ -5168,24 +5168,24 @@
       <c r="E88" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="F88" s="22" t="s">
+      <c r="F88" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="G88" s="12" t="s">
+      <c r="G88" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="15"/>
       <c r="K88" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L88" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M88" s="14"/>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L88" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M88" s="15"/>
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
         <v>355</v>
       </c>
@@ -5201,24 +5201,24 @@
       <c r="E89" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="F89" s="22" t="s">
+      <c r="F89" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="G89" s="12" t="s">
+      <c r="G89" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="15"/>
       <c r="K89" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L89" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M89" s="14"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L89" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M89" s="15"/>
+    </row>
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="50" t="s">
         <v>359</v>
       </c>
@@ -5234,24 +5234,24 @@
       <c r="E90" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="F90" s="22" t="s">
+      <c r="F90" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="G90" s="12" t="s">
+      <c r="G90" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="15"/>
       <c r="K90" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L90" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M90" s="14"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L90" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M90" s="15"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="50" t="s">
         <v>363</v>
       </c>
@@ -5267,24 +5267,24 @@
       <c r="E91" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="F91" s="22" t="s">
+      <c r="F91" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="G91" s="12" t="s">
+      <c r="G91" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="15"/>
       <c r="K91" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L91" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M91" s="14"/>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L91" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M91" s="15"/>
+    </row>
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="50" t="s">
         <v>367</v>
       </c>
@@ -5297,27 +5297,27 @@
       <c r="D92" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E92" s="22" t="s">
+      <c r="E92" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="F92" s="22" t="s">
+      <c r="F92" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="G92" s="20" t="s">
+      <c r="G92" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="15"/>
       <c r="K92" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L92" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M92" s="14"/>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L92" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M92" s="15"/>
+    </row>
+    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="50" t="s">
         <v>371</v>
       </c>
@@ -5333,22 +5333,22 @@
       <c r="E93" s="46" t="s">
         <v>373</v>
       </c>
-      <c r="F93" s="10"/>
-      <c r="G93" s="20" t="s">
+      <c r="F93" s="12"/>
+      <c r="G93" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="15"/>
       <c r="K93" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L93" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M93" s="14"/>
-    </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L93" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M93" s="15"/>
+    </row>
+    <row r="94" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="50" t="s">
         <v>374</v>
       </c>
@@ -5361,25 +5361,25 @@
       <c r="D94" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="E94" s="22" t="s">
+      <c r="E94" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="F94" s="10"/>
-      <c r="G94" s="20" t="s">
+      <c r="F94" s="12"/>
+      <c r="G94" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="15"/>
       <c r="K94" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L94" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M94" s="14"/>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L94" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M94" s="15"/>
+    </row>
+    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="50" t="s">
         <v>378</v>
       </c>
@@ -5395,24 +5395,24 @@
       <c r="E95" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="F95" s="10"/>
-      <c r="G95" s="20" t="s">
+      <c r="F95" s="12"/>
+      <c r="G95" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H95" s="52" t="s">
         <v>381</v>
       </c>
-      <c r="I95" s="13"/>
-      <c r="J95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="15"/>
       <c r="K95" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="L95" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M95" s="14"/>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L95" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M95" s="15"/>
+    </row>
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="50" t="s">
         <v>382</v>
       </c>
@@ -5428,24 +5428,24 @@
       <c r="E96" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F96" s="22" t="s">
+      <c r="F96" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="G96" s="20" t="s">
+      <c r="G96" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="15"/>
       <c r="K96" s="53" t="s">
         <v>374</v>
       </c>
-      <c r="L96" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M96" s="14"/>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L96" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M96" s="15"/>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="50" t="s">
         <v>386</v>
       </c>
@@ -5461,22 +5461,22 @@
       <c r="E97" s="54" t="s">
         <v>390</v>
       </c>
-      <c r="F97" s="10"/>
-      <c r="G97" s="20" t="s">
+      <c r="F97" s="12"/>
+      <c r="G97" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="15"/>
       <c r="K97" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L97" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M97" s="14"/>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L97" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M97" s="15"/>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="50" t="s">
         <v>391</v>
       </c>
@@ -5492,22 +5492,22 @@
       <c r="E98" s="55" t="s">
         <v>393</v>
       </c>
-      <c r="F98" s="10"/>
-      <c r="G98" s="20" t="s">
+      <c r="F98" s="12"/>
+      <c r="G98" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="15"/>
       <c r="K98" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L98" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M98" s="14"/>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L98" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M98" s="15"/>
+    </row>
+    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="50" t="s">
         <v>394</v>
       </c>
@@ -5523,22 +5523,22 @@
       <c r="E99" s="54" t="s">
         <v>396</v>
       </c>
-      <c r="F99" s="10"/>
-      <c r="G99" s="20" t="s">
+      <c r="F99" s="12"/>
+      <c r="G99" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="14"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="15"/>
       <c r="K99" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L99" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M99" s="14"/>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L99" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M99" s="15"/>
+    </row>
+    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="50" t="s">
         <v>397</v>
       </c>
@@ -5554,22 +5554,22 @@
       <c r="E100" s="54" t="s">
         <v>400</v>
       </c>
-      <c r="F100" s="10"/>
-      <c r="G100" s="20" t="s">
+      <c r="F100" s="12"/>
+      <c r="G100" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="15"/>
       <c r="K100" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L100" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M100" s="14"/>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L100" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M100" s="15"/>
+    </row>
+    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="50" t="s">
         <v>401</v>
       </c>
@@ -5585,22 +5585,22 @@
       <c r="E101" s="54" t="s">
         <v>403</v>
       </c>
-      <c r="F101" s="10"/>
-      <c r="G101" s="20" t="s">
+      <c r="F101" s="12"/>
+      <c r="G101" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="15"/>
       <c r="K101" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L101" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M101" s="14"/>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L101" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M101" s="15"/>
+    </row>
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="50" t="s">
         <v>404</v>
       </c>
@@ -5616,22 +5616,22 @@
       <c r="E102" s="54" t="s">
         <v>406</v>
       </c>
-      <c r="F102" s="10"/>
-      <c r="G102" s="20" t="s">
+      <c r="F102" s="12"/>
+      <c r="G102" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="15"/>
       <c r="K102" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L102" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M102" s="14"/>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L102" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M102" s="15"/>
+    </row>
+    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="50" t="s">
         <v>407</v>
       </c>
@@ -5647,22 +5647,22 @@
       <c r="E103" s="55" t="s">
         <v>410</v>
       </c>
-      <c r="F103" s="10"/>
-      <c r="G103" s="20" t="s">
+      <c r="F103" s="12"/>
+      <c r="G103" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="15"/>
       <c r="K103" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L103" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M103" s="14"/>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L103" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M103" s="15"/>
+    </row>
+    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="50" t="s">
         <v>411</v>
       </c>
@@ -5678,22 +5678,22 @@
       <c r="E104" s="55" t="s">
         <v>413</v>
       </c>
-      <c r="F104" s="10"/>
-      <c r="G104" s="20" t="s">
+      <c r="F104" s="12"/>
+      <c r="G104" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="15"/>
       <c r="K104" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L104" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M104" s="14"/>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L104" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M104" s="15"/>
+    </row>
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="50" t="s">
         <v>414</v>
       </c>
@@ -5709,22 +5709,22 @@
       <c r="E105" s="55" t="s">
         <v>415</v>
       </c>
-      <c r="F105" s="10"/>
-      <c r="G105" s="20" t="s">
+      <c r="F105" s="12"/>
+      <c r="G105" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="15"/>
       <c r="K105" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L105" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M105" s="14"/>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L105" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M105" s="15"/>
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="50" t="s">
         <v>416</v>
       </c>
@@ -5740,22 +5740,22 @@
       <c r="E106" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="F106" s="10"/>
-      <c r="G106" s="20" t="s">
+      <c r="F106" s="12"/>
+      <c r="G106" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="15"/>
       <c r="K106" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L106" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M106" s="14"/>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L106" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M106" s="15"/>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="50" t="s">
         <v>420</v>
       </c>
@@ -5771,22 +5771,22 @@
       <c r="E107" s="55" t="s">
         <v>422</v>
       </c>
-      <c r="F107" s="10"/>
-      <c r="G107" s="20" t="s">
+      <c r="F107" s="12"/>
+      <c r="G107" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="15"/>
       <c r="K107" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L107" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M107" s="14"/>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L107" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M107" s="15"/>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="50" t="s">
         <v>423</v>
       </c>
@@ -5802,22 +5802,22 @@
       <c r="E108" s="55" t="s">
         <v>425</v>
       </c>
-      <c r="F108" s="10"/>
-      <c r="G108" s="20" t="s">
+      <c r="F108" s="12"/>
+      <c r="G108" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="15"/>
       <c r="K108" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L108" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M108" s="14"/>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L108" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M108" s="15"/>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="50" t="s">
         <v>426</v>
       </c>
@@ -5833,22 +5833,22 @@
       <c r="E109" s="55" t="s">
         <v>429</v>
       </c>
-      <c r="F109" s="10"/>
-      <c r="G109" s="20" t="s">
+      <c r="F109" s="12"/>
+      <c r="G109" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="14"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="15"/>
       <c r="K109" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L109" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M109" s="14"/>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L109" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M109" s="15"/>
+    </row>
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="50" t="s">
         <v>430</v>
       </c>
@@ -5864,22 +5864,22 @@
       <c r="E110" s="55" t="s">
         <v>432</v>
       </c>
-      <c r="F110" s="10"/>
-      <c r="G110" s="12" t="s">
+      <c r="F110" s="12"/>
+      <c r="G110" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="H110" s="13"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="15"/>
       <c r="K110" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L110" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M110" s="14"/>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L110" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M110" s="15"/>
+    </row>
+    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="50" t="s">
         <v>433</v>
       </c>
@@ -5895,22 +5895,22 @@
       <c r="E111" s="55" t="s">
         <v>435</v>
       </c>
-      <c r="F111" s="10"/>
+      <c r="F111" s="12"/>
       <c r="G111" s="56" t="s">
         <v>305</v>
       </c>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="14"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="15"/>
       <c r="K111" s="53" t="s">
         <v>13</v>
       </c>
       <c r="L111" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="M111" s="14"/>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M111" s="15"/>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="50" t="s">
         <v>436</v>
       </c>
@@ -5924,22 +5924,22 @@
         <v>437</v>
       </c>
       <c r="E112" s="55"/>
-      <c r="F112" s="10"/>
-      <c r="G112" s="20" t="s">
+      <c r="F112" s="12"/>
+      <c r="G112" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+      <c r="J112" s="15"/>
       <c r="K112" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L112" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M112" s="14"/>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L112" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M112" s="15"/>
+    </row>
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="50" t="s">
         <v>438</v>
       </c>
@@ -5955,22 +5955,22 @@
       <c r="E113" s="55" t="s">
         <v>440</v>
       </c>
-      <c r="F113" s="10"/>
-      <c r="G113" s="20" t="s">
+      <c r="F113" s="12"/>
+      <c r="G113" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
-      <c r="J113" s="14"/>
+      <c r="H113" s="14"/>
+      <c r="I113" s="14"/>
+      <c r="J113" s="15"/>
       <c r="K113" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="L113" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M113" s="14"/>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M113" s="15"/>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="50" t="s">
         <v>441</v>
       </c>
@@ -5986,24 +5986,24 @@
       <c r="E114" s="55" t="s">
         <v>443</v>
       </c>
-      <c r="F114" s="10"/>
-      <c r="G114" s="20" t="s">
+      <c r="F114" s="12"/>
+      <c r="G114" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13" t="s">
+      <c r="H114" s="14"/>
+      <c r="I114" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="J114" s="14"/>
+      <c r="J114" s="15"/>
       <c r="K114" s="53" t="s">
         <v>438</v>
       </c>
-      <c r="L114" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M114" s="14"/>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L114" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M114" s="15"/>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="50" t="s">
         <v>445</v>
       </c>
@@ -6019,22 +6019,22 @@
       <c r="E115" s="55" t="s">
         <v>448</v>
       </c>
-      <c r="F115" s="10"/>
-      <c r="G115" s="20" t="s">
+      <c r="F115" s="12"/>
+      <c r="G115" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
-      <c r="J115" s="14"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="14"/>
+      <c r="J115" s="15"/>
       <c r="K115" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="L115" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M115" s="14"/>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L115" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M115" s="15"/>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="50" t="s">
         <v>449</v>
       </c>
@@ -6050,24 +6050,24 @@
       <c r="E116" s="55" t="s">
         <v>451</v>
       </c>
-      <c r="F116" s="22" t="s">
+      <c r="F116" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="G116" s="20" t="s">
+      <c r="G116" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
-      <c r="J116" s="14"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="15"/>
       <c r="K116" s="53" t="s">
         <v>445</v>
       </c>
-      <c r="L116" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M116" s="14"/>
-    </row>
-    <row r="117" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L116" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M116" s="15"/>
+    </row>
+    <row r="117" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="50" t="s">
         <v>453</v>
       </c>
@@ -6080,27 +6080,27 @@
       <c r="D117" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="E117" s="22" t="s">
+      <c r="E117" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="F117" s="22" t="s">
+      <c r="F117" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="G117" s="20" t="s">
+      <c r="G117" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="15"/>
       <c r="K117" s="53" t="s">
         <v>445</v>
       </c>
-      <c r="L117" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M117" s="14"/>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L117" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M117" s="15"/>
+    </row>
+    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="50" t="s">
         <v>457</v>
       </c>
@@ -6116,24 +6116,24 @@
       <c r="E118" s="58" t="s">
         <v>460</v>
       </c>
-      <c r="F118" s="10"/>
-      <c r="G118" s="12" t="s">
+      <c r="F118" s="12"/>
+      <c r="G118" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H118" s="12" t="s">
+      <c r="H118" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="I118" s="13"/>
-      <c r="J118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="15"/>
       <c r="K118" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L118" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M118" s="14"/>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L118" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M118" s="15"/>
+    </row>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="50" t="s">
         <v>462</v>
       </c>
@@ -6149,14 +6149,14 @@
       <c r="E119" s="58" t="s">
         <v>464</v>
       </c>
-      <c r="F119" s="22" t="s">
+      <c r="F119" s="12" t="s">
         <v>465</v>
       </c>
       <c r="G119" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="H119" s="12"/>
-      <c r="I119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="14"/>
       <c r="J119" s="60"/>
       <c r="K119" s="61" t="s">
         <v>13</v>
@@ -6164,9 +6164,9 @@
       <c r="L119" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="M119" s="14"/>
-    </row>
-    <row r="120" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M119" s="15"/>
+    </row>
+    <row r="120" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="50" t="s">
         <v>466</v>
       </c>
@@ -6179,25 +6179,25 @@
       <c r="D120" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="E120" s="22" t="s">
+      <c r="E120" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="F120" s="10"/>
-      <c r="G120" s="20" t="s">
+      <c r="F120" s="12"/>
+      <c r="G120" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
       <c r="J120" s="27"/>
       <c r="K120" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L120" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M120" s="14"/>
-    </row>
-    <row r="121" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L120" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M120" s="15"/>
+    </row>
+    <row r="121" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="63" t="s">
         <v>470</v>
       </c>
@@ -6210,16 +6210,16 @@
       <c r="D121" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E121" s="22" t="s">
+      <c r="E121" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="F121" s="22" t="s">
+      <c r="F121" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="G121" s="20" t="s">
+      <c r="G121" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H121" s="13"/>
+      <c r="H121" s="14"/>
       <c r="K121" s="63" t="s">
         <v>466</v>
       </c>

</xml_diff>

<commit_message>
add soziales and governance
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9091F44-F62A-43BB-8A16-778674FC35C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C0AE6-A199-4DD9-B03D-C16D727CFCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -48,8 +48,19 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH">130000</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -58,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="664">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1759,6 +1770,297 @@
   </si>
   <si>
     <t>1333333</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.2</t>
+  </si>
+  <si>
+    <t>18.1.3</t>
+  </si>
+  <si>
+    <t>18.1.4</t>
+  </si>
+  <si>
+    <t>Governance</t>
+  </si>
+  <si>
+    <t>Vorstandsprofil</t>
+  </si>
+  <si>
+    <t>Umfang des Top-Management im Unternehmen</t>
+  </si>
+  <si>
+    <t>Welche Ebenen des Management werden in ihrem Unternehmen zum Top-Management gezählt?</t>
+  </si>
+  <si>
+    <t>Die Ebenen des Top-Managements im Unternehmen.</t>
+  </si>
+  <si>
+    <t>Vorstand + 1. Ebene | Vorstand + 1. und 2. Ebene</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil diverser Personen im Top-Management in Prozent?</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil männlicher Personen im Top-Management in Prozent?</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil weiblicher Personen im Top-Management in Prozent?</t>
+  </si>
+  <si>
+    <t>Anteil weiblicher Personen im Top-Management in Prozent.</t>
+  </si>
+  <si>
+    <t>Anteil männlicher Personen im Top-Management in Prozent.</t>
+  </si>
+  <si>
+    <t>Anteil diverser Personen im Top-Management in Prozent.</t>
+  </si>
+  <si>
+    <t>18.2.1</t>
+  </si>
+  <si>
+    <t>18.2.2</t>
+  </si>
+  <si>
+    <t>Stakeholderdialog</t>
+  </si>
+  <si>
+    <t>Risiken und Maßnahmen</t>
+  </si>
+  <si>
+    <t>Weitere wesentliche Governance-Risiken</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>20.2</t>
+  </si>
+  <si>
+    <t>CSRD-konformer Prozess zur Berücksichtigung der Stakeholderinteressen</t>
+  </si>
+  <si>
+    <t>Welchen weiteren wesentlichen governance-bezogenen Risiken ist das Unternehmen ausgesetzt?</t>
+  </si>
+  <si>
+    <t>Welche Maßnahmen hat das Unternehmen zur Reduzierung dieser governance-bezogenen Risiken getroffen, außer der in Frage 5.1 genannten Richtlinien?</t>
+  </si>
+  <si>
+    <t>Verfügt das Unternehmen über einen institutionalisierten, CSRD-konformen Prozess zur Berücksichtigung der Interessen der Stakeholder des Unternehmens?</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitte den Prozess in seiner Methodik skizzieren und wichtigste Schlussfolgerungen darstellen. </t>
+  </si>
+  <si>
+    <t>CSRD-konformer Prozess zur Berücksichtigung der Stakeholderinteressen Erläuterung</t>
+  </si>
+  <si>
+    <t>Ist die Vergütung des Top-Managements (auch) explizit an Nachhaltigkeitsziele gekoppelt (bspw. ESG-Rating)?</t>
+  </si>
+  <si>
+    <t>Kopplung von Vergütung des Top-Managements an Nachhaltigkeitsziele</t>
+  </si>
+  <si>
+    <t>Kopplung von Vergütung des Top-Managements an Nachhaltigkeitsziele Erläuterung</t>
+  </si>
+  <si>
+    <t>Bitte die bestehende Regelung skizzieren.</t>
+  </si>
+  <si>
+    <t>Skizze des Prozesses und Darstellung der wichtigsten Schlussfolgerungen.</t>
+  </si>
+  <si>
+    <t>Skizze der bestehenden Regelung.</t>
+  </si>
+  <si>
+    <t>Beschäftigtenprofil und Entlohnung</t>
+  </si>
+  <si>
+    <t>Wie viele Beschäftigte hat das Unternehmen insgesamt? Die Beschäftigtenanzahl bezieht sich auf die Anzahl der Arbeitnehmer, nicht auf die Anzahl von Vollzeitstellen. Besondere Beschäftigungsverhältnisse wie z. B. Praktika und Traineeprogramme sollten mit einbezogen werden, wenn die Arbeitsverträge die nationalen rechtlichen Vorrausetzungen für ein Arbeitnehmerverhältnis erfüllen.</t>
+  </si>
+  <si>
+    <t>Die Zahl der im Unternehmen beschäftigten Personen.</t>
+  </si>
+  <si>
+    <t>Zahl der Beschäftigten insgesamt</t>
+  </si>
+  <si>
+    <t>Anteil weiblicher Personen im Top-Management</t>
+  </si>
+  <si>
+    <t>Anteil männlicher Personen im Top-Management</t>
+  </si>
+  <si>
+    <t>Anteil diverser Personen im Top-Management</t>
+  </si>
+  <si>
+    <t>Anteil weiblicher Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil weiblicher Personen unter den Beschäftigten in Prozent?</t>
+  </si>
+  <si>
+    <t>14.1.3</t>
+  </si>
+  <si>
+    <t>14.1.4</t>
+  </si>
+  <si>
+    <t>Anteil männlicher Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>Anteil diverser Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil männlicher Personen unter den Beschäftigten in Prozent?</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil diverser Personen unter den Beschäftigten in Prozent?</t>
+  </si>
+  <si>
+    <t>Der prozentuale Anteil männlicher Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>Der prozentuale Anteil weiblicher Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>Geschlechtsspezifisches Lohngefälle</t>
+  </si>
+  <si>
+    <t>Besteht im Unternehmen bei gleicher Tätigkeit ein signifikanter Unterschied in der Vergütung weiblicher und männlicher Personen? Methodik analog zu ESRS S1-16.</t>
+  </si>
+  <si>
+    <t>Der prozentuale Anteil diverser Personen unter den Beschäftigten</t>
+  </si>
+  <si>
+    <t>In welchem Verhältnis steht die Vergütung der höchstbezahlten Person des Unternehmens zum Median der jährlichen Gesamtvergütung aller Beschäftigen? Methodik analog zu ESRS S1-16.</t>
+  </si>
+  <si>
+    <t>Jährliche Gesamtvergütungsquote</t>
+  </si>
+  <si>
+    <t>14.4.1</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil der unter 30-Jährigen an der Beschäftigtenzahl in Prozent? Methodik analog zu ESRS S1-9.</t>
+  </si>
+  <si>
+    <t>14.4.2</t>
+  </si>
+  <si>
+    <t>14.4.3</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil der über 50-Jährigen an der Beschäftigtenzahl in Prozent? Methodik analog zu ESRS S1-9.</t>
+  </si>
+  <si>
+    <t>Wie hoch ist der Anteil der 30- bis 50-Jährigen an der Beschäftigtenzahl in Prozent? Methodik analog zu ESRS S1-9.</t>
+  </si>
+  <si>
+    <t>Anteil von unter Dreißigjährigen</t>
+  </si>
+  <si>
+    <t>Anteil von über Fünfzigjährigen</t>
+  </si>
+  <si>
+    <t>Anteil von Dreißig- bis Fünfzigjährigen</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>14.6</t>
+  </si>
+  <si>
+    <t>Fluktuationsquote</t>
+  </si>
+  <si>
+    <t>Durchschnittliche Anzahl an Trainingsstunden</t>
+  </si>
+  <si>
+    <t>Wieviele Tranings- und Fortbildungsstunden erhielten Beschäftigte im letzten abgeschlossenen Geschäftsjahr?</t>
+  </si>
+  <si>
+    <t>Wie hoch war die Fluktuationsquote im Unternehmen im letzten abgeschlossenen Geschäftsjahr?</t>
+  </si>
+  <si>
+    <t>15.1</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>17.1.1</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>17.2</t>
+  </si>
+  <si>
+    <t>Einbindung der Beschäftigten</t>
+  </si>
+  <si>
+    <t>Arbeitsschutz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risiken und Maßnahmen </t>
+  </si>
+  <si>
+    <t>Maßnahmen zur Reduzierung von Governance-Risiken</t>
+  </si>
+  <si>
+    <t>Maßnahmen zur Reduzierung von sozialen Risiken</t>
+  </si>
+  <si>
+    <t>Welche Maßnahmen hat das Unternehmen zur Reduzierung dieser sozialen Risiken getroffen, außer der in Frage 5.1 genannten Richtlinien?</t>
+  </si>
+  <si>
+    <t>Gibt es weitere wesentliche soziale Risiken für das Unternehmen?</t>
+  </si>
+  <si>
+    <t>Erläutern sie die weiteren wesentlichenn sozialen Risiken.</t>
+  </si>
+  <si>
+    <t>Weitere wesentliche soziale Risiken</t>
+  </si>
+  <si>
+    <t>Weitere wesentliche soziale Risiken Erläuterung</t>
+  </si>
+  <si>
+    <t>Anzahl der Arbeitsunfälle pro fünfhundert Vollzeitbeschäftigte</t>
+  </si>
+  <si>
+    <t>Wie hoch ist die Häufigkeitsrate von Arbeitsunfällen des Unternehmens pro 500 Vollzeitbeschäftigte?</t>
+  </si>
+  <si>
+    <t>Welche Maßnahmen hat das Unternehmen ergriffen, um die rechtlichen Vorgaben zum Schutz der Gesundheit und Verbesserung der Sicherheit von Beschäftigten umzusetzen?</t>
+  </si>
+  <si>
+    <t>Maßnahmen zum Schutz der Gesundheit und Verbesserung der Sicherheit</t>
+  </si>
+  <si>
+    <t>Sind Beschäftigte in betriebliche Entscheidungen des Unternehmens eingebunden?</t>
+  </si>
+  <si>
+    <t>Bei Unternehmen, die aufgrund länderspezifischer Besonderheiten nicht zu einer eindeutigen Antwort kommen, bitte hier erläutern.</t>
+  </si>
+  <si>
+    <t>Einbindung von Beschäftigten in Entscheidungen</t>
+  </si>
+  <si>
+    <t>Einbindung von Beschäftigten in Entscheidungen Erläuterungen</t>
+  </si>
+  <si>
+    <t>Einbindung in Betriebsrat / gesetzliche Vertretungsorgane | Aufsichtsrat | Verwaltungsrat | Keine Einbindung in Entscheidungsgremien | Kein Arbeitnehmervertretung gesetzlich vorgeschrieben</t>
   </si>
 </sst>
 </file>
@@ -2595,25 +2897,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="E141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H170" sqref="H170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1"/>
-    <col min="2" max="2" width="18.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="122.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="85.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.36328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.54296875" style="2" customWidth="1"/>
-    <col min="9" max="10" width="12.54296875" style="2"/>
-    <col min="11" max="11" width="12.54296875" style="1"/>
-    <col min="12" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="1" width="12.5703125" style="1"/>
+    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="122.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="12.5703125" style="2"/>
+    <col min="11" max="11" width="12.5703125" style="1"/>
+    <col min="12" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2657,7 +2959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="38.5">
+    <row r="2" spans="1:13" ht="39">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -2744,7 +3046,7 @@
       </c>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:13" ht="26">
+    <row r="5" spans="1:13" ht="26.25">
       <c r="A5" s="23" t="s">
         <v>26</v>
       </c>
@@ -4010,7 +4312,7 @@
       </c>
       <c r="M44" s="15"/>
     </row>
-    <row r="45" spans="1:13" ht="26">
+    <row r="45" spans="1:13" ht="26.25">
       <c r="A45" s="81" t="s">
         <v>41</v>
       </c>
@@ -4045,7 +4347,7 @@
       </c>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="1:13" ht="26">
+    <row r="46" spans="1:13" ht="26.25">
       <c r="A46" s="81" t="s">
         <v>49</v>
       </c>
@@ -4080,7 +4382,7 @@
       </c>
       <c r="M46" s="15"/>
     </row>
-    <row r="47" spans="1:13" ht="26">
+    <row r="47" spans="1:13" ht="26.25">
       <c r="A47" s="81" t="s">
         <v>528</v>
       </c>
@@ -4115,7 +4417,7 @@
       </c>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="1:13" ht="26">
+    <row r="48" spans="1:13" ht="26.25">
       <c r="A48" s="81" t="s">
         <v>529</v>
       </c>
@@ -4150,7 +4452,7 @@
       </c>
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="1:13" ht="26">
+    <row r="49" spans="1:13" ht="26.25">
       <c r="A49" s="81" t="s">
         <v>530</v>
       </c>
@@ -4185,7 +4487,7 @@
       </c>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="1:13" ht="26">
+    <row r="50" spans="1:13" ht="26.25">
       <c r="A50" s="81" t="s">
         <v>532</v>
       </c>
@@ -4220,7 +4522,7 @@
       </c>
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" ht="26.25">
       <c r="A51" s="81" t="s">
         <v>534</v>
       </c>
@@ -4255,7 +4557,7 @@
       </c>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" ht="26.25">
       <c r="A52" s="81" t="s">
         <v>57</v>
       </c>
@@ -4286,7 +4588,7 @@
       </c>
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="1:13" ht="26">
+    <row r="53" spans="1:13" ht="26.25">
       <c r="A53" s="81" t="s">
         <v>551</v>
       </c>
@@ -4352,7 +4654,7 @@
       </c>
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="1:13" ht="26">
+    <row r="55" spans="1:13" ht="26.25">
       <c r="A55" s="81" t="s">
         <v>60</v>
       </c>
@@ -4383,7 +4685,7 @@
       </c>
       <c r="M55" s="69"/>
     </row>
-    <row r="56" spans="1:13" ht="26">
+    <row r="56" spans="1:13" ht="26.25">
       <c r="A56" s="81" t="s">
         <v>61</v>
       </c>
@@ -4449,7 +4751,7 @@
       </c>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="1:13" ht="26">
+    <row r="58" spans="1:13" ht="26.25">
       <c r="A58" s="81" t="s">
         <v>62</v>
       </c>
@@ -4575,7 +4877,7 @@
       </c>
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="1:13" ht="26">
+    <row r="62" spans="1:13" ht="26.25">
       <c r="A62" s="26" t="s">
         <v>555</v>
       </c>
@@ -4610,7 +4912,7 @@
       </c>
       <c r="M62" s="15"/>
     </row>
-    <row r="63" spans="1:13" ht="26">
+    <row r="63" spans="1:13" ht="26.25">
       <c r="A63" s="26" t="s">
         <v>566</v>
       </c>
@@ -4645,7 +4947,7 @@
       </c>
       <c r="M63" s="15"/>
     </row>
-    <row r="64" spans="1:13" ht="26">
+    <row r="64" spans="1:13" ht="26.25">
       <c r="A64" s="26" t="s">
         <v>565</v>
       </c>
@@ -5095,7 +5397,7 @@
       </c>
       <c r="M77" s="15"/>
     </row>
-    <row r="78" spans="1:13" ht="26">
+    <row r="78" spans="1:13" ht="26.25">
       <c r="A78" s="26" t="s">
         <v>127</v>
       </c>
@@ -5159,7 +5461,7 @@
       </c>
       <c r="M79" s="15"/>
     </row>
-    <row r="80" spans="1:13" ht="38.5">
+    <row r="80" spans="1:13" ht="39">
       <c r="A80" s="26" t="s">
         <v>135</v>
       </c>
@@ -5192,7 +5494,7 @@
       </c>
       <c r="M80" s="15"/>
     </row>
-    <row r="81" spans="1:13" ht="26">
+    <row r="81" spans="1:13" ht="26.25">
       <c r="A81" s="26" t="s">
         <v>142</v>
       </c>
@@ -5223,7 +5525,7 @@
       </c>
       <c r="M81" s="15"/>
     </row>
-    <row r="82" spans="1:13" ht="38.5">
+    <row r="82" spans="1:13" ht="39">
       <c r="A82" s="26" t="s">
         <v>145</v>
       </c>
@@ -5384,7 +5686,7 @@
       </c>
       <c r="M86" s="15"/>
     </row>
-    <row r="87" spans="1:13" ht="28.5">
+    <row r="87" spans="1:13" ht="29.25">
       <c r="A87" s="26" t="s">
         <v>165</v>
       </c>
@@ -5450,7 +5752,7 @@
       </c>
       <c r="M88" s="15"/>
     </row>
-    <row r="89" spans="1:13" ht="28.5">
+    <row r="89" spans="1:13" ht="29.25">
       <c r="A89" s="26" t="s">
         <v>174</v>
       </c>
@@ -5483,7 +5785,7 @@
       </c>
       <c r="M89" s="15"/>
     </row>
-    <row r="90" spans="1:13" ht="28.5">
+    <row r="90" spans="1:13" ht="29.25">
       <c r="A90" s="26" t="s">
         <v>176</v>
       </c>
@@ -5516,7 +5818,7 @@
       </c>
       <c r="M90" s="15"/>
     </row>
-    <row r="91" spans="1:13" ht="28.5">
+    <row r="91" spans="1:13" ht="29.25">
       <c r="A91" s="26" t="s">
         <v>181</v>
       </c>
@@ -5549,7 +5851,7 @@
       </c>
       <c r="M91" s="15"/>
     </row>
-    <row r="92" spans="1:13" ht="42.5">
+    <row r="92" spans="1:13" ht="43.5">
       <c r="A92" s="26" t="s">
         <v>183</v>
       </c>
@@ -5582,7 +5884,7 @@
       </c>
       <c r="M92" s="15"/>
     </row>
-    <row r="93" spans="1:13" ht="26">
+    <row r="93" spans="1:13" ht="26.25">
       <c r="A93" s="26" t="s">
         <v>188</v>
       </c>
@@ -5615,7 +5917,7 @@
       </c>
       <c r="M93" s="15"/>
     </row>
-    <row r="94" spans="1:13" ht="28.5">
+    <row r="94" spans="1:13" ht="29.25">
       <c r="A94" s="26" t="s">
         <v>190</v>
       </c>
@@ -5648,7 +5950,7 @@
       </c>
       <c r="M94" s="15"/>
     </row>
-    <row r="95" spans="1:13" ht="26">
+    <row r="95" spans="1:13" ht="26.25">
       <c r="A95" s="26" t="s">
         <v>194</v>
       </c>
@@ -5679,7 +5981,7 @@
       </c>
       <c r="M95" s="15"/>
     </row>
-    <row r="96" spans="1:13" ht="26">
+    <row r="96" spans="1:13" ht="26.25">
       <c r="A96" s="26" t="s">
         <v>197</v>
       </c>
@@ -5710,7 +6012,7 @@
       </c>
       <c r="M96" s="15"/>
     </row>
-    <row r="97" spans="1:13" ht="38.5">
+    <row r="97" spans="1:13" ht="39">
       <c r="A97" s="26" t="s">
         <v>201</v>
       </c>
@@ -5743,7 +6045,7 @@
       </c>
       <c r="M97" s="15"/>
     </row>
-    <row r="98" spans="1:13" ht="26">
+    <row r="98" spans="1:13" ht="26.25">
       <c r="A98" s="26" t="s">
         <v>205</v>
       </c>
@@ -5774,7 +6076,7 @@
       </c>
       <c r="M98" s="15"/>
     </row>
-    <row r="99" spans="1:13" ht="38.5">
+    <row r="99" spans="1:13" ht="39">
       <c r="A99" s="26" t="s">
         <v>208</v>
       </c>
@@ -5807,7 +6109,7 @@
       </c>
       <c r="M99" s="15"/>
     </row>
-    <row r="100" spans="1:13" ht="26">
+    <row r="100" spans="1:13" ht="26.25">
       <c r="A100" s="26" t="s">
         <v>212</v>
       </c>
@@ -5838,7 +6140,7 @@
       </c>
       <c r="M100" s="15"/>
     </row>
-    <row r="101" spans="1:13" ht="28.5">
+    <row r="101" spans="1:13" ht="29.25">
       <c r="A101" s="26" t="s">
         <v>216</v>
       </c>
@@ -5935,7 +6237,7 @@
       </c>
       <c r="M103" s="15"/>
     </row>
-    <row r="104" spans="1:13" ht="38.5">
+    <row r="104" spans="1:13" ht="39">
       <c r="A104" s="26" t="s">
         <v>229</v>
       </c>
@@ -6131,7 +6433,7 @@
       </c>
       <c r="M109" s="15"/>
     </row>
-    <row r="110" spans="1:13" ht="26">
+    <row r="110" spans="1:13" ht="26.25">
       <c r="A110" s="26" t="s">
         <v>255</v>
       </c>
@@ -6164,7 +6466,7 @@
       </c>
       <c r="M110" s="15"/>
     </row>
-    <row r="111" spans="1:13" ht="26">
+    <row r="111" spans="1:13" ht="26.25">
       <c r="A111" s="26" t="s">
         <v>259</v>
       </c>
@@ -6292,7 +6594,7 @@
       </c>
       <c r="M114" s="15"/>
     </row>
-    <row r="115" spans="1:13" ht="26">
+    <row r="115" spans="1:13" ht="26.25">
       <c r="A115" s="26" t="s">
         <v>275</v>
       </c>
@@ -6325,7 +6627,7 @@
       </c>
       <c r="M115" s="15"/>
     </row>
-    <row r="116" spans="1:13" ht="26">
+    <row r="116" spans="1:13" ht="26.25">
       <c r="A116" s="26" t="s">
         <v>279</v>
       </c>
@@ -6358,7 +6660,7 @@
       </c>
       <c r="M116" s="15"/>
     </row>
-    <row r="117" spans="1:13" ht="26">
+    <row r="117" spans="1:13" ht="26.25">
       <c r="A117" s="26" t="s">
         <v>284</v>
       </c>
@@ -7304,7 +7606,7 @@
       </c>
       <c r="M146" s="15"/>
     </row>
-    <row r="147" spans="1:13" ht="26">
+    <row r="147" spans="1:13" ht="26.25">
       <c r="A147" s="44" t="s">
         <v>390</v>
       </c>
@@ -7434,7 +7736,7 @@
       </c>
       <c r="M150" s="15"/>
     </row>
-    <row r="151" spans="1:13" ht="38.5">
+    <row r="151" spans="1:13" ht="39">
       <c r="A151" s="57" t="s">
         <v>407</v>
       </c>
@@ -7463,6 +7765,898 @@
       <c r="L151" s="58" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="158" spans="1:13" ht="39">
+      <c r="A158" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C158" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D158" s="10" t="s">
+        <v>606</v>
+      </c>
+      <c r="E158" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="F158" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="G158" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="H158" s="14"/>
+      <c r="I158" s="14"/>
+      <c r="J158" s="15"/>
+      <c r="K158" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L158" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M158" s="15"/>
+    </row>
+    <row r="159" spans="1:13">
+      <c r="A159" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C159" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D159" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="E159" s="12" t="s">
+        <v>611</v>
+      </c>
+      <c r="F159" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="G159" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H159" s="14"/>
+      <c r="I159" s="14"/>
+      <c r="J159" s="15"/>
+      <c r="K159" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L159" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M159" s="15"/>
+    </row>
+    <row r="160" spans="1:13">
+      <c r="A160" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C160" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D160" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="E160" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="F160" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="G160" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H160" s="14"/>
+      <c r="I160" s="14"/>
+      <c r="J160" s="15"/>
+      <c r="K160" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L160" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M160" s="15"/>
+    </row>
+    <row r="161" spans="1:13">
+      <c r="A161" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C161" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D161" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="E161" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="F161" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="G161" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H161" s="14"/>
+      <c r="I161" s="14"/>
+      <c r="J161" s="15"/>
+      <c r="K161" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L161" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M161" s="15"/>
+    </row>
+    <row r="162" spans="1:13" ht="26.25">
+      <c r="A162" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C162" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D162" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="E162" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="F162" s="12"/>
+      <c r="G162" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H162" s="14"/>
+      <c r="I162" s="14"/>
+      <c r="J162" s="15"/>
+      <c r="K162" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L162" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M162" s="15"/>
+    </row>
+    <row r="163" spans="1:13" ht="26.25">
+      <c r="A163" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C163" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D163" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="E163" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="F163" s="12"/>
+      <c r="G163" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H163" s="14"/>
+      <c r="I163" s="14"/>
+      <c r="J163" s="15"/>
+      <c r="K163" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L163" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M163" s="15"/>
+    </row>
+    <row r="164" spans="1:13">
+      <c r="A164" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C164" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D164" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="F164" s="12"/>
+      <c r="G164" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H164" s="14"/>
+      <c r="I164" s="14"/>
+      <c r="J164" s="15"/>
+      <c r="K164" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L164" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M164" s="15"/>
+    </row>
+    <row r="165" spans="1:13">
+      <c r="A165" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C165" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D165" s="10" t="s">
+        <v>633</v>
+      </c>
+      <c r="E165" s="12" t="s">
+        <v>630</v>
+      </c>
+      <c r="F165" s="12"/>
+      <c r="G165" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H165" s="14"/>
+      <c r="I165" s="14"/>
+      <c r="J165" s="15"/>
+      <c r="K165" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L165" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M165" s="15"/>
+    </row>
+    <row r="166" spans="1:13">
+      <c r="A166" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C166" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D166" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="F166" s="12"/>
+      <c r="G166" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H166" s="14"/>
+      <c r="I166" s="14"/>
+      <c r="J166" s="15"/>
+      <c r="K166" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L166" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M166" s="15"/>
+    </row>
+    <row r="167" spans="1:13">
+      <c r="A167" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C167" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D167" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="E167" s="12" t="s">
+        <v>638</v>
+      </c>
+      <c r="F167" s="12"/>
+      <c r="G167" s="75" t="s">
+        <v>120</v>
+      </c>
+      <c r="H167" s="14"/>
+      <c r="I167" s="14"/>
+      <c r="J167" s="15"/>
+      <c r="K167" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L167" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M167" s="15"/>
+    </row>
+    <row r="168" spans="1:13">
+      <c r="A168" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C168" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="D168" s="10" t="s">
+        <v>636</v>
+      </c>
+      <c r="E168" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="F168" s="12"/>
+      <c r="G168" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H168" s="14"/>
+      <c r="I168" s="14"/>
+      <c r="J168" s="15"/>
+      <c r="K168" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L168" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M168" s="15"/>
+    </row>
+    <row r="169" spans="1:13">
+      <c r="A169" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C169" s="41" t="s">
+        <v>645</v>
+      </c>
+      <c r="D169" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="F169" s="12"/>
+      <c r="G169" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="H169" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="I169" s="14"/>
+      <c r="J169" s="15"/>
+      <c r="K169" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L169" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M169" s="15"/>
+    </row>
+    <row r="170" spans="1:13">
+      <c r="A170" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C170" s="41" t="s">
+        <v>645</v>
+      </c>
+      <c r="D170" s="10" t="s">
+        <v>662</v>
+      </c>
+      <c r="E170" s="12" t="s">
+        <v>660</v>
+      </c>
+      <c r="F170" s="12"/>
+      <c r="G170" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H170" s="14"/>
+      <c r="I170" s="14"/>
+      <c r="J170" s="15"/>
+      <c r="K170" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L170" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M170" s="15"/>
+    </row>
+    <row r="171" spans="1:13" ht="26.25">
+      <c r="A171" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C171" s="41" t="s">
+        <v>646</v>
+      </c>
+      <c r="D171" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="E171" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="F171" s="12"/>
+      <c r="G171" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H171" s="14"/>
+      <c r="I171" s="14"/>
+      <c r="J171" s="15"/>
+      <c r="K171" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L171" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M171" s="15"/>
+    </row>
+    <row r="172" spans="1:13">
+      <c r="A172" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C172" s="41" t="s">
+        <v>646</v>
+      </c>
+      <c r="D172" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="E172" s="12" t="s">
+        <v>656</v>
+      </c>
+      <c r="F172" s="12"/>
+      <c r="G172" s="75" t="s">
+        <v>120</v>
+      </c>
+      <c r="H172" s="14"/>
+      <c r="I172" s="14"/>
+      <c r="J172" s="15"/>
+      <c r="K172" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L172" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M172" s="15"/>
+    </row>
+    <row r="173" spans="1:13">
+      <c r="A173" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C173" s="41" t="s">
+        <v>647</v>
+      </c>
+      <c r="D173" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="E173" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="F173" s="12"/>
+      <c r="G173" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H173" s="14"/>
+      <c r="I173" s="14"/>
+      <c r="J173" s="15"/>
+      <c r="K173" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L173" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M173" s="15"/>
+    </row>
+    <row r="174" spans="1:13">
+      <c r="A174" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C174" s="41" t="s">
+        <v>647</v>
+      </c>
+      <c r="D174" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="E174" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="F174" s="12"/>
+      <c r="G174" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H174" s="14"/>
+      <c r="I174" s="14"/>
+      <c r="J174" s="15"/>
+      <c r="K174" s="47" t="s">
+        <v>643</v>
+      </c>
+      <c r="L174" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M174" s="15"/>
+    </row>
+    <row r="175" spans="1:13">
+      <c r="A175" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C175" s="41" t="s">
+        <v>647</v>
+      </c>
+      <c r="D175" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="E175" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="F175" s="12"/>
+      <c r="G175" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H175" s="14"/>
+      <c r="I175" s="14"/>
+      <c r="J175" s="15"/>
+      <c r="K175" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L175" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M175" s="15"/>
+    </row>
+    <row r="176" spans="1:13">
+      <c r="A176" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C176" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D176" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="E176" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="F176" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="G176" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H176" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="I176" s="14"/>
+      <c r="J176" s="15"/>
+      <c r="K176" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L176" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M176" s="15"/>
+    </row>
+    <row r="177" spans="1:13">
+      <c r="A177" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C177" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D177" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="E177" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="F177" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="G177" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H177" s="14"/>
+      <c r="I177" s="14"/>
+      <c r="J177" s="15"/>
+      <c r="K177" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L177" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M177" s="15"/>
+    </row>
+    <row r="178" spans="1:13">
+      <c r="A178" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C178" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D178" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="E178" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="F178" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="G178" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H178" s="14"/>
+      <c r="I178" s="14"/>
+      <c r="J178" s="15"/>
+      <c r="K178" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L178" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M178" s="15"/>
+    </row>
+    <row r="179" spans="1:13">
+      <c r="A179" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C179" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D179" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="E179" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="F179" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="G179" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="H179" s="14"/>
+      <c r="I179" s="14"/>
+      <c r="J179" s="15"/>
+      <c r="K179" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L179" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M179" s="15"/>
+    </row>
+    <row r="180" spans="1:13">
+      <c r="A180" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C180" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D180" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E180" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="F180" s="12"/>
+      <c r="G180" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H180" s="14"/>
+      <c r="I180" s="14"/>
+      <c r="J180" s="15"/>
+      <c r="K180" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L180" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M180" s="15"/>
+    </row>
+    <row r="181" spans="1:13">
+      <c r="A181" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C181" s="41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D181" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="E181" s="12" t="s">
+        <v>600</v>
+      </c>
+      <c r="F181" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="G181" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H181" s="14"/>
+      <c r="I181" s="14"/>
+      <c r="J181" s="15"/>
+      <c r="K181" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="L181" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M181" s="15"/>
+    </row>
+    <row r="182" spans="1:13" ht="26.25">
+      <c r="A182" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C182" s="41" t="s">
+        <v>585</v>
+      </c>
+      <c r="D182" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="E182" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="F182" s="12"/>
+      <c r="G182" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H182" s="14"/>
+      <c r="I182" s="14"/>
+      <c r="J182" s="15"/>
+      <c r="K182" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L182" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M182" s="15"/>
+    </row>
+    <row r="183" spans="1:13">
+      <c r="A183" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C183" s="41" t="s">
+        <v>585</v>
+      </c>
+      <c r="D183" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="E183" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="F183" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="G183" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H183" s="14"/>
+      <c r="I183" s="14"/>
+      <c r="J183" s="15"/>
+      <c r="K183" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="L183" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M183" s="15"/>
+    </row>
+    <row r="184" spans="1:13">
+      <c r="A184" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C184" s="41" t="s">
+        <v>586</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="E184" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="F184" s="12"/>
+      <c r="G184" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H184" s="14"/>
+      <c r="I184" s="14"/>
+      <c r="J184" s="15"/>
+      <c r="K184" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L184" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M184" s="15"/>
+    </row>
+    <row r="185" spans="1:13" ht="26.25">
+      <c r="A185" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C185" s="41" t="s">
+        <v>586</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="E185" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="F185" s="12"/>
+      <c r="G185" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H185" s="14"/>
+      <c r="I185" s="14"/>
+      <c r="J185" s="15"/>
+      <c r="K185" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="L185" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M185" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
some cleanup and also some work on EsgQuestionnairePreparedFixtures.ts
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784EF707-EF4E-48F8-A621-712E3C79B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7149841D-3517-4E66-88E4-CDC54C990FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="513">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -418,9 +418,6 @@
     <t>Welche grundsätzlichen Chancen oder Hindernisse bestehen für das Unternehmen bei der Berücksichtigung von ESG-Belangen?</t>
   </si>
   <si>
-    <t>Taxonomie KPIs &amp; bestimmte Aktivitäten</t>
-  </si>
-  <si>
     <t>Wirtschaftszweige</t>
   </si>
   <si>
@@ -523,9 +520,6 @@
     <t>8.1.1</t>
   </si>
   <si>
-    <t>Aktivität im Sektor Fossile Brennstoffe</t>
-  </si>
-  <si>
     <t>Ist das Unternehmen im Sektor "Fossile Brennstoffe (Kohle, Gas, Öl)" aktiv?</t>
   </si>
   <si>
@@ -670,9 +664,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>ESG-Rating &amp; Zertifizierung</t>
-  </si>
-  <si>
     <t>9.1</t>
   </si>
   <si>
@@ -961,9 +952,6 @@
     <t>Welche Menge an gefährlichen Abfällen fielen im Unternehmen im letzten abgeschlossenen Geschäftsjahr (in t) an? Gefährliche Abfälle umfassen Abfälle, die bspw. eine der folgenden Eigenschaften aufweisen: explosiv, brandfördernden, entzündbar, reizend oder toxisch.</t>
   </si>
   <si>
-    <t>Risiken &amp; Maßnahmen Klima</t>
-  </si>
-  <si>
     <t>Transitorische Klima- und Umweltrisiken</t>
   </si>
   <si>
@@ -1595,6 +1583,15 @@
   </si>
   <si>
     <t>52.2</t>
+  </si>
+  <si>
+    <t>Aktivität im Sektor "Fossile Brennstoffe"</t>
+  </si>
+  <si>
+    <t>Taxonomie KPIs und bestimmte Aktivitäten</t>
+  </si>
+  <si>
+    <t>ESG-Rating und Zertifizierung</t>
   </si>
 </sst>
 </file>
@@ -2511,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2773,7 +2770,7 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="17" t="s">
@@ -2806,7 +2803,7 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="17" t="s">
@@ -2839,7 +2836,7 @@
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="23" t="s">
@@ -2872,7 +2869,7 @@
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="23" t="s">
@@ -2894,7 +2891,7 @@
         <v>97</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" s="39" t="s">
         <v>118</v>
@@ -2905,7 +2902,7 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="23" t="s">
@@ -2927,10 +2924,10 @@
         <v>97</v>
       </c>
       <c r="D13" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="39" t="s">
         <v>142</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>143</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="20" t="s">
@@ -2938,7 +2935,7 @@
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="23" t="s">
@@ -2988,17 +2985,17 @@
         <v>25</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="45" t="s">
         <v>122</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>123</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -3019,13 +3016,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D16" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="45" t="s">
         <v>125</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>126</v>
       </c>
       <c r="F16" s="27"/>
       <c r="G16" s="20" t="s">
@@ -3033,7 +3030,7 @@
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="23" t="s">
@@ -3046,19 +3043,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="20" t="s">
@@ -3066,7 +3063,7 @@
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="23" t="s">
@@ -3079,19 +3076,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="20" t="s">
@@ -3099,7 +3096,7 @@
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="23" t="s">
@@ -3112,19 +3109,19 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E19" s="47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="20" t="s">
@@ -3132,7 +3129,7 @@
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="23" t="s">
@@ -3145,19 +3142,19 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="46" t="s">
         <v>137</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>138</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="20" t="s">
@@ -3165,7 +3162,7 @@
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="23" t="s">
@@ -3178,19 +3175,19 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D21" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="47" t="s">
         <v>139</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>140</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="20" t="s">
@@ -3198,7 +3195,7 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="23" t="s">
@@ -3211,19 +3208,19 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D22" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="47" t="s">
         <v>144</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>145</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="20" t="s">
@@ -3242,29 +3239,29 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D23" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="47" t="s">
         <v>148</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>149</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="28"/>
       <c r="J23" s="12"/>
       <c r="K23" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L23" s="26" t="s">
         <v>19</v>
@@ -3273,29 +3270,29 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D24" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="47" t="s">
         <v>153</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>154</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="28"/>
       <c r="J24" s="12"/>
       <c r="K24" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L24" s="26" t="s">
         <v>19</v>
@@ -3304,19 +3301,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>156</v>
+        <v>511</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>510</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F25" s="27"/>
       <c r="G25" s="20" t="s">
@@ -3335,29 +3332,29 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="28"/>
       <c r="J26" s="12"/>
       <c r="K26" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L26" s="26" t="s">
         <v>19</v>
@@ -3366,29 +3363,29 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E27" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="28"/>
       <c r="J27" s="12"/>
       <c r="K27" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L27" s="26" t="s">
         <v>19</v>
@@ -3397,29 +3394,29 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E28" s="47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="28"/>
       <c r="J28" s="12"/>
       <c r="K28" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L28" s="26" t="s">
         <v>19</v>
@@ -3428,19 +3425,19 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E29" s="47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="20" t="s">
@@ -3459,29 +3456,29 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="28"/>
       <c r="J30" s="12"/>
       <c r="K30" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L30" s="26" t="s">
         <v>19</v>
@@ -3490,29 +3487,29 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="28"/>
       <c r="J31" s="12"/>
       <c r="K31" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L31" s="26" t="s">
         <v>19</v>
@@ -3521,29 +3518,29 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="28"/>
       <c r="J32" s="12"/>
       <c r="K32" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L32" s="26" t="s">
         <v>19</v>
@@ -3552,19 +3549,19 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E33" s="47" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F33" s="27"/>
       <c r="G33" s="20" t="s">
@@ -3583,29 +3580,29 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E34" s="47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="28"/>
       <c r="J34" s="12"/>
       <c r="K34" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L34" s="26" t="s">
         <v>19</v>
@@ -3614,29 +3611,29 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="28"/>
       <c r="J35" s="12"/>
       <c r="K35" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L35" s="26" t="s">
         <v>19</v>
@@ -3645,29 +3642,29 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="28"/>
       <c r="J36" s="12"/>
       <c r="K36" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L36" s="26" t="s">
         <v>19</v>
@@ -3676,19 +3673,19 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E37" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F37" s="27"/>
       <c r="G37" s="20" t="s">
@@ -3707,29 +3704,29 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E38" s="47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F38" s="27"/>
       <c r="G38" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="28"/>
       <c r="J38" s="12"/>
       <c r="K38" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L38" s="26" t="s">
         <v>19</v>
@@ -3738,29 +3735,29 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E39" s="47" t="s">
         <v>200</v>
-      </c>
-      <c r="E39" s="47" t="s">
-        <v>202</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="28"/>
       <c r="J39" s="12"/>
       <c r="K39" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L39" s="26" t="s">
         <v>19</v>
@@ -3769,29 +3766,29 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="47" t="s">
         <v>201</v>
-      </c>
-      <c r="E40" s="47" t="s">
-        <v>203</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="28"/>
       <c r="J40" s="12"/>
       <c r="K40" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L40" s="26" t="s">
         <v>19</v>
@@ -3800,13 +3797,13 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>65</v>
@@ -3831,16 +3828,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="E42" s="39" t="s">
         <v>67</v>
@@ -3853,7 +3850,7 @@
       <c r="I42" s="11"/>
       <c r="J42" s="12"/>
       <c r="K42" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>19</v>
@@ -3862,16 +3859,16 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E43" s="39" t="s">
         <v>69</v>
@@ -3884,7 +3881,7 @@
       <c r="I43" s="11"/>
       <c r="J43" s="15"/>
       <c r="K43" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>19</v>
@@ -3893,13 +3890,13 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>70</v>
@@ -3917,7 +3914,7 @@
         <v>36</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L44" s="12" t="s">
         <v>19</v>
@@ -3932,16 +3929,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G45" s="25" t="s">
         <v>18</v>
@@ -3967,16 +3964,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G46" s="25" t="s">
         <v>18</v>
@@ -3996,22 +3993,22 @@
     </row>
     <row r="47" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A47" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G47" s="25" t="s">
         <v>18</v>
@@ -4031,22 +4028,22 @@
     </row>
     <row r="48" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A48" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>40</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G48" s="25" t="s">
         <v>18</v>
@@ -4066,22 +4063,22 @@
     </row>
     <row r="49" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G49" s="25" t="s">
         <v>18</v>
@@ -4101,22 +4098,22 @@
     </row>
     <row r="50" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G50" s="25" t="s">
         <v>18</v>
@@ -4136,22 +4133,22 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>205</v>
+        <v>512</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G51" s="25" t="s">
         <v>18</v>
@@ -4177,7 +4174,7 @@
         <v>25</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>42</v>
@@ -4202,19 +4199,19 @@
     </row>
     <row r="53" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A53" s="34" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D53" s="21" t="s">
         <v>44</v>
       </c>
       <c r="E53" s="35" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>45</v>
@@ -4235,13 +4232,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>46</v>
@@ -4332,7 +4329,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>25</v>
@@ -4371,10 +4368,10 @@
         <v>25</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E58" s="39" t="s">
         <v>58</v>
@@ -4402,20 +4399,20 @@
         <v>25</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E59" s="38" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I59" s="11"/>
       <c r="J59" s="12"/>
@@ -4435,13 +4432,13 @@
         <v>25</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E60" s="38" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F60" s="27"/>
       <c r="G60" s="29" t="s">
@@ -4460,7 +4457,7 @@
     </row>
     <row r="61" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A61" s="34" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>25</v>
@@ -4469,10 +4466,10 @@
         <v>63</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="15" t="s">
@@ -4500,10 +4497,10 @@
         <v>63</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E62" s="38" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="29" t="s">
@@ -4513,7 +4510,7 @@
       <c r="I62" s="11"/>
       <c r="J62" s="12"/>
       <c r="K62" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L62" s="12" t="s">
         <v>19</v>
@@ -4528,10 +4525,10 @@
         <v>25</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>73</v>
@@ -4553,19 +4550,19 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C64" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D64" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="D64" s="21" t="s">
-        <v>255</v>
-      </c>
       <c r="E64" s="38" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="29" t="s">
@@ -4590,10 +4587,10 @@
         <v>25</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>75</v>
@@ -4615,19 +4612,19 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="34" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E66" s="38" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="29" t="s">
@@ -4646,19 +4643,19 @@
     </row>
     <row r="67" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A67" s="34" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="21" t="s">
@@ -4666,7 +4663,7 @@
       </c>
       <c r="H67" s="11"/>
       <c r="I67" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="17" t="s">
@@ -4679,19 +4676,19 @@
     </row>
     <row r="68" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A68" s="34" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D68" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E68" s="31" t="s">
         <v>269</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>272</v>
       </c>
       <c r="F68" s="41"/>
       <c r="G68" s="21" t="s">
@@ -4699,7 +4696,7 @@
       </c>
       <c r="H68" s="11"/>
       <c r="I68" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="17" t="s">
@@ -4712,19 +4709,19 @@
     </row>
     <row r="69" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A69" s="34" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F69" s="41"/>
       <c r="G69" s="21" t="s">
@@ -4732,7 +4729,7 @@
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="17" t="s">
@@ -4745,19 +4742,19 @@
     </row>
     <row r="70" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A70" s="34" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F70" s="41"/>
       <c r="G70" s="21" t="s">
@@ -4765,7 +4762,7 @@
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="17" t="s">
@@ -4784,13 +4781,13 @@
         <v>78</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E71" s="38" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F71" s="41"/>
       <c r="G71" s="29" t="s">
@@ -4798,7 +4795,7 @@
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="17" t="s">
@@ -4817,13 +4814,13 @@
         <v>78</v>
       </c>
       <c r="C72" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E72" s="38" t="s">
         <v>279</v>
-      </c>
-      <c r="D72" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="E72" s="38" t="s">
-        <v>282</v>
       </c>
       <c r="F72" s="41"/>
       <c r="G72" s="29" t="s">
@@ -4831,7 +4828,7 @@
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="17" t="s">
@@ -4844,19 +4841,19 @@
     </row>
     <row r="73" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A73" s="34" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E73" s="38" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F73" s="41"/>
       <c r="G73" s="29" t="s">
@@ -4864,7 +4861,7 @@
       </c>
       <c r="H73" s="11"/>
       <c r="I73" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="17" t="s">
@@ -4877,19 +4874,19 @@
     </row>
     <row r="74" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A74" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="29" t="s">
@@ -4897,7 +4894,7 @@
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="17" t="s">
@@ -4916,13 +4913,13 @@
         <v>78</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>83</v>
       </c>
       <c r="E75" s="38" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F75" s="41"/>
       <c r="G75" s="29" t="s">
@@ -4930,7 +4927,7 @@
       </c>
       <c r="H75" s="11"/>
       <c r="I75" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="17" t="s">
@@ -4943,23 +4940,23 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="34" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C76" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="D76" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D76" s="21" t="s">
-        <v>290</v>
-      </c>
       <c r="E76" s="42" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F76" s="41"/>
       <c r="G76" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
@@ -4980,13 +4977,13 @@
         <v>78</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D77" s="21" t="s">
         <v>87</v>
       </c>
       <c r="E77" s="38" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F77" s="41"/>
       <c r="G77" s="29" t="s">
@@ -4994,7 +4991,7 @@
       </c>
       <c r="H77" s="11"/>
       <c r="I77" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="17" t="s">
@@ -5013,13 +5010,13 @@
         <v>78</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E78" s="38" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F78" s="41"/>
       <c r="G78" s="29" t="s">
@@ -5027,7 +5024,7 @@
       </c>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="17" t="s">
@@ -5040,23 +5037,23 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="34" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E79" s="38" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
@@ -5077,13 +5074,13 @@
         <v>78</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E80" s="38" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F80" s="41"/>
       <c r="G80" s="29" t="s">
@@ -5091,7 +5088,7 @@
       </c>
       <c r="H80" s="11"/>
       <c r="I80" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="17" t="s">
@@ -5109,14 +5106,14 @@
       <c r="B81" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="16" t="s">
-        <v>302</v>
+      <c r="C81" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E81" s="38" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F81" s="41"/>
       <c r="G81" s="29" t="s">
@@ -5135,26 +5132,26 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="34" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C82" s="105" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E82" s="38" t="s">
         <v>302</v>
-      </c>
-      <c r="D82" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="E82" s="38" t="s">
-        <v>306</v>
       </c>
       <c r="F82" s="41"/>
       <c r="G82" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I82" s="11"/>
       <c r="J82" s="12"/>
@@ -5168,19 +5165,19 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="34" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C83" s="16" t="s">
-        <v>302</v>
+      <c r="C83" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E83" s="38" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F83" s="41"/>
       <c r="G83" s="29" t="s">
@@ -5204,14 +5201,14 @@
       <c r="B84" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="16" t="s">
-        <v>302</v>
+      <c r="C84" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E84" s="38" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="29" t="s">
@@ -5230,19 +5227,19 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="34" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C85" s="16" t="s">
-        <v>302</v>
+      <c r="C85" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E85" s="38" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F85" s="41"/>
       <c r="G85" s="29" t="s">
@@ -5261,19 +5258,19 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="34" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C86" s="16" t="s">
-        <v>302</v>
+      <c r="C86" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E86" s="38" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="29" t="s">
@@ -5292,19 +5289,19 @@
     </row>
     <row r="87" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A87" s="34" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="16" t="s">
-        <v>302</v>
+      <c r="C87" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D87" s="55" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E87" s="56" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F87" s="41"/>
       <c r="G87" s="29" t="s">
@@ -5314,7 +5311,7 @@
       <c r="I87" s="11"/>
       <c r="J87" s="12"/>
       <c r="K87" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="L87" s="12" t="s">
         <v>19</v>
@@ -5323,19 +5320,19 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="34" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C88" s="16" t="s">
-        <v>302</v>
+      <c r="C88" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="29" t="s">
@@ -5354,19 +5351,19 @@
     </row>
     <row r="89" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A89" s="34" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C89" s="16" t="s">
-        <v>302</v>
+      <c r="C89" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E89" s="38" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F89" s="41"/>
       <c r="G89" s="29" t="s">
@@ -5376,7 +5373,7 @@
       <c r="I89" s="11"/>
       <c r="J89" s="12"/>
       <c r="K89" s="17" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="L89" s="12" t="s">
         <v>19</v>
@@ -5385,19 +5382,19 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="34" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C90" s="16" t="s">
-        <v>302</v>
+      <c r="C90" s="105" t="s">
+        <v>409</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E90" s="38" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F90" s="41"/>
       <c r="G90" s="29" t="s">
@@ -5418,19 +5415,19 @@
     </row>
     <row r="91" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A91" s="63" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B91" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C91" s="61" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E91" s="39" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F91" s="57"/>
       <c r="G91" s="60" t="s">
@@ -5449,19 +5446,19 @@
     </row>
     <row r="92" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A92" s="63" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B92" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C92" s="61" t="s">
+        <v>409</v>
+      </c>
+      <c r="D92" s="40" t="s">
+        <v>412</v>
+      </c>
+      <c r="E92" s="39" t="s">
         <v>413</v>
-      </c>
-      <c r="D92" s="40" t="s">
-        <v>416</v>
-      </c>
-      <c r="E92" s="39" t="s">
-        <v>417</v>
       </c>
       <c r="F92" s="57"/>
       <c r="G92" s="60" t="s">
@@ -5480,23 +5477,23 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="73" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B93" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C93" s="70" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E93" s="39" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F93" s="66"/>
       <c r="G93" s="69" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H93" s="67"/>
       <c r="I93" s="67"/>
@@ -5511,19 +5508,19 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="72" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B94" s="65" t="s">
         <v>78</v>
       </c>
       <c r="C94" s="70" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E94" s="39" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F94" s="66"/>
       <c r="G94" s="69" t="s">
@@ -5533,7 +5530,7 @@
       <c r="I94" s="67"/>
       <c r="J94" s="68"/>
       <c r="K94" s="71" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="L94" s="68" t="s">
         <v>19</v>
@@ -5542,23 +5539,23 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="63" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B95" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C95" s="78" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E95" s="39" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F95" s="74"/>
       <c r="G95" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H95" s="75"/>
       <c r="I95" s="75"/>
@@ -5573,23 +5570,23 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="63" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B96" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C96" s="78" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E96" s="39" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F96" s="74"/>
       <c r="G96" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H96" s="75"/>
       <c r="I96" s="75"/>
@@ -5604,23 +5601,23 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="63" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B97" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C97" s="78" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D97" s="40" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E97" s="39" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F97" s="74"/>
       <c r="G97" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H97" s="75"/>
       <c r="I97" s="75"/>
@@ -5635,19 +5632,19 @@
     </row>
     <row r="98" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A98" s="63" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B98" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C98" s="78" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D98" s="40" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E98" s="39" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F98" s="74"/>
       <c r="G98" s="77" t="s">
@@ -5666,19 +5663,19 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="73" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B99" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E99" s="39" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F99" s="80"/>
       <c r="G99" s="83" t="s">
@@ -5697,19 +5694,19 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="73" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B100" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E100" s="39" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F100" s="80"/>
       <c r="G100" s="83" t="s">
@@ -5719,7 +5716,7 @@
       <c r="I100" s="81"/>
       <c r="J100" s="82"/>
       <c r="K100" s="85" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="L100" s="82" t="s">
         <v>19</v>
@@ -5728,23 +5725,23 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="63" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B101" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C101" s="90" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D101" s="40" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E101" s="39" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F101" s="86"/>
       <c r="G101" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H101" s="87"/>
       <c r="I101" s="87"/>
@@ -5759,23 +5756,23 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="63" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B102" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C102" s="90" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E102" s="39" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F102" s="86"/>
       <c r="G102" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H102" s="87"/>
       <c r="I102" s="87"/>
@@ -5790,23 +5787,23 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="63" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B103" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C103" s="90" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D103" s="40" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E103" s="39" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F103" s="86"/>
       <c r="G103" s="89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H103" s="87"/>
       <c r="I103" s="87"/>
@@ -5821,19 +5818,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="63" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B104" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C104" s="90" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E104" s="39" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F104" s="86"/>
       <c r="G104" s="89" t="s">
@@ -5852,23 +5849,23 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="73" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B105" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C105" s="97" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E105" s="39" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F105" s="93"/>
       <c r="G105" s="96" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H105" s="94"/>
       <c r="I105" s="94"/>
@@ -5883,19 +5880,19 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="73" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B106" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C106" s="97" t="s">
+        <v>463</v>
+      </c>
+      <c r="D106" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="E106" s="39" t="s">
         <v>467</v>
-      </c>
-      <c r="D106" s="40" t="s">
-        <v>470</v>
-      </c>
-      <c r="E106" s="39" t="s">
-        <v>471</v>
       </c>
       <c r="F106" s="93"/>
       <c r="G106" s="96" t="s">
@@ -5905,7 +5902,7 @@
       <c r="I106" s="94"/>
       <c r="J106" s="95"/>
       <c r="K106" s="98" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="L106" s="95" t="s">
         <v>19</v>
@@ -5914,23 +5911,23 @@
     </row>
     <row r="107" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A107" s="73" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B107" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C107" s="97" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E107" s="39" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F107" s="93"/>
       <c r="G107" s="96" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H107" s="94"/>
       <c r="I107" s="94"/>
@@ -5945,23 +5942,23 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" s="73" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B108" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C108" s="97" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E108" s="39" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F108" s="93"/>
       <c r="G108" s="96" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H108" s="94"/>
       <c r="I108" s="94"/>
@@ -5976,19 +5973,19 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="73" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B109" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C109" s="97" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D109" s="40" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E109" s="39" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F109" s="93"/>
       <c r="G109" s="96" t="s">
@@ -5998,7 +5995,7 @@
       <c r="I109" s="94"/>
       <c r="J109" s="95"/>
       <c r="K109" s="98" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="L109" s="95" t="s">
         <v>19</v>
@@ -6007,23 +6004,23 @@
     </row>
     <row r="110" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="63" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B110" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C110" s="105" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D110" s="40" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E110" s="39" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F110" s="101"/>
       <c r="G110" s="104" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H110" s="102"/>
       <c r="I110" s="102"/>
@@ -6038,19 +6035,19 @@
     </row>
     <row r="111" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="63" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B111" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C111" s="105" t="s">
+        <v>479</v>
+      </c>
+      <c r="D111" s="40" t="s">
+        <v>482</v>
+      </c>
+      <c r="E111" s="39" t="s">
         <v>483</v>
-      </c>
-      <c r="D111" s="40" t="s">
-        <v>486</v>
-      </c>
-      <c r="E111" s="39" t="s">
-        <v>487</v>
       </c>
       <c r="F111" s="101"/>
       <c r="G111" s="104" t="s">
@@ -6060,7 +6057,7 @@
       <c r="I111" s="102"/>
       <c r="J111" s="103"/>
       <c r="K111" s="106" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="L111" s="103" t="s">
         <v>19</v>
@@ -6069,23 +6066,23 @@
     </row>
     <row r="112" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="63" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B112" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C112" s="105" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="E112" s="39" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F112" s="101"/>
       <c r="G112" s="104" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H112" s="102"/>
       <c r="I112" s="102"/>
@@ -6100,19 +6097,19 @@
     </row>
     <row r="113" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="63" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B113" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C113" s="105" t="s">
+        <v>479</v>
+      </c>
+      <c r="D113" s="40" t="s">
+        <v>486</v>
+      </c>
+      <c r="E113" s="39" t="s">
         <v>483</v>
-      </c>
-      <c r="D113" s="40" t="s">
-        <v>490</v>
-      </c>
-      <c r="E113" s="39" t="s">
-        <v>487</v>
       </c>
       <c r="F113" s="101"/>
       <c r="G113" s="104" t="s">
@@ -6122,7 +6119,7 @@
       <c r="I113" s="102"/>
       <c r="J113" s="103"/>
       <c r="K113" s="106" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="L113" s="103" t="s">
         <v>19</v>
@@ -6131,19 +6128,19 @@
     </row>
     <row r="114" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="63" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B114" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C114" s="105" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E114" s="39" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F114" s="101"/>
       <c r="G114" s="104" t="s">
@@ -6153,7 +6150,7 @@
       <c r="I114" s="102"/>
       <c r="J114" s="103"/>
       <c r="K114" s="106" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="L114" s="103" t="s">
         <v>19</v>
@@ -6162,23 +6159,23 @@
     </row>
     <row r="115" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="63" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B115" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C115" s="105" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E115" s="39" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F115" s="101"/>
       <c r="G115" s="104" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H115" s="102"/>
       <c r="I115" s="102"/>
@@ -6193,19 +6190,19 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="63" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B116" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C116" s="105" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F116" s="101"/>
       <c r="G116" s="104" t="s">
@@ -6215,7 +6212,7 @@
       <c r="I116" s="102"/>
       <c r="J116" s="103"/>
       <c r="K116" s="106" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="L116" s="103" t="s">
         <v>19</v>
@@ -6230,16 +6227,16 @@
         <v>89</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D117" s="110" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E117" s="111" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F117" s="49" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G117" s="50" t="s">
         <v>90</v>
@@ -6263,19 +6260,19 @@
         <v>89</v>
       </c>
       <c r="C118" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="D118" s="110" t="s">
         <v>323</v>
       </c>
-      <c r="D118" s="110" t="s">
-        <v>327</v>
-      </c>
       <c r="E118" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F118" s="49" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G118" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H118" s="51"/>
       <c r="I118" s="51"/>
@@ -6290,25 +6287,25 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="99" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B119" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D119" s="110" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E119" s="111" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F119" s="49" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G119" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H119" s="51"/>
       <c r="I119" s="51"/>
@@ -6323,25 +6320,25 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="99" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B120" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D120" s="110" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E120" s="111" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F120" s="49" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G120" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H120" s="51"/>
       <c r="I120" s="51"/>
@@ -6362,17 +6359,17 @@
         <v>89</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D121" s="110" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E121" s="111" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F121" s="49"/>
       <c r="G121" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H121" s="51"/>
       <c r="I121" s="51"/>
@@ -6393,17 +6390,17 @@
         <v>89</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D122" s="110" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E122" s="111" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F122" s="49"/>
       <c r="G122" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H122" s="51"/>
       <c r="I122" s="51"/>
@@ -6418,23 +6415,23 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="99" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B123" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D123" s="110" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E123" s="111" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F123" s="49"/>
       <c r="G123" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H123" s="51"/>
       <c r="I123" s="51"/>
@@ -6449,23 +6446,23 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="99" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B124" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D124" s="110" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E124" s="111" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F124" s="49"/>
       <c r="G124" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H124" s="51"/>
       <c r="I124" s="51"/>
@@ -6480,23 +6477,23 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="99" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B125" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D125" s="110" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E125" s="111" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F125" s="49"/>
       <c r="G125" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H125" s="51"/>
       <c r="I125" s="51"/>
@@ -6511,19 +6508,19 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="99" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B126" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D126" s="110" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E126" s="111" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F126" s="49"/>
       <c r="G126" s="54" t="s">
@@ -6542,23 +6539,23 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="99" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B127" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D127" s="110" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E127" s="111" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F127" s="49"/>
       <c r="G127" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H127" s="51"/>
       <c r="I127" s="51"/>
@@ -6573,26 +6570,26 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="99" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B128" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D128" s="110" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E128" s="111" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F128" s="49"/>
       <c r="G128" s="54" t="s">
         <v>30</v>
       </c>
       <c r="H128" s="51" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="I128" s="51"/>
       <c r="J128" s="52"/>
@@ -6606,19 +6603,19 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="99" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B129" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C129" s="48" t="s">
+        <v>346</v>
+      </c>
+      <c r="D129" s="110" t="s">
         <v>350</v>
       </c>
-      <c r="D129" s="110" t="s">
-        <v>354</v>
-      </c>
       <c r="E129" s="111" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F129" s="49"/>
       <c r="G129" s="50" t="s">
@@ -6637,19 +6634,19 @@
     </row>
     <row r="130" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A130" s="99" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B130" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D130" s="110" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E130" s="111" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F130" s="49"/>
       <c r="G130" s="50" t="s">
@@ -6668,19 +6665,19 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="99" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B131" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C131" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="D131" s="110" t="s">
+        <v>355</v>
+      </c>
+      <c r="E131" s="111" t="s">
         <v>356</v>
-      </c>
-      <c r="D131" s="110" t="s">
-        <v>359</v>
-      </c>
-      <c r="E131" s="111" t="s">
-        <v>360</v>
       </c>
       <c r="F131" s="49"/>
       <c r="G131" s="54" t="s">
@@ -6699,19 +6696,19 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="99" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B132" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D132" s="110" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E132" s="111" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F132" s="49"/>
       <c r="G132" s="50" t="s">
@@ -6730,19 +6727,19 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="99" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B133" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C133" s="48" t="s">
+        <v>357</v>
+      </c>
+      <c r="D133" s="110" t="s">
+        <v>360</v>
+      </c>
+      <c r="E133" s="111" t="s">
         <v>361</v>
-      </c>
-      <c r="D133" s="110" t="s">
-        <v>364</v>
-      </c>
-      <c r="E133" s="111" t="s">
-        <v>365</v>
       </c>
       <c r="F133" s="49"/>
       <c r="G133" s="50" t="s">
@@ -6752,7 +6749,7 @@
       <c r="I133" s="51"/>
       <c r="J133" s="52"/>
       <c r="K133" s="53" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L133" s="52" t="s">
         <v>19</v>
@@ -6761,19 +6758,19 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="99" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B134" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D134" s="110" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E134" s="111" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F134" s="49"/>
       <c r="G134" s="50" t="s">
@@ -6792,28 +6789,28 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="99" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B135" s="100" t="s">
+        <v>364</v>
+      </c>
+      <c r="C135" s="48" t="s">
+        <v>365</v>
+      </c>
+      <c r="D135" s="110" t="s">
+        <v>366</v>
+      </c>
+      <c r="E135" s="111" t="s">
+        <v>367</v>
+      </c>
+      <c r="F135" s="49" t="s">
         <v>368</v>
-      </c>
-      <c r="C135" s="48" t="s">
-        <v>369</v>
-      </c>
-      <c r="D135" s="110" t="s">
-        <v>370</v>
-      </c>
-      <c r="E135" s="111" t="s">
-        <v>371</v>
-      </c>
-      <c r="F135" s="49" t="s">
-        <v>372</v>
       </c>
       <c r="G135" s="50" t="s">
         <v>32</v>
       </c>
       <c r="H135" s="51" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="I135" s="51"/>
       <c r="J135" s="52"/>
@@ -6827,25 +6824,25 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="99" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B136" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C136" s="48" t="s">
+        <v>365</v>
+      </c>
+      <c r="D136" s="110" t="s">
         <v>369</v>
       </c>
-      <c r="D136" s="110" t="s">
-        <v>373</v>
-      </c>
       <c r="E136" s="111" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F136" s="49" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G136" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H136" s="51"/>
       <c r="I136" s="51"/>
@@ -6860,25 +6857,25 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="99" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B137" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D137" s="110" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E137" s="111" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F137" s="49" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G137" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H137" s="51"/>
       <c r="I137" s="51"/>
@@ -6893,25 +6890,25 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="99" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B138" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D138" s="110" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E138" s="111" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F138" s="49" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G138" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H138" s="51"/>
       <c r="I138" s="51"/>
@@ -6926,19 +6923,19 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="99" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B139" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D139" s="110" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E139" s="111" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F139" s="49"/>
       <c r="G139" s="50" t="s">
@@ -6957,22 +6954,22 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="99" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B140" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D140" s="110" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E140" s="111" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F140" s="49" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G140" s="50" t="s">
         <v>27</v>
@@ -6981,7 +6978,7 @@
       <c r="I140" s="51"/>
       <c r="J140" s="52"/>
       <c r="K140" s="53" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="L140" s="52" t="s">
         <v>19</v>
@@ -6990,19 +6987,19 @@
     </row>
     <row r="141" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A141" s="99" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B141" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D141" s="110" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E141" s="111" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F141" s="49"/>
       <c r="G141" s="50" t="s">
@@ -7021,22 +7018,22 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="99" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B142" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C142" s="48" t="s">
+        <v>383</v>
+      </c>
+      <c r="D142" s="110" t="s">
+        <v>386</v>
+      </c>
+      <c r="E142" s="111" t="s">
         <v>387</v>
       </c>
-      <c r="D142" s="110" t="s">
-        <v>390</v>
-      </c>
-      <c r="E142" s="111" t="s">
-        <v>391</v>
-      </c>
       <c r="F142" s="49" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G142" s="50" t="s">
         <v>27</v>
@@ -7045,7 +7042,7 @@
       <c r="I142" s="51"/>
       <c r="J142" s="52"/>
       <c r="K142" s="53" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="L142" s="52" t="s">
         <v>19</v>
@@ -7054,19 +7051,19 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="99" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B143" s="100" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C143" s="48" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D143" s="110" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E143" s="111" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F143" s="49"/>
       <c r="G143" s="50" t="s">
@@ -7085,19 +7082,19 @@
     </row>
     <row r="144" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A144" s="109" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B144" s="108" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C144" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="D144" s="110" t="s">
+        <v>392</v>
+      </c>
+      <c r="E144" s="111" t="s">
         <v>393</v>
-      </c>
-      <c r="D144" s="110" t="s">
-        <v>396</v>
-      </c>
-      <c r="E144" s="111" t="s">
-        <v>397</v>
       </c>
       <c r="F144" s="49"/>
       <c r="G144" s="50" t="s">

</xml_diff>

<commit_message>
main merge + adjustment "rechtsstreitigkeiten"
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7149841D-3517-4E66-88E4-CDC54C990FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD2F9AA-9712-4D4A-9D5E-54C85D8D19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -790,9 +790,6 @@
     <t>16</t>
   </si>
   <si>
-    <t>ESG-bezogene Rechtsstreitigkeiten Involvierung</t>
-  </si>
-  <si>
     <t>Einzelheiten zu ESG-bezogenen Rechtsstreitigkeiten</t>
   </si>
   <si>
@@ -1592,6 +1589,9 @@
   </si>
   <si>
     <t>ESG-Rating und Zertifizierung</t>
+  </si>
+  <si>
+    <t>Rechtsstreitigkeiten mit ESG-Bezug</t>
   </si>
 </sst>
 </file>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2985,7 +2985,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>121</v>
@@ -3016,7 +3016,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>124</v>
@@ -3049,7 +3049,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>133</v>
@@ -3082,7 +3082,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>134</v>
@@ -3115,7 +3115,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>135</v>
@@ -3148,7 +3148,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>136</v>
@@ -3181,7 +3181,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>138</v>
@@ -3214,7 +3214,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>143</v>
@@ -3245,7 +3245,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>147</v>
@@ -3276,7 +3276,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>152</v>
@@ -3307,10 +3307,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E25" s="47" t="s">
         <v>155</v>
@@ -3338,7 +3338,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>178</v>
@@ -3369,7 +3369,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>179</v>
@@ -3400,7 +3400,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>180</v>
@@ -3431,7 +3431,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>181</v>
@@ -3462,7 +3462,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>182</v>
@@ -3493,7 +3493,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>183</v>
@@ -3524,7 +3524,7 @@
         <v>25</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>184</v>
@@ -3555,7 +3555,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>185</v>
@@ -3586,7 +3586,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>186</v>
@@ -3617,7 +3617,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>187</v>
@@ -3648,7 +3648,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>188</v>
@@ -3679,7 +3679,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>194</v>
@@ -3710,7 +3710,7 @@
         <v>25</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>196</v>
@@ -3741,7 +3741,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>198</v>
@@ -3772,7 +3772,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>199</v>
@@ -3803,7 +3803,7 @@
         <v>25</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>65</v>
@@ -3834,7 +3834,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>205</v>
@@ -3865,7 +3865,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>206</v>
@@ -3896,7 +3896,7 @@
         <v>25</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>70</v>
@@ -3929,7 +3929,7 @@
         <v>25</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>35</v>
@@ -3964,7 +3964,7 @@
         <v>25</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>38</v>
@@ -3999,7 +3999,7 @@
         <v>25</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>39</v>
@@ -4034,7 +4034,7 @@
         <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>40</v>
@@ -4069,7 +4069,7 @@
         <v>25</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>212</v>
@@ -4104,7 +4104,7 @@
         <v>25</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>214</v>
@@ -4139,7 +4139,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D51" s="21" t="s">
         <v>216</v>
@@ -4466,10 +4466,10 @@
         <v>63</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>245</v>
+        <v>512</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="15" t="s">
@@ -4497,10 +4497,10 @@
         <v>63</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E62" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="29" t="s">
@@ -4525,10 +4525,10 @@
         <v>25</v>
       </c>
       <c r="C63" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D63" s="40" t="s">
         <v>249</v>
-      </c>
-      <c r="D63" s="40" t="s">
-        <v>250</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>73</v>
@@ -4550,19 +4550,19 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D64" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="E64" s="38" t="s">
         <v>252</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>253</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="29" t="s">
@@ -4587,10 +4587,10 @@
         <v>25</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>75</v>
@@ -4612,19 +4612,19 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D66" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="E66" s="38" t="s">
         <v>256</v>
-      </c>
-      <c r="E66" s="38" t="s">
-        <v>257</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="29" t="s">
@@ -4643,19 +4643,19 @@
     </row>
     <row r="67" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A67" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="21" t="s">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="H67" s="11"/>
       <c r="I67" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="17" t="s">
@@ -4676,19 +4676,19 @@
     </row>
     <row r="68" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A68" s="34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F68" s="41"/>
       <c r="G68" s="21" t="s">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="H68" s="11"/>
       <c r="I68" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="17" t="s">
@@ -4709,19 +4709,19 @@
     </row>
     <row r="69" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A69" s="34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D69" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E69" s="31" t="s">
         <v>267</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>268</v>
       </c>
       <c r="F69" s="41"/>
       <c r="G69" s="21" t="s">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="17" t="s">
@@ -4742,19 +4742,19 @@
     </row>
     <row r="70" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A70" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D70" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E70" s="31" t="s">
         <v>263</v>
-      </c>
-      <c r="E70" s="31" t="s">
-        <v>264</v>
       </c>
       <c r="F70" s="41"/>
       <c r="G70" s="21" t="s">
@@ -4762,7 +4762,7 @@
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="17" t="s">
@@ -4781,13 +4781,13 @@
         <v>78</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E71" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F71" s="41"/>
       <c r="G71" s="29" t="s">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="17" t="s">
@@ -4814,13 +4814,13 @@
         <v>78</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E72" s="38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F72" s="41"/>
       <c r="G72" s="29" t="s">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="H72" s="11"/>
       <c r="I72" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="17" t="s">
@@ -4841,19 +4841,19 @@
     </row>
     <row r="73" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A73" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C73" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D73" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="E73" s="38" t="s">
         <v>277</v>
-      </c>
-      <c r="E73" s="38" t="s">
-        <v>278</v>
       </c>
       <c r="F73" s="41"/>
       <c r="G73" s="29" t="s">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="H73" s="11"/>
       <c r="I73" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="17" t="s">
@@ -4874,19 +4874,19 @@
     </row>
     <row r="74" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A74" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D74" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="E74" s="38" t="s">
         <v>280</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>281</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="29" t="s">
@@ -4894,7 +4894,7 @@
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="17" t="s">
@@ -4913,13 +4913,13 @@
         <v>78</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>83</v>
       </c>
       <c r="E75" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F75" s="41"/>
       <c r="G75" s="29" t="s">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="H75" s="11"/>
       <c r="I75" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="17" t="s">
@@ -4940,19 +4940,19 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D76" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E76" s="42" t="s">
         <v>287</v>
-      </c>
-      <c r="E76" s="42" t="s">
-        <v>288</v>
       </c>
       <c r="F76" s="41"/>
       <c r="G76" s="29" t="s">
@@ -4977,13 +4977,13 @@
         <v>78</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D77" s="21" t="s">
         <v>87</v>
       </c>
       <c r="E77" s="38" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F77" s="41"/>
       <c r="G77" s="29" t="s">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="H77" s="11"/>
       <c r="I77" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="17" t="s">
@@ -5010,13 +5010,13 @@
         <v>78</v>
       </c>
       <c r="C78" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="D78" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="D78" s="21" t="s">
+      <c r="E78" s="38" t="s">
         <v>292</v>
-      </c>
-      <c r="E78" s="38" t="s">
-        <v>293</v>
       </c>
       <c r="F78" s="41"/>
       <c r="G78" s="29" t="s">
@@ -5024,7 +5024,7 @@
       </c>
       <c r="H78" s="11"/>
       <c r="I78" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="17" t="s">
@@ -5037,19 +5037,19 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E79" s="38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="29" t="s">
@@ -5074,13 +5074,13 @@
         <v>78</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D80" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="E80" s="38" t="s">
         <v>297</v>
-      </c>
-      <c r="E80" s="38" t="s">
-        <v>298</v>
       </c>
       <c r="F80" s="41"/>
       <c r="G80" s="29" t="s">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="H80" s="11"/>
       <c r="I80" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="17" t="s">
@@ -5107,13 +5107,13 @@
         <v>78</v>
       </c>
       <c r="C81" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D81" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="E81" s="38" t="s">
         <v>299</v>
-      </c>
-      <c r="E81" s="38" t="s">
-        <v>300</v>
       </c>
       <c r="F81" s="41"/>
       <c r="G81" s="29" t="s">
@@ -5132,26 +5132,26 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C82" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D82" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="E82" s="38" t="s">
         <v>301</v>
-      </c>
-      <c r="E82" s="38" t="s">
-        <v>302</v>
       </c>
       <c r="F82" s="41"/>
       <c r="G82" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I82" s="11"/>
       <c r="J82" s="12"/>
@@ -5165,19 +5165,19 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C83" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D83" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="E83" s="38" t="s">
         <v>306</v>
-      </c>
-      <c r="E83" s="38" t="s">
-        <v>307</v>
       </c>
       <c r="F83" s="41"/>
       <c r="G83" s="29" t="s">
@@ -5202,13 +5202,13 @@
         <v>78</v>
       </c>
       <c r="C84" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D84" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="E84" s="38" t="s">
         <v>308</v>
-      </c>
-      <c r="E84" s="38" t="s">
-        <v>309</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="29" t="s">
@@ -5227,19 +5227,19 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C85" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D85" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="E85" s="38" t="s">
         <v>311</v>
-      </c>
-      <c r="E85" s="38" t="s">
-        <v>312</v>
       </c>
       <c r="F85" s="41"/>
       <c r="G85" s="29" t="s">
@@ -5258,19 +5258,19 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C86" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D86" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="E86" s="38" t="s">
         <v>314</v>
-      </c>
-      <c r="E86" s="38" t="s">
-        <v>315</v>
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="29" t="s">
@@ -5289,19 +5289,19 @@
     </row>
     <row r="87" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A87" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C87" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D87" s="55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E87" s="56" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F87" s="41"/>
       <c r="G87" s="29" t="s">
@@ -5311,7 +5311,7 @@
       <c r="I87" s="11"/>
       <c r="J87" s="12"/>
       <c r="K87" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L87" s="12" t="s">
         <v>19</v>
@@ -5320,19 +5320,19 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="34" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C88" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="29" t="s">
@@ -5351,19 +5351,19 @@
     </row>
     <row r="89" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A89" s="34" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C89" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E89" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F89" s="41"/>
       <c r="G89" s="29" t="s">
@@ -5373,7 +5373,7 @@
       <c r="I89" s="11"/>
       <c r="J89" s="12"/>
       <c r="K89" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L89" s="12" t="s">
         <v>19</v>
@@ -5382,19 +5382,19 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C90" s="105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D90" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="E90" s="38" t="s">
         <v>422</v>
-      </c>
-      <c r="E90" s="38" t="s">
-        <v>423</v>
       </c>
       <c r="F90" s="41"/>
       <c r="G90" s="29" t="s">
@@ -5415,19 +5415,19 @@
     </row>
     <row r="91" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A91" s="63" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B91" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C91" s="61" t="s">
+        <v>408</v>
+      </c>
+      <c r="D91" s="40" t="s">
         <v>409</v>
       </c>
-      <c r="D91" s="40" t="s">
+      <c r="E91" s="39" t="s">
         <v>410</v>
-      </c>
-      <c r="E91" s="39" t="s">
-        <v>411</v>
       </c>
       <c r="F91" s="57"/>
       <c r="G91" s="60" t="s">
@@ -5446,19 +5446,19 @@
     </row>
     <row r="92" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A92" s="63" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B92" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C92" s="61" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D92" s="40" t="s">
+        <v>411</v>
+      </c>
+      <c r="E92" s="39" t="s">
         <v>412</v>
-      </c>
-      <c r="E92" s="39" t="s">
-        <v>413</v>
       </c>
       <c r="F92" s="57"/>
       <c r="G92" s="60" t="s">
@@ -5477,23 +5477,23 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="73" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B93" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C93" s="70" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D93" s="40" t="s">
+        <v>425</v>
+      </c>
+      <c r="E93" s="39" t="s">
         <v>426</v>
-      </c>
-      <c r="E93" s="39" t="s">
-        <v>427</v>
       </c>
       <c r="F93" s="66"/>
       <c r="G93" s="69" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H93" s="67"/>
       <c r="I93" s="67"/>
@@ -5508,19 +5508,19 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="72" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B94" s="65" t="s">
         <v>78</v>
       </c>
       <c r="C94" s="70" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D94" s="40" t="s">
+        <v>428</v>
+      </c>
+      <c r="E94" s="39" t="s">
         <v>429</v>
-      </c>
-      <c r="E94" s="39" t="s">
-        <v>430</v>
       </c>
       <c r="F94" s="66"/>
       <c r="G94" s="69" t="s">
@@ -5530,7 +5530,7 @@
       <c r="I94" s="67"/>
       <c r="J94" s="68"/>
       <c r="K94" s="71" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L94" s="68" t="s">
         <v>19</v>
@@ -5539,19 +5539,19 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="63" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B95" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C95" s="78" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D95" s="40" t="s">
+        <v>432</v>
+      </c>
+      <c r="E95" s="39" t="s">
         <v>433</v>
-      </c>
-      <c r="E95" s="39" t="s">
-        <v>434</v>
       </c>
       <c r="F95" s="74"/>
       <c r="G95" s="77" t="s">
@@ -5570,19 +5570,19 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="63" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B96" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C96" s="78" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D96" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="E96" s="39" t="s">
         <v>435</v>
-      </c>
-      <c r="E96" s="39" t="s">
-        <v>436</v>
       </c>
       <c r="F96" s="74"/>
       <c r="G96" s="77" t="s">
@@ -5601,19 +5601,19 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="63" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B97" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C97" s="78" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D97" s="40" t="s">
+        <v>436</v>
+      </c>
+      <c r="E97" s="39" t="s">
         <v>437</v>
-      </c>
-      <c r="E97" s="39" t="s">
-        <v>438</v>
       </c>
       <c r="F97" s="74"/>
       <c r="G97" s="77" t="s">
@@ -5632,19 +5632,19 @@
     </row>
     <row r="98" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A98" s="63" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B98" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C98" s="78" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D98" s="40" t="s">
+        <v>438</v>
+      </c>
+      <c r="E98" s="39" t="s">
         <v>439</v>
-      </c>
-      <c r="E98" s="39" t="s">
-        <v>440</v>
       </c>
       <c r="F98" s="74"/>
       <c r="G98" s="77" t="s">
@@ -5663,19 +5663,19 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="73" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B99" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D99" s="40" t="s">
+        <v>444</v>
+      </c>
+      <c r="E99" s="39" t="s">
         <v>445</v>
-      </c>
-      <c r="E99" s="39" t="s">
-        <v>446</v>
       </c>
       <c r="F99" s="80"/>
       <c r="G99" s="83" t="s">
@@ -5694,19 +5694,19 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="73" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B100" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E100" s="39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F100" s="80"/>
       <c r="G100" s="83" t="s">
@@ -5716,7 +5716,7 @@
       <c r="I100" s="81"/>
       <c r="J100" s="82"/>
       <c r="K100" s="85" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L100" s="82" t="s">
         <v>19</v>
@@ -5725,19 +5725,19 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="63" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B101" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C101" s="90" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D101" s="40" t="s">
+        <v>450</v>
+      </c>
+      <c r="E101" s="39" t="s">
         <v>451</v>
-      </c>
-      <c r="E101" s="39" t="s">
-        <v>452</v>
       </c>
       <c r="F101" s="86"/>
       <c r="G101" s="89" t="s">
@@ -5756,19 +5756,19 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="63" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B102" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C102" s="90" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D102" s="40" t="s">
+        <v>452</v>
+      </c>
+      <c r="E102" s="39" t="s">
         <v>453</v>
-      </c>
-      <c r="E102" s="39" t="s">
-        <v>454</v>
       </c>
       <c r="F102" s="86"/>
       <c r="G102" s="89" t="s">
@@ -5787,19 +5787,19 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="63" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B103" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C103" s="90" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D103" s="40" t="s">
+        <v>454</v>
+      </c>
+      <c r="E103" s="39" t="s">
         <v>455</v>
-      </c>
-      <c r="E103" s="39" t="s">
-        <v>456</v>
       </c>
       <c r="F103" s="86"/>
       <c r="G103" s="89" t="s">
@@ -5818,19 +5818,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="63" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B104" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C104" s="90" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E104" s="39" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F104" s="86"/>
       <c r="G104" s="89" t="s">
@@ -5849,23 +5849,23 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="73" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B105" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C105" s="97" t="s">
+        <v>462</v>
+      </c>
+      <c r="D105" s="40" t="s">
         <v>463</v>
       </c>
-      <c r="D105" s="40" t="s">
+      <c r="E105" s="39" t="s">
         <v>464</v>
-      </c>
-      <c r="E105" s="39" t="s">
-        <v>465</v>
       </c>
       <c r="F105" s="93"/>
       <c r="G105" s="96" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H105" s="94"/>
       <c r="I105" s="94"/>
@@ -5880,19 +5880,19 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="73" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B106" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C106" s="97" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D106" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="E106" s="39" t="s">
         <v>466</v>
-      </c>
-      <c r="E106" s="39" t="s">
-        <v>467</v>
       </c>
       <c r="F106" s="93"/>
       <c r="G106" s="96" t="s">
@@ -5902,7 +5902,7 @@
       <c r="I106" s="94"/>
       <c r="J106" s="95"/>
       <c r="K106" s="98" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L106" s="95" t="s">
         <v>19</v>
@@ -5911,19 +5911,19 @@
     </row>
     <row r="107" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A107" s="73" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B107" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C107" s="97" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E107" s="39" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F107" s="93"/>
       <c r="G107" s="96" t="s">
@@ -5942,23 +5942,23 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" s="73" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B108" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C108" s="97" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D108" s="40" t="s">
+        <v>468</v>
+      </c>
+      <c r="E108" s="39" t="s">
         <v>469</v>
-      </c>
-      <c r="E108" s="39" t="s">
-        <v>470</v>
       </c>
       <c r="F108" s="93"/>
       <c r="G108" s="96" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H108" s="94"/>
       <c r="I108" s="94"/>
@@ -5973,19 +5973,19 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B109" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C109" s="97" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D109" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="E109" s="39" t="s">
         <v>471</v>
-      </c>
-      <c r="E109" s="39" t="s">
-        <v>472</v>
       </c>
       <c r="F109" s="93"/>
       <c r="G109" s="96" t="s">
@@ -5995,7 +5995,7 @@
       <c r="I109" s="94"/>
       <c r="J109" s="95"/>
       <c r="K109" s="98" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L109" s="95" t="s">
         <v>19</v>
@@ -6004,23 +6004,23 @@
     </row>
     <row r="110" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="63" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B110" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C110" s="105" t="s">
+        <v>478</v>
+      </c>
+      <c r="D110" s="40" t="s">
         <v>479</v>
       </c>
-      <c r="D110" s="40" t="s">
+      <c r="E110" s="39" t="s">
         <v>480</v>
-      </c>
-      <c r="E110" s="39" t="s">
-        <v>481</v>
       </c>
       <c r="F110" s="101"/>
       <c r="G110" s="104" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H110" s="102"/>
       <c r="I110" s="102"/>
@@ -6035,19 +6035,19 @@
     </row>
     <row r="111" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="63" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B111" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C111" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D111" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="E111" s="39" t="s">
         <v>482</v>
-      </c>
-      <c r="E111" s="39" t="s">
-        <v>483</v>
       </c>
       <c r="F111" s="101"/>
       <c r="G111" s="104" t="s">
@@ -6057,7 +6057,7 @@
       <c r="I111" s="102"/>
       <c r="J111" s="103"/>
       <c r="K111" s="106" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L111" s="103" t="s">
         <v>19</v>
@@ -6066,23 +6066,23 @@
     </row>
     <row r="112" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="63" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B112" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C112" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D112" s="40" t="s">
+        <v>483</v>
+      </c>
+      <c r="E112" s="39" t="s">
         <v>484</v>
-      </c>
-      <c r="E112" s="39" t="s">
-        <v>485</v>
       </c>
       <c r="F112" s="101"/>
       <c r="G112" s="104" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H112" s="102"/>
       <c r="I112" s="102"/>
@@ -6097,19 +6097,19 @@
     </row>
     <row r="113" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="63" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B113" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C113" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E113" s="39" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F113" s="101"/>
       <c r="G113" s="104" t="s">
@@ -6119,7 +6119,7 @@
       <c r="I113" s="102"/>
       <c r="J113" s="103"/>
       <c r="K113" s="106" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L113" s="103" t="s">
         <v>19</v>
@@ -6128,19 +6128,19 @@
     </row>
     <row r="114" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="63" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B114" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C114" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D114" s="40" t="s">
+        <v>486</v>
+      </c>
+      <c r="E114" s="39" t="s">
         <v>487</v>
-      </c>
-      <c r="E114" s="39" t="s">
-        <v>488</v>
       </c>
       <c r="F114" s="101"/>
       <c r="G114" s="104" t="s">
@@ -6150,7 +6150,7 @@
       <c r="I114" s="102"/>
       <c r="J114" s="103"/>
       <c r="K114" s="106" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L114" s="103" t="s">
         <v>19</v>
@@ -6159,23 +6159,23 @@
     </row>
     <row r="115" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="63" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B115" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C115" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D115" s="40" t="s">
+        <v>488</v>
+      </c>
+      <c r="E115" s="39" t="s">
         <v>489</v>
-      </c>
-      <c r="E115" s="39" t="s">
-        <v>490</v>
       </c>
       <c r="F115" s="101"/>
       <c r="G115" s="104" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H115" s="102"/>
       <c r="I115" s="102"/>
@@ -6190,19 +6190,19 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="63" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B116" s="64" t="s">
         <v>78</v>
       </c>
       <c r="C116" s="105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D116" s="40" t="s">
+        <v>490</v>
+      </c>
+      <c r="E116" s="39" t="s">
         <v>491</v>
-      </c>
-      <c r="E116" s="39" t="s">
-        <v>492</v>
       </c>
       <c r="F116" s="101"/>
       <c r="G116" s="104" t="s">
@@ -6212,7 +6212,7 @@
       <c r="I116" s="102"/>
       <c r="J116" s="103"/>
       <c r="K116" s="106" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L116" s="103" t="s">
         <v>19</v>
@@ -6227,16 +6227,16 @@
         <v>89</v>
       </c>
       <c r="C117" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="D117" s="110" t="s">
         <v>319</v>
       </c>
-      <c r="D117" s="110" t="s">
+      <c r="E117" s="111" t="s">
         <v>320</v>
       </c>
-      <c r="E117" s="111" t="s">
+      <c r="F117" s="49" t="s">
         <v>321</v>
-      </c>
-      <c r="F117" s="49" t="s">
-        <v>322</v>
       </c>
       <c r="G117" s="50" t="s">
         <v>90</v>
@@ -6260,16 +6260,16 @@
         <v>89</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D118" s="110" t="s">
+        <v>322</v>
+      </c>
+      <c r="E118" s="111" t="s">
         <v>323</v>
       </c>
-      <c r="E118" s="111" t="s">
+      <c r="F118" s="49" t="s">
         <v>324</v>
-      </c>
-      <c r="F118" s="49" t="s">
-        <v>325</v>
       </c>
       <c r="G118" s="54" t="s">
         <v>149</v>
@@ -6287,22 +6287,22 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="99" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B119" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D119" s="110" t="s">
+        <v>325</v>
+      </c>
+      <c r="E119" s="111" t="s">
         <v>326</v>
       </c>
-      <c r="E119" s="111" t="s">
+      <c r="F119" s="49" t="s">
         <v>327</v>
-      </c>
-      <c r="F119" s="49" t="s">
-        <v>328</v>
       </c>
       <c r="G119" s="54" t="s">
         <v>149</v>
@@ -6320,22 +6320,22 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B120" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D120" s="110" t="s">
+        <v>328</v>
+      </c>
+      <c r="E120" s="111" t="s">
         <v>329</v>
       </c>
-      <c r="E120" s="111" t="s">
+      <c r="F120" s="49" t="s">
         <v>330</v>
-      </c>
-      <c r="F120" s="49" t="s">
-        <v>331</v>
       </c>
       <c r="G120" s="54" t="s">
         <v>149</v>
@@ -6359,13 +6359,13 @@
         <v>89</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D121" s="110" t="s">
+        <v>331</v>
+      </c>
+      <c r="E121" s="111" t="s">
         <v>332</v>
-      </c>
-      <c r="E121" s="111" t="s">
-        <v>333</v>
       </c>
       <c r="F121" s="49"/>
       <c r="G121" s="54" t="s">
@@ -6390,13 +6390,13 @@
         <v>89</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D122" s="110" t="s">
+        <v>333</v>
+      </c>
+      <c r="E122" s="111" t="s">
         <v>334</v>
-      </c>
-      <c r="E122" s="111" t="s">
-        <v>335</v>
       </c>
       <c r="F122" s="49"/>
       <c r="G122" s="54" t="s">
@@ -6415,19 +6415,19 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="99" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B123" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D123" s="110" t="s">
+        <v>335</v>
+      </c>
+      <c r="E123" s="111" t="s">
         <v>336</v>
-      </c>
-      <c r="E123" s="111" t="s">
-        <v>337</v>
       </c>
       <c r="F123" s="49"/>
       <c r="G123" s="54" t="s">
@@ -6446,19 +6446,19 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="99" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B124" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D124" s="110" t="s">
+        <v>337</v>
+      </c>
+      <c r="E124" s="111" t="s">
         <v>338</v>
-      </c>
-      <c r="E124" s="111" t="s">
-        <v>339</v>
       </c>
       <c r="F124" s="49"/>
       <c r="G124" s="54" t="s">
@@ -6477,19 +6477,19 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="99" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B125" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D125" s="110" t="s">
+        <v>339</v>
+      </c>
+      <c r="E125" s="111" t="s">
         <v>340</v>
-      </c>
-      <c r="E125" s="111" t="s">
-        <v>341</v>
       </c>
       <c r="F125" s="49"/>
       <c r="G125" s="54" t="s">
@@ -6508,19 +6508,19 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="99" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B126" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D126" s="110" t="s">
+        <v>341</v>
+      </c>
+      <c r="E126" s="111" t="s">
         <v>342</v>
-      </c>
-      <c r="E126" s="111" t="s">
-        <v>343</v>
       </c>
       <c r="F126" s="49"/>
       <c r="G126" s="54" t="s">
@@ -6539,19 +6539,19 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="99" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B127" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D127" s="110" t="s">
+        <v>343</v>
+      </c>
+      <c r="E127" s="111" t="s">
         <v>344</v>
-      </c>
-      <c r="E127" s="111" t="s">
-        <v>345</v>
       </c>
       <c r="F127" s="49"/>
       <c r="G127" s="54" t="s">
@@ -6570,26 +6570,26 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="99" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B128" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C128" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="D128" s="110" t="s">
         <v>346</v>
       </c>
-      <c r="D128" s="110" t="s">
+      <c r="E128" s="111" t="s">
         <v>347</v>
-      </c>
-      <c r="E128" s="111" t="s">
-        <v>348</v>
       </c>
       <c r="F128" s="49"/>
       <c r="G128" s="54" t="s">
         <v>30</v>
       </c>
       <c r="H128" s="51" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I128" s="51"/>
       <c r="J128" s="52"/>
@@ -6603,19 +6603,19 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="99" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B129" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D129" s="110" t="s">
+        <v>349</v>
+      </c>
+      <c r="E129" s="111" t="s">
         <v>350</v>
-      </c>
-      <c r="E129" s="111" t="s">
-        <v>351</v>
       </c>
       <c r="F129" s="49"/>
       <c r="G129" s="50" t="s">
@@ -6634,19 +6634,19 @@
     </row>
     <row r="130" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A130" s="99" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B130" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C130" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="D130" s="110" t="s">
         <v>352</v>
       </c>
-      <c r="D130" s="110" t="s">
+      <c r="E130" s="111" t="s">
         <v>353</v>
-      </c>
-      <c r="E130" s="111" t="s">
-        <v>354</v>
       </c>
       <c r="F130" s="49"/>
       <c r="G130" s="50" t="s">
@@ -6665,19 +6665,19 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="99" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B131" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D131" s="110" t="s">
+        <v>354</v>
+      </c>
+      <c r="E131" s="111" t="s">
         <v>355</v>
-      </c>
-      <c r="E131" s="111" t="s">
-        <v>356</v>
       </c>
       <c r="F131" s="49"/>
       <c r="G131" s="54" t="s">
@@ -6696,19 +6696,19 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="99" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B132" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C132" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="D132" s="110" t="s">
         <v>357</v>
       </c>
-      <c r="D132" s="110" t="s">
+      <c r="E132" s="111" t="s">
         <v>358</v>
-      </c>
-      <c r="E132" s="111" t="s">
-        <v>359</v>
       </c>
       <c r="F132" s="49"/>
       <c r="G132" s="50" t="s">
@@ -6727,19 +6727,19 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="99" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B133" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D133" s="110" t="s">
+        <v>359</v>
+      </c>
+      <c r="E133" s="111" t="s">
         <v>360</v>
-      </c>
-      <c r="E133" s="111" t="s">
-        <v>361</v>
       </c>
       <c r="F133" s="49"/>
       <c r="G133" s="50" t="s">
@@ -6749,7 +6749,7 @@
       <c r="I133" s="51"/>
       <c r="J133" s="52"/>
       <c r="K133" s="53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L133" s="52" t="s">
         <v>19</v>
@@ -6758,19 +6758,19 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="99" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B134" s="100" t="s">
         <v>89</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D134" s="110" t="s">
+        <v>361</v>
+      </c>
+      <c r="E134" s="111" t="s">
         <v>362</v>
-      </c>
-      <c r="E134" s="111" t="s">
-        <v>363</v>
       </c>
       <c r="F134" s="49"/>
       <c r="G134" s="50" t="s">
@@ -6789,28 +6789,28 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="99" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B135" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C135" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C135" s="48" t="s">
+      <c r="D135" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="D135" s="110" t="s">
+      <c r="E135" s="111" t="s">
         <v>366</v>
       </c>
-      <c r="E135" s="111" t="s">
+      <c r="F135" s="49" t="s">
         <v>367</v>
-      </c>
-      <c r="F135" s="49" t="s">
-        <v>368</v>
       </c>
       <c r="G135" s="50" t="s">
         <v>32</v>
       </c>
       <c r="H135" s="51" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I135" s="51"/>
       <c r="J135" s="52"/>
@@ -6824,22 +6824,22 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="99" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B136" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C136" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C136" s="48" t="s">
-        <v>365</v>
-      </c>
       <c r="D136" s="110" t="s">
+        <v>368</v>
+      </c>
+      <c r="E136" s="111" t="s">
         <v>369</v>
       </c>
-      <c r="E136" s="111" t="s">
+      <c r="F136" s="49" t="s">
         <v>370</v>
-      </c>
-      <c r="F136" s="49" t="s">
-        <v>371</v>
       </c>
       <c r="G136" s="54" t="s">
         <v>149</v>
@@ -6857,22 +6857,22 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="99" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B137" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C137" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C137" s="48" t="s">
-        <v>365</v>
-      </c>
       <c r="D137" s="110" t="s">
+        <v>371</v>
+      </c>
+      <c r="E137" s="111" t="s">
         <v>372</v>
       </c>
-      <c r="E137" s="111" t="s">
+      <c r="F137" s="49" t="s">
         <v>373</v>
-      </c>
-      <c r="F137" s="49" t="s">
-        <v>374</v>
       </c>
       <c r="G137" s="54" t="s">
         <v>149</v>
@@ -6890,22 +6890,22 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B138" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C138" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C138" s="48" t="s">
-        <v>365</v>
-      </c>
       <c r="D138" s="110" t="s">
+        <v>374</v>
+      </c>
+      <c r="E138" s="111" t="s">
         <v>375</v>
       </c>
-      <c r="E138" s="111" t="s">
+      <c r="F138" s="49" t="s">
         <v>376</v>
-      </c>
-      <c r="F138" s="49" t="s">
-        <v>377</v>
       </c>
       <c r="G138" s="54" t="s">
         <v>149</v>
@@ -6923,19 +6923,19 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="99" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B139" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C139" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C139" s="48" t="s">
-        <v>365</v>
-      </c>
       <c r="D139" s="110" t="s">
+        <v>377</v>
+      </c>
+      <c r="E139" s="111" t="s">
         <v>378</v>
-      </c>
-      <c r="E139" s="111" t="s">
-        <v>379</v>
       </c>
       <c r="F139" s="49"/>
       <c r="G139" s="50" t="s">
@@ -6954,22 +6954,22 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="99" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B140" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C140" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C140" s="48" t="s">
-        <v>365</v>
-      </c>
       <c r="D140" s="110" t="s">
+        <v>379</v>
+      </c>
+      <c r="E140" s="111" t="s">
         <v>380</v>
       </c>
-      <c r="E140" s="111" t="s">
+      <c r="F140" s="49" t="s">
         <v>381</v>
-      </c>
-      <c r="F140" s="49" t="s">
-        <v>382</v>
       </c>
       <c r="G140" s="50" t="s">
         <v>27</v>
@@ -6978,7 +6978,7 @@
       <c r="I140" s="51"/>
       <c r="J140" s="52"/>
       <c r="K140" s="53" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L140" s="52" t="s">
         <v>19</v>
@@ -6987,19 +6987,19 @@
     </row>
     <row r="141" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A141" s="99" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B141" s="100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C141" s="48" t="s">
+        <v>382</v>
+      </c>
+      <c r="D141" s="110" t="s">
         <v>383</v>
       </c>
-      <c r="D141" s="110" t="s">
+      <c r="E141" s="111" t="s">
         <v>384</v>
-      </c>
-      <c r="E141" s="111" t="s">
-        <v>385</v>
       </c>
       <c r="F141" s="49"/>
       <c r="G141" s="50" t="s">
@@ -7018,22 +7018,22 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="99" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B142" s="100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D142" s="110" t="s">
+        <v>385</v>
+      </c>
+      <c r="E142" s="111" t="s">
         <v>386</v>
       </c>
-      <c r="E142" s="111" t="s">
+      <c r="F142" s="49" t="s">
         <v>387</v>
-      </c>
-      <c r="F142" s="49" t="s">
-        <v>388</v>
       </c>
       <c r="G142" s="50" t="s">
         <v>27</v>
@@ -7042,7 +7042,7 @@
       <c r="I142" s="51"/>
       <c r="J142" s="52"/>
       <c r="K142" s="53" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L142" s="52" t="s">
         <v>19</v>
@@ -7051,19 +7051,19 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="99" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B143" s="100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C143" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="D143" s="110" t="s">
         <v>389</v>
       </c>
-      <c r="D143" s="110" t="s">
+      <c r="E143" s="111" t="s">
         <v>390</v>
-      </c>
-      <c r="E143" s="111" t="s">
-        <v>391</v>
       </c>
       <c r="F143" s="49"/>
       <c r="G143" s="50" t="s">
@@ -7082,19 +7082,19 @@
     </row>
     <row r="144" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A144" s="109" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B144" s="108" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C144" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D144" s="110" t="s">
+        <v>391</v>
+      </c>
+      <c r="E144" s="111" t="s">
         <v>392</v>
-      </c>
-      <c r="E144" s="111" t="s">
-        <v>393</v>
       </c>
       <c r="F144" s="49"/>
       <c r="G144" s="50" t="s">

</xml_diff>

<commit_message>
add 3 missing questions from questionnaire + add reasonable ranges to number fields
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD2F9AA-9712-4D4A-9D5E-54C85D8D19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B2402-0C23-4FE8-99BE-CE307779CB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="523">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1555,9 +1555,6 @@
     <t>50.2.1</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>50.1.1</t>
   </si>
   <si>
@@ -1579,9 +1576,6 @@
     <t>52.1</t>
   </si>
   <si>
-    <t>52.2</t>
-  </si>
-  <si>
     <t>Aktivität im Sektor "Fossile Brennstoffe"</t>
   </si>
   <si>
@@ -1592,6 +1586,45 @@
   </si>
   <si>
     <t>Rechtsstreitigkeiten mit ESG-Bezug</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53.1</t>
+  </si>
+  <si>
+    <t>53.2</t>
+  </si>
+  <si>
+    <t>51.2</t>
+  </si>
+  <si>
+    <t>51.3</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie die Gesamtanzahl der Mitglieder des Aufsichtsrats an. Hinweise: Methodik analog zu ESRS 2 Governance; Definition Aufsichtsgremien aus ESRS S1-9;
+In einigen Rechtsordnungen bestehen die Governance-Systeme aus zwei Ebenen, in denen Aufsicht und Management voneinander getrennt sind. Hier geht es nur um die Zusammensetzung des Aufsichtsrats.</t>
+  </si>
+  <si>
+    <t>Gesamtanzahl Aufsichtsrat-Mitglieder</t>
+  </si>
+  <si>
+    <t>Anzahl unabhängiger Aufsichtsrat-Mitglieder</t>
+  </si>
+  <si>
+    <t>Anzahl weiblicher oder diverser Aufsichtsrat-Mitglieder</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie die Anzahl der unabhängigen Mitglieder des Aufsichtsrats an. Hinweise: Methodik analog zu ESRS 2 Governance; Definition Aufsichtsgremien aus ESRS S1-9;
+In einigen Rechtsordnungen bestehen die Governance-Systeme aus zwei Ebenen, in denen Aufsicht und Management voneinander getrennt sind. Hier geht es nur um die Zusammensetzung des Aufsichtsrats.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie die Anzahl der  Mitglieder des Aufsichtsrats an, welche sich als weiblich oder divers identifizieren. Hinweise: Methodik analog zu ESRS 2 Governance; Definition Aufsichtsgremien aus ESRS S1-9;
+In einigen Rechtsordnungen bestehen die Governance-Systeme aus zwei Ebenen, in denen Aufsicht und Management voneinander getrennt sind. Hier geht es nur um die Zusammensetzung des Aufsichtsrats.</t>
+  </si>
+  <si>
+    <t>Allowed Range: [0, INF]</t>
   </si>
 </sst>
 </file>
@@ -2506,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M145"/>
+  <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="E131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2768,7 +2801,9 @@
       <c r="G8" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I8" s="11" t="s">
         <v>126</v>
       </c>
@@ -2801,7 +2836,9 @@
       <c r="G9" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I9" s="11" t="s">
         <v>126</v>
       </c>
@@ -2834,7 +2871,9 @@
       <c r="G10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I10" s="11" t="s">
         <v>126</v>
       </c>
@@ -2867,7 +2906,9 @@
       <c r="G11" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I11" s="11" t="s">
         <v>126</v>
       </c>
@@ -2900,7 +2941,9 @@
       <c r="G12" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I12" s="11" t="s">
         <v>189</v>
       </c>
@@ -2933,7 +2976,9 @@
       <c r="G13" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I13" s="11" t="s">
         <v>189</v>
       </c>
@@ -2985,7 +3030,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>121</v>
@@ -3016,7 +3061,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>124</v>
@@ -3028,7 +3073,9 @@
       <c r="G16" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I16" s="28" t="s">
         <v>126</v>
       </c>
@@ -3049,7 +3096,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>133</v>
@@ -3061,7 +3108,9 @@
       <c r="G17" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I17" s="28" t="s">
         <v>126</v>
       </c>
@@ -3082,7 +3131,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>134</v>
@@ -3094,7 +3143,9 @@
       <c r="G18" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I18" s="28" t="s">
         <v>126</v>
       </c>
@@ -3115,7 +3166,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>135</v>
@@ -3127,7 +3178,9 @@
       <c r="G19" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I19" s="28" t="s">
         <v>126</v>
       </c>
@@ -3148,7 +3201,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>136</v>
@@ -3160,7 +3213,9 @@
       <c r="G20" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="11"/>
+      <c r="H20" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I20" s="28" t="s">
         <v>126</v>
       </c>
@@ -3181,7 +3236,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>138</v>
@@ -3193,7 +3248,9 @@
       <c r="G21" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I21" s="28" t="s">
         <v>126</v>
       </c>
@@ -3214,7 +3271,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>143</v>
@@ -3245,7 +3302,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>147</v>
@@ -3276,7 +3333,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>152</v>
@@ -3307,10 +3364,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E25" s="47" t="s">
         <v>155</v>
@@ -3338,7 +3395,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>178</v>
@@ -3369,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>179</v>
@@ -3400,7 +3457,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>180</v>
@@ -3431,7 +3488,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>181</v>
@@ -3462,7 +3519,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>182</v>
@@ -3493,7 +3550,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>183</v>
@@ -3524,7 +3581,7 @@
         <v>25</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>184</v>
@@ -3555,7 +3612,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>185</v>
@@ -3586,7 +3643,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>186</v>
@@ -3617,7 +3674,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>187</v>
@@ -3648,7 +3705,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>188</v>
@@ -3679,7 +3736,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>194</v>
@@ -3710,7 +3767,7 @@
         <v>25</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>196</v>
@@ -3741,7 +3798,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>198</v>
@@ -3772,7 +3829,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>199</v>
@@ -3803,7 +3860,7 @@
         <v>25</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>65</v>
@@ -3834,7 +3891,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>205</v>
@@ -3865,7 +3922,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>206</v>
@@ -3896,7 +3953,7 @@
         <v>25</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>70</v>
@@ -3929,7 +3986,7 @@
         <v>25</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>35</v>
@@ -3964,7 +4021,7 @@
         <v>25</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>38</v>
@@ -3999,7 +4056,7 @@
         <v>25</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>39</v>
@@ -4034,7 +4091,7 @@
         <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>40</v>
@@ -4069,7 +4126,7 @@
         <v>25</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>212</v>
@@ -4104,7 +4161,7 @@
         <v>25</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>214</v>
@@ -4139,7 +4196,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D51" s="21" t="s">
         <v>216</v>
@@ -4466,7 +4523,7 @@
         <v>63</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E61" s="39" t="s">
         <v>246</v>
@@ -4661,7 +4718,9 @@
       <c r="G67" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H67" s="11"/>
+      <c r="H67" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I67" s="11" t="s">
         <v>258</v>
       </c>
@@ -4694,7 +4753,9 @@
       <c r="G68" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H68" s="11"/>
+      <c r="H68" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I68" s="11" t="s">
         <v>258</v>
       </c>
@@ -4727,7 +4788,9 @@
       <c r="G69" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H69" s="11"/>
+      <c r="H69" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I69" s="11" t="s">
         <v>258</v>
       </c>
@@ -4760,7 +4823,9 @@
       <c r="G70" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="11"/>
+      <c r="H70" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I70" s="11" t="s">
         <v>258</v>
       </c>
@@ -4793,7 +4858,9 @@
       <c r="G71" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H71" s="11"/>
+      <c r="H71" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I71" s="11" t="s">
         <v>271</v>
       </c>
@@ -4826,7 +4893,9 @@
       <c r="G72" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H72" s="11"/>
+      <c r="H72" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I72" s="11" t="s">
         <v>273</v>
       </c>
@@ -4859,7 +4928,9 @@
       <c r="G73" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H73" s="11"/>
+      <c r="H73" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I73" s="11" t="s">
         <v>273</v>
       </c>
@@ -4892,7 +4963,9 @@
       <c r="G74" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H74" s="11"/>
+      <c r="H74" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I74" s="11" t="s">
         <v>273</v>
       </c>
@@ -4925,7 +4998,9 @@
       <c r="G75" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H75" s="11"/>
+      <c r="H75" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I75" s="11" t="s">
         <v>285</v>
       </c>
@@ -4989,7 +5064,9 @@
       <c r="G77" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H77" s="11"/>
+      <c r="H77" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I77" s="11" t="s">
         <v>289</v>
       </c>
@@ -5022,7 +5099,9 @@
       <c r="G78" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H78" s="11"/>
+      <c r="H78" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I78" s="11" t="s">
         <v>273</v>
       </c>
@@ -5086,7 +5165,9 @@
       <c r="G80" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H80" s="11"/>
+      <c r="H80" s="11" t="s">
+        <v>522</v>
+      </c>
       <c r="I80" s="11" t="s">
         <v>273</v>
       </c>
@@ -6241,7 +6322,9 @@
       <c r="G117" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="H117" s="51"/>
+      <c r="H117" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I117" s="51"/>
       <c r="J117" s="52"/>
       <c r="K117" s="53" t="s">
@@ -6526,7 +6609,9 @@
       <c r="G126" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="H126" s="51"/>
+      <c r="H126" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I126" s="51"/>
       <c r="J126" s="52"/>
       <c r="K126" s="53" t="s">
@@ -6683,7 +6768,9 @@
       <c r="G131" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="H131" s="51"/>
+      <c r="H131" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I131" s="51"/>
       <c r="J131" s="52"/>
       <c r="K131" s="53" t="s">
@@ -6789,7 +6876,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="99" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B135" s="100" t="s">
         <v>363</v>
@@ -6824,7 +6911,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="99" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B136" s="100" t="s">
         <v>363</v>
@@ -6857,7 +6944,7 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="99" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B137" s="100" t="s">
         <v>363</v>
@@ -6890,7 +6977,7 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="99" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B138" s="100" t="s">
         <v>363</v>
@@ -6954,7 +7041,7 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B140" s="100" t="s">
         <v>363</v>
@@ -6985,27 +7072,29 @@
       </c>
       <c r="M140" s="12"/>
     </row>
-    <row r="141" spans="1:13" ht="26" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A141" s="99" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="B141" s="100" t="s">
         <v>363</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="D141" s="110" t="s">
-        <v>383</v>
+        <v>517</v>
       </c>
       <c r="E141" s="111" t="s">
-        <v>384</v>
+        <v>516</v>
       </c>
       <c r="F141" s="49"/>
       <c r="G141" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="H141" s="51"/>
+        <v>90</v>
+      </c>
+      <c r="H141" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I141" s="51"/>
       <c r="J141" s="52"/>
       <c r="K141" s="53" t="s">
@@ -7014,62 +7103,64 @@
       <c r="L141" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="M141" s="12"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M141" s="103"/>
+    </row>
+    <row r="142" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A142" s="99" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B142" s="100" t="s">
         <v>363</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="D142" s="110" t="s">
-        <v>385</v>
+        <v>518</v>
       </c>
       <c r="E142" s="111" t="s">
-        <v>386</v>
-      </c>
-      <c r="F142" s="49" t="s">
-        <v>387</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="F142" s="49"/>
       <c r="G142" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="H142" s="51"/>
+        <v>90</v>
+      </c>
+      <c r="H142" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I142" s="51"/>
       <c r="J142" s="52"/>
       <c r="K142" s="53" t="s">
-        <v>500</v>
+        <v>13</v>
       </c>
       <c r="L142" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="M142" s="12"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M142" s="103"/>
+    </row>
+    <row r="143" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A143" s="99" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="B143" s="100" t="s">
         <v>363</v>
       </c>
       <c r="C143" s="48" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="D143" s="110" t="s">
-        <v>389</v>
+        <v>519</v>
       </c>
       <c r="E143" s="111" t="s">
-        <v>390</v>
+        <v>521</v>
       </c>
       <c r="F143" s="49"/>
       <c r="G143" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="H143" s="51"/>
+        <v>90</v>
+      </c>
+      <c r="H143" s="51" t="s">
+        <v>522</v>
+      </c>
       <c r="I143" s="51"/>
       <c r="J143" s="52"/>
       <c r="K143" s="53" t="s">
@@ -7078,27 +7169,27 @@
       <c r="L143" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="M143" s="12"/>
+      <c r="M143" s="103"/>
     </row>
     <row r="144" spans="1:13" ht="26" x14ac:dyDescent="0.35">
-      <c r="A144" s="109" t="s">
-        <v>508</v>
-      </c>
-      <c r="B144" s="108" t="s">
+      <c r="A144" s="99" t="s">
+        <v>511</v>
+      </c>
+      <c r="B144" s="100" t="s">
         <v>363</v>
       </c>
       <c r="C144" s="48" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D144" s="110" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E144" s="111" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="F144" s="49"/>
       <c r="G144" s="50" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H144" s="51"/>
       <c r="I144" s="51"/>
@@ -7111,8 +7202,103 @@
       </c>
       <c r="M144" s="12"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="107"/>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A145" s="99" t="s">
+        <v>506</v>
+      </c>
+      <c r="B145" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C145" s="48" t="s">
+        <v>382</v>
+      </c>
+      <c r="D145" s="110" t="s">
+        <v>385</v>
+      </c>
+      <c r="E145" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="F145" s="49" t="s">
+        <v>387</v>
+      </c>
+      <c r="G145" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H145" s="51"/>
+      <c r="I145" s="51"/>
+      <c r="J145" s="52"/>
+      <c r="K145" s="53" t="s">
+        <v>511</v>
+      </c>
+      <c r="L145" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="M145" s="12"/>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A146" s="99" t="s">
+        <v>512</v>
+      </c>
+      <c r="B146" s="100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C146" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="D146" s="110" t="s">
+        <v>389</v>
+      </c>
+      <c r="E146" s="111" t="s">
+        <v>390</v>
+      </c>
+      <c r="F146" s="49"/>
+      <c r="G146" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H146" s="51"/>
+      <c r="I146" s="51"/>
+      <c r="J146" s="52"/>
+      <c r="K146" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="L146" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="M146" s="12"/>
+    </row>
+    <row r="147" spans="1:13" ht="26" x14ac:dyDescent="0.35">
+      <c r="A147" s="109" t="s">
+        <v>513</v>
+      </c>
+      <c r="B147" s="108" t="s">
+        <v>363</v>
+      </c>
+      <c r="C147" s="48" t="s">
+        <v>388</v>
+      </c>
+      <c r="D147" s="110" t="s">
+        <v>391</v>
+      </c>
+      <c r="E147" s="111" t="s">
+        <v>392</v>
+      </c>
+      <c r="F147" s="49"/>
+      <c r="G147" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H147" s="51"/>
+      <c r="I147" s="51"/>
+      <c r="J147" s="52"/>
+      <c r="K147" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="L147" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="M147" s="12"/>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A148" s="107"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
make yes/no-description-fields consistent by choosing right wording by staying aligned to the original questionnaire
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
+++ b/dataland-framework-toolbox/inputs/esg-questionnaire/esg-questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92432\Documents\Projekte\02-Dataland\Dataland\dataland-framework-toolbox\inputs\esg-questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B2402-0C23-4FE8-99BE-CE307779CB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5FFDB0-B6F9-4110-BE93-902E9C7E257E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,9 +217,6 @@
     <t>Richtlinien zur Einhaltung der OECD-Leitsätze</t>
   </si>
   <si>
-    <t>Bitte teilen Sie die Richtlinien mit uns die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD-Leitsätze überwacht.</t>
-  </si>
-  <si>
     <t>Richtlinien die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD-Leitsätze überwacht</t>
   </si>
   <si>
@@ -340,9 +337,6 @@
     <t>40.3</t>
   </si>
   <si>
-    <t>Nachhaltigkeitsstrategie vorhanden</t>
-  </si>
-  <si>
     <t>Verfügt das Unternehmen über eine Nachhaltigkeitsstrategie?</t>
   </si>
   <si>
@@ -355,18 +349,9 @@
     <t>Werden spezielle Ziele / Maßnahmen ergriffen, um das 1,5 °C Ziel zu erreichen?</t>
   </si>
   <si>
-    <t>Maßnahmen bezüglich 1,5 Grad Celsius Ziel vorhanden</t>
-  </si>
-  <si>
     <t>Dokumente zur Nachhaltigkeitsstrategie</t>
   </si>
   <si>
-    <t>Beschreibung Maßnahmen bezüglich 1,5 Grad Celsius Ziel</t>
-  </si>
-  <si>
-    <t>Beschreiben Sie spezielle Ziele / Maßnahmen, um das 1,5°C Ziel zu erreichen.</t>
-  </si>
-  <si>
     <t>Zugewiesene Budgets bis 2030</t>
   </si>
   <si>
@@ -484,9 +469,6 @@
     <t>Bezüglich der angegebenen Maßnahmen: Bitte die geplanten Vollzeitäquivalente ab dem Jahr 2031 angeben.</t>
   </si>
   <si>
-    <t>Taxonomiebezogene CapEx-Planung vorhanden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hat das Unternehmen eine taxonomiebezogene CapEx-Planung? </t>
   </si>
   <si>
@@ -790,9 +772,6 @@
     <t>16</t>
   </si>
   <si>
-    <t>Einzelheiten zu ESG-bezogenen Rechtsstreitigkeiten</t>
-  </si>
-  <si>
     <t>Ist das Unternehmen in laufende bzw. war das Unternehmen in den letzten 3 Jahren in rechtskräftig abgeschlossene Rechtsstreitigkeiten im Zusammenhang mit Nachhaltigkeit / ESG involviert? Im Vordergrund stehen vor Gericht bereits anhängige Verfahren.</t>
   </si>
   <si>
@@ -1132,9 +1111,6 @@
     <t>Gibt es weitere wesentliche soziale Risiken für das Unternehmen?</t>
   </si>
   <si>
-    <t>Weitere wesentliche soziale Risiken Erläuterung</t>
-  </si>
-  <si>
     <t>Erläutern sie die weiteren wesentlichenn sozialen Risiken.</t>
   </si>
   <si>
@@ -1192,9 +1168,6 @@
     <t>Ist die Vergütung des Top-Managements (auch) explizit an Nachhaltigkeitsziele gekoppelt (bspw. ESG-Rating)?</t>
   </si>
   <si>
-    <t>Kopplung von Vergütung des Top-Managements an Nachhaltigkeitsziele Erläuterung</t>
-  </si>
-  <si>
     <t>Bitte die bestehende Regelung skizzieren.</t>
   </si>
   <si>
@@ -1210,9 +1183,6 @@
     <t>Verfügt das Unternehmen über einen institutionalisierten, CSRD-konformen Prozess zur Berücksichtigung der Interessen der Stakeholder des Unternehmens?</t>
   </si>
   <si>
-    <t>CSRD-konformer Prozess zur Berücksichtigung der Stakeholderinteressen Erläuterung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bitte den Prozess in seiner Methodik skizzieren und wichtigste Schlussfolgerungen darstellen. </t>
   </si>
   <si>
@@ -1318,9 +1288,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>Transitionsplan vorhanden</t>
-  </si>
-  <si>
     <t>Verfügt das Unternehmen über einen Transitionsplan?</t>
   </si>
   <si>
@@ -1339,9 +1306,6 @@
     <t>Yes/No/NA</t>
   </si>
   <si>
-    <t>Produkte zur Reduzierung der Umweltbelastung Erläuterungen</t>
-  </si>
-  <si>
     <t>Bitte kurz skizzieren wie die Produkte die Umweltbelastung verringern.</t>
   </si>
   <si>
@@ -1393,9 +1357,6 @@
     <t>Nutzt das Unternehmen Kompensationsinstrumente in Bezug auf Treibhausgasemissionen?</t>
   </si>
   <si>
-    <t>Kompensationsinstrumente Treibhausgasemissionen Zertifizierungen</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -1450,9 +1411,6 @@
     <t>Verfügt das Unternehmen über ein Abfallmanagementsystem?</t>
   </si>
   <si>
-    <t>Abfallmanagementsystem Erläuterungen</t>
-  </si>
-  <si>
     <t>Bitte skizzieren sie kurz das vorhandene System, insbesondere zur Produktion von und Umgang mit gefährlichen Abfällen.</t>
   </si>
   <si>
@@ -1465,9 +1423,6 @@
     <t>Plant das Unternehmen den Anteil von Recyclaten im Produktionsprozess zu erhöhen?</t>
   </si>
   <si>
-    <t>Geplante Erhöhung des Anteils von Recyclaten Erläuterungen</t>
-  </si>
-  <si>
     <t>Bitte Basisjahr / Basiswert und entsprechende Planwerte angeben.</t>
   </si>
   <si>
@@ -1498,9 +1453,6 @@
     <t>Wirken sich die Geschäftsaktivitäten des Unternehmens negativ auf die Biodiversität oder das Ökosystem aus?</t>
   </si>
   <si>
-    <t>Negative Auswirkungen auf Biodiversität und Ökosystem Erläuterungen</t>
-  </si>
-  <si>
     <t>Soweit vorhanden, bitte verwendete Methodik benennen auf deren Basis das Ergebnis ermittelt wurde.</t>
   </si>
   <si>
@@ -1510,9 +1462,6 @@
     <t>Wirken sich die Geschäftsaktivitäten des Unternehmens positiv auf die Biodiversität oder das Ökosystem aus?</t>
   </si>
   <si>
-    <t>Positive Auswirkungen auf Biodiversität und Ökosystem Erläuterungen</t>
-  </si>
-  <si>
     <t>Gegenmaßnahmen negative Auswirkungen auf Biodiversität und Ökosystem</t>
   </si>
   <si>
@@ -1523,9 +1472,6 @@
   </si>
   <si>
     <t>Plant das Unternehmen seinen Wasserverbrauch zu reduzieren?</t>
-  </si>
-  <si>
-    <t>Plan zur Reduktion des Wasserverbrauchs Erläuterung</t>
   </si>
   <si>
     <t>Bitte skizzieren sie kurz, wie der Wasserverbrauch reduziert werden soll.</t>
@@ -1625,6 +1571,60 @@
   </si>
   <si>
     <t>Allowed Range: [0, INF]</t>
+  </si>
+  <si>
+    <t>Nachhaltigkeitsstrategie</t>
+  </si>
+  <si>
+    <t>Skizzieren Sie spezielle Ziele / Maßnahmen, um das 1,5°C Ziel zu erreichen.</t>
+  </si>
+  <si>
+    <t>Maßnahmen zur Erreichung des 1,5 Grad Celsius Ziels</t>
+  </si>
+  <si>
+    <t>Skizzierung von Maßnahmen zur Erreichung des 1,5 Grad Celsius Ziels</t>
+  </si>
+  <si>
+    <t>Taxonomiebezogene CapEx-Planung</t>
+  </si>
+  <si>
+    <t>Bitte teilen Sie die Richtlinien mit uns, die beschreiben oder Informationen darüber liefern, wie das Unternehmen die Einhaltung der OECD-Leitsätze überwacht.</t>
+  </si>
+  <si>
+    <t>Einzelheiten zu Rechtsstreitigkeiten mit ESG-Bezug</t>
+  </si>
+  <si>
+    <t>Transitionsplan</t>
+  </si>
+  <si>
+    <t>Skizzierung der Produkte zur Reduzierung der Umweltbelastung</t>
+  </si>
+  <si>
+    <t>Zertifizierungen bezüglich Kompensationinstrumenten</t>
+  </si>
+  <si>
+    <t>Skizzierung Abfallmanagementsystem</t>
+  </si>
+  <si>
+    <t>Angaben zur geplanten Erhöhung des Anteils von Recyclaten</t>
+  </si>
+  <si>
+    <t>Methodik zur Ermittlung von negativen Auswirkungen auf Biodiversität und Ökosystem</t>
+  </si>
+  <si>
+    <t>Methodik zur Ermittlung von positiven Auswirkungen auf Biodiversität und Ökosystem</t>
+  </si>
+  <si>
+    <t>Skizzierung des Plans zur Reduktion des Wasserverbrauchs</t>
+  </si>
+  <si>
+    <t>Erläuterung zu weiteren wesentlichen sozialen Risiken</t>
+  </si>
+  <si>
+    <t>Skizzierung der Regelung zur Kopplung von Vergütung des Top-Managements an Nachhaltigkeitsziele</t>
+  </si>
+  <si>
+    <t>Skizzierung des CSRD-konformen Prozesses zur Berücksichtigung der Stakeholderinteressen</t>
   </si>
 </sst>
 </file>
@@ -2542,7 +2542,7 @@
   <dimension ref="A1:M148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2665,13 +2665,13 @@
         <v>25</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>95</v>
+        <v>505</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="15" t="s">
@@ -2696,13 +2696,13 @@
         <v>25</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="15" t="s">
@@ -2727,13 +2727,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>97</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>99</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="15" t="s">
@@ -2758,13 +2758,13 @@
         <v>25</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>102</v>
+        <v>95</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>508</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>103</v>
+        <v>506</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="20" t="s">
@@ -2783,29 +2783,29 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="17" t="s">
@@ -2818,29 +2818,29 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="17" t="s">
@@ -2853,29 +2853,29 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="23" t="s">
@@ -2888,29 +2888,29 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="23" t="s">
@@ -2923,29 +2923,29 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="23" t="s">
@@ -2958,29 +2958,29 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="23" t="s">
@@ -2999,13 +2999,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="20" t="s">
@@ -3030,17 +3030,17 @@
         <v>25</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -3061,23 +3061,23 @@
         <v>25</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F16" s="27"/>
       <c r="G16" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="23" t="s">
@@ -3090,29 +3090,29 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="23" t="s">
@@ -3125,29 +3125,29 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E18" s="47" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="23" t="s">
@@ -3160,29 +3160,29 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E19" s="47" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="23" t="s">
@@ -3195,29 +3195,29 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="23" t="s">
@@ -3230,29 +3230,29 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E21" s="47" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="23" t="s">
@@ -3265,19 +3265,19 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>508</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>143</v>
+        <v>490</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>509</v>
       </c>
       <c r="E22" s="47" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="20" t="s">
@@ -3296,29 +3296,29 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E23" s="47" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="28"/>
       <c r="J23" s="12"/>
       <c r="K23" s="17" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="L23" s="26" t="s">
         <v>19</v>
@@ -3327,29 +3327,29 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E24" s="47" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="28"/>
       <c r="J24" s="12"/>
       <c r="K24" s="17" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="L24" s="26" t="s">
         <v>19</v>
@@ -3358,19 +3358,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F25" s="27"/>
       <c r="G25" s="20" t="s">
@@ -3389,29 +3389,29 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="28"/>
       <c r="J26" s="12"/>
       <c r="K26" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L26" s="26" t="s">
         <v>19</v>
@@ -3420,29 +3420,29 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E27" s="47" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="28"/>
       <c r="J27" s="12"/>
       <c r="K27" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L27" s="26" t="s">
         <v>19</v>
@@ -3451,29 +3451,29 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E28" s="47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="28"/>
       <c r="J28" s="12"/>
       <c r="K28" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L28" s="26" t="s">
         <v>19</v>
@@ -3482,19 +3482,19 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E29" s="47" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="20" t="s">
@@ -3513,29 +3513,29 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="28"/>
       <c r="J30" s="12"/>
       <c r="K30" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L30" s="26" t="s">
         <v>19</v>
@@ -3544,29 +3544,29 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="28"/>
       <c r="J31" s="12"/>
       <c r="K31" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L31" s="26" t="s">
         <v>19</v>
@@ -3575,29 +3575,29 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="28"/>
       <c r="J32" s="12"/>
       <c r="K32" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L32" s="26" t="s">
         <v>19</v>
@@ -3606,19 +3606,19 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E33" s="47" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F33" s="27"/>
       <c r="G33" s="20" t="s">
@@ -3637,29 +3637,29 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E34" s="47" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="28"/>
       <c r="J34" s="12"/>
       <c r="K34" s="23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L34" s="26" t="s">
         <v>19</v>
@@ -3668,29 +3668,29 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="28"/>
       <c r="J35" s="12"/>
       <c r="K35" s="23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L35" s="26" t="s">
         <v>19</v>
@@ -3699,29 +3699,29 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="28"/>
       <c r="J36" s="12"/>
       <c r="K36" s="23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L36" s="26" t="s">
         <v>19</v>
@@ -3730,19 +3730,19 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E37" s="47" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F37" s="27"/>
       <c r="G37" s="20" t="s">
@@ -3761,29 +3761,29 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E38" s="47" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F38" s="27"/>
       <c r="G38" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="28"/>
       <c r="J38" s="12"/>
       <c r="K38" s="17" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="L38" s="26" t="s">
         <v>19</v>
@@ -3792,29 +3792,29 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="28"/>
       <c r="J39" s="12"/>
       <c r="K39" s="17" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="L39" s="26" t="s">
         <v>19</v>
@@ -3823,29 +3823,29 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E40" s="47" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="28"/>
       <c r="J40" s="12"/>
       <c r="K40" s="17" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="L40" s="26" t="s">
         <v>19</v>
@@ -3854,19 +3854,19 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="39" t="s">
         <v>65</v>
-      </c>
-      <c r="E41" s="39" t="s">
-        <v>66</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="15" t="s">
@@ -3885,29 +3885,29 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="12"/>
       <c r="K42" s="17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>19</v>
@@ -3916,29 +3916,29 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E43" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="15"/>
       <c r="K43" s="17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>19</v>
@@ -3947,19 +3947,19 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D44" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="39" t="s">
         <v>70</v>
-      </c>
-      <c r="E44" s="39" t="s">
-        <v>71</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="15" t="s">
@@ -3971,7 +3971,7 @@
         <v>36</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="L44" s="12" t="s">
         <v>19</v>
@@ -3986,16 +3986,16 @@
         <v>25</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E45" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="F45" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="G45" s="25" t="s">
         <v>18</v>
@@ -4021,16 +4021,16 @@
         <v>25</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E46" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="G46" s="25" t="s">
         <v>18</v>
@@ -4050,22 +4050,22 @@
     </row>
     <row r="47" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A47" s="34" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D47" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E47" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>220</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="G47" s="25" t="s">
         <v>18</v>
@@ -4085,22 +4085,22 @@
     </row>
     <row r="48" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A48" s="34" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>40</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G48" s="25" t="s">
         <v>18</v>
@@ -4120,22 +4120,22 @@
     </row>
     <row r="49" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A49" s="34" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G49" s="25" t="s">
         <v>18</v>
@@ -4155,22 +4155,22 @@
     </row>
     <row r="50" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="34" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E50" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>229</v>
       </c>
       <c r="G50" s="25" t="s">
         <v>18</v>
@@ -4190,22 +4190,22 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="34" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G51" s="25" t="s">
         <v>18</v>
@@ -4225,13 +4225,13 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>42</v>
@@ -4256,19 +4256,19 @@
     </row>
     <row r="53" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A53" s="34" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D53" s="21" t="s">
         <v>44</v>
       </c>
       <c r="E53" s="35" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>45</v>
@@ -4280,7 +4280,7 @@
       <c r="I53" s="25"/>
       <c r="J53" s="15"/>
       <c r="K53" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>19</v>
@@ -4289,13 +4289,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="34" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>46</v>
@@ -4313,7 +4313,7 @@
       <c r="I54" s="25"/>
       <c r="J54" s="15"/>
       <c r="K54" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L54" s="12" t="s">
         <v>19</v>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="55" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A55" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>25</v>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="56" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A56" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>25</v>
@@ -4365,10 +4365,10 @@
         <v>53</v>
       </c>
       <c r="E56" s="35" t="s">
+        <v>510</v>
+      </c>
+      <c r="F56" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="G56" s="25" t="s">
         <v>33</v>
@@ -4377,7 +4377,7 @@
       <c r="I56" s="11"/>
       <c r="J56" s="15"/>
       <c r="K56" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L56" s="12" t="s">
         <v>19</v>
@@ -4386,7 +4386,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="34" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>25</v>
@@ -4395,7 +4395,7 @@
         <v>50</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="36" t="s">
         <v>47</v>
@@ -4410,7 +4410,7 @@
       <c r="I57" s="11"/>
       <c r="J57" s="12"/>
       <c r="K57" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L57" s="12" t="s">
         <v>19</v>
@@ -4419,19 +4419,19 @@
     </row>
     <row r="58" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A58" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="15" t="s">
@@ -4450,26 +4450,26 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E59" s="38" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I59" s="11"/>
       <c r="J59" s="12"/>
@@ -4483,19 +4483,19 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E60" s="38" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F60" s="27"/>
       <c r="G60" s="29" t="s">
@@ -4514,19 +4514,19 @@
     </row>
     <row r="61" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A61" s="34" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="15" t="s">
@@ -4545,19 +4545,19 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>245</v>
+        <v>511</v>
       </c>
       <c r="E62" s="38" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F62" s="27"/>
       <c r="G62" s="29" t="s">
@@ -4567,7 +4567,7 @@
       <c r="I62" s="11"/>
       <c r="J62" s="12"/>
       <c r="K62" s="17" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L62" s="12" t="s">
         <v>19</v>
@@ -4576,19 +4576,19 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="15" t="s">
@@ -4607,19 +4607,19 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="34" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E64" s="38" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F64" s="27"/>
       <c r="G64" s="29" t="s">
@@ -4629,7 +4629,7 @@
       <c r="I64" s="11"/>
       <c r="J64" s="12"/>
       <c r="K64" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L64" s="12" t="s">
         <v>19</v>
@@ -4638,19 +4638,19 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="15" t="s">
@@ -4669,19 +4669,19 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="34" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="D66" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="D66" s="21" t="s">
-        <v>255</v>
-      </c>
       <c r="E66" s="38" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="29" t="s">
@@ -4691,7 +4691,7 @@
       <c r="I66" s="11"/>
       <c r="J66" s="12"/>
       <c r="K66" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L66" s="12" t="s">
         <v>19</v>
@@ -4700,29 +4700,29 @@
     </row>
     <row r="67" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A67" s="34" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J67" s="12"/>
       <c r="K67" s="17" t="s">
@@ -4735,29 +4735,29 @@
     </row>
     <row r="68" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A68" s="34" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="F68" s="41"/>
       <c r="G68" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J68" s="12"/>
       <c r="K68" s="17" t="s">
@@ -4770,29 +4770,29 @@
     </row>
     <row r="69" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A69" s="34" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F69" s="41"/>
       <c r="G69" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="17" t="s">
@@ -4805,29 +4805,29 @@
     </row>
     <row r="70" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A70" s="34" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F70" s="41"/>
       <c r="G70" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J70" s="12"/>
       <c r="K70" s="17" t="s">
@@ -4840,29 +4840,29 @@
     </row>
     <row r="71" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A71" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E71" s="38" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F71" s="41"/>
       <c r="G71" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="17" t="s">
@@ -4875,29 +4875,29 @@
     </row>
     <row r="72" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A72" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E72" s="38" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F72" s="41"/>
       <c r="G72" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J72" s="12"/>
       <c r="K72" s="17" t="s">
@@ -4910,29 +4910,29 @@
     </row>
     <row r="73" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A73" s="34" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E73" s="38" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F73" s="41"/>
       <c r="G73" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J73" s="12"/>
       <c r="K73" s="17" t="s">
@@ -4945,29 +4945,29 @@
     </row>
     <row r="74" spans="1:13" ht="51" x14ac:dyDescent="0.35">
       <c r="A74" s="34" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J74" s="12"/>
       <c r="K74" s="17" t="s">
@@ -4980,29 +4980,29 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E75" s="38" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F75" s="41"/>
       <c r="G75" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="J75" s="12"/>
       <c r="K75" s="17" t="s">
@@ -5015,23 +5015,23 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="34" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E76" s="42" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F76" s="41"/>
       <c r="G76" s="29" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
@@ -5046,29 +5046,29 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E77" s="38" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F77" s="41"/>
       <c r="G77" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="J77" s="12"/>
       <c r="K77" s="17" t="s">
@@ -5081,29 +5081,29 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E78" s="38" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="F78" s="41"/>
       <c r="G78" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J78" s="12"/>
       <c r="K78" s="17" t="s">
@@ -5116,23 +5116,23 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="34" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E79" s="38" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="29" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
@@ -5147,29 +5147,29 @@
     </row>
     <row r="80" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A80" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E80" s="38" t="s">
         <v>290</v>
-      </c>
-      <c r="D80" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="E80" s="38" t="s">
-        <v>297</v>
       </c>
       <c r="F80" s="41"/>
       <c r="G80" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J80" s="12"/>
       <c r="K80" s="17" t="s">
@@ -5182,19 +5182,19 @@
     </row>
     <row r="81" spans="1:13" ht="63.5" x14ac:dyDescent="0.35">
       <c r="A81" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E81" s="38" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F81" s="41"/>
       <c r="G81" s="29" t="s">
@@ -5213,26 +5213,26 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="34" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E82" s="38" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="F82" s="41"/>
       <c r="G82" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="I82" s="11"/>
       <c r="J82" s="12"/>
@@ -5246,19 +5246,19 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="34" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E83" s="38" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="F83" s="41"/>
       <c r="G83" s="29" t="s">
@@ -5277,19 +5277,19 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C84" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E84" s="38" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="29" t="s">
@@ -5308,19 +5308,19 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="34" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E85" s="38" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="F85" s="41"/>
       <c r="G85" s="29" t="s">
@@ -5330,7 +5330,7 @@
       <c r="I85" s="11"/>
       <c r="J85" s="12"/>
       <c r="K85" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L85" s="12" t="s">
         <v>19</v>
@@ -5339,19 +5339,19 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="34" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C86" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E86" s="38" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="29" t="s">
@@ -5361,7 +5361,7 @@
       <c r="I86" s="11"/>
       <c r="J86" s="12"/>
       <c r="K86" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L86" s="12" t="s">
         <v>19</v>
@@ -5370,19 +5370,19 @@
     </row>
     <row r="87" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A87" s="34" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C87" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D87" s="55" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E87" s="56" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="F87" s="41"/>
       <c r="G87" s="29" t="s">
@@ -5392,7 +5392,7 @@
       <c r="I87" s="11"/>
       <c r="J87" s="12"/>
       <c r="K87" s="17" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="L87" s="12" t="s">
         <v>19</v>
@@ -5401,19 +5401,19 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="34" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C88" s="105" t="s">
+        <v>398</v>
+      </c>
+      <c r="D88" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="D88" s="21" t="s">
-        <v>418</v>
-      </c>
       <c r="E88" s="38" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="29" t="s">
@@ -5432,19 +5432,19 @@
     </row>
     <row r="89" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A89" s="34" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="E89" s="38" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F89" s="41"/>
       <c r="G89" s="29" t="s">
@@ -5454,7 +5454,7 @@
       <c r="I89" s="11"/>
       <c r="J89" s="12"/>
       <c r="K89" s="17" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="L89" s="12" t="s">
         <v>19</v>
@@ -5463,19 +5463,19 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="34" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90" s="105" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>421</v>
+        <v>512</v>
       </c>
       <c r="E90" s="38" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="F90" s="41"/>
       <c r="G90" s="29" t="s">
@@ -5496,19 +5496,19 @@
     </row>
     <row r="91" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A91" s="63" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="B91" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C91" s="61" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="E91" s="39" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="F91" s="57"/>
       <c r="G91" s="60" t="s">
@@ -5527,19 +5527,19 @@
     </row>
     <row r="92" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A92" s="63" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="B92" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C92" s="61" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="E92" s="39" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F92" s="57"/>
       <c r="G92" s="60" t="s">
@@ -5558,23 +5558,23 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="73" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B93" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C93" s="70" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="E93" s="39" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="F93" s="66"/>
       <c r="G93" s="69" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H93" s="67"/>
       <c r="I93" s="67"/>
@@ -5589,19 +5589,19 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="72" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C94" s="70" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>428</v>
+        <v>513</v>
       </c>
       <c r="E94" s="39" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="F94" s="66"/>
       <c r="G94" s="69" t="s">
@@ -5611,7 +5611,7 @@
       <c r="I94" s="67"/>
       <c r="J94" s="68"/>
       <c r="K94" s="71" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="L94" s="68" t="s">
         <v>19</v>
@@ -5620,23 +5620,23 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="63" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="B95" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C95" s="78" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="E95" s="39" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="F95" s="74"/>
       <c r="G95" s="77" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H95" s="75"/>
       <c r="I95" s="75"/>
@@ -5651,23 +5651,23 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="63" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="B96" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C96" s="78" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="E96" s="39" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="F96" s="74"/>
       <c r="G96" s="77" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H96" s="75"/>
       <c r="I96" s="75"/>
@@ -5682,23 +5682,23 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="63" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="B97" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C97" s="78" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D97" s="40" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="E97" s="39" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="F97" s="74"/>
       <c r="G97" s="77" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H97" s="75"/>
       <c r="I97" s="75"/>
@@ -5713,19 +5713,19 @@
     </row>
     <row r="98" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A98" s="63" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="B98" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C98" s="78" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D98" s="40" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="E98" s="39" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="F98" s="74"/>
       <c r="G98" s="77" t="s">
@@ -5744,19 +5744,19 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="73" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="B99" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="E99" s="39" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="F99" s="80"/>
       <c r="G99" s="83" t="s">
@@ -5775,19 +5775,19 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="73" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B100" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>446</v>
+        <v>514</v>
       </c>
       <c r="E100" s="39" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="F100" s="80"/>
       <c r="G100" s="83" t="s">
@@ -5797,7 +5797,7 @@
       <c r="I100" s="81"/>
       <c r="J100" s="82"/>
       <c r="K100" s="85" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="L100" s="82" t="s">
         <v>19</v>
@@ -5806,23 +5806,23 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="63" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="B101" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C101" s="90" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D101" s="40" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="E101" s="39" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="F101" s="86"/>
       <c r="G101" s="89" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H101" s="87"/>
       <c r="I101" s="87"/>
@@ -5837,23 +5837,23 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="63" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B102" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C102" s="90" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="E102" s="39" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="F102" s="86"/>
       <c r="G102" s="89" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H102" s="87"/>
       <c r="I102" s="87"/>
@@ -5868,23 +5868,23 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="63" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="B103" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C103" s="90" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D103" s="40" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="E103" s="39" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="F103" s="86"/>
       <c r="G103" s="89" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H103" s="87"/>
       <c r="I103" s="87"/>
@@ -5899,19 +5899,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" s="63" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B104" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C104" s="90" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="E104" s="39" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="F104" s="86"/>
       <c r="G104" s="89" t="s">
@@ -5930,23 +5930,23 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" s="73" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="B105" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C105" s="97" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E105" s="39" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="F105" s="93"/>
       <c r="G105" s="96" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H105" s="94"/>
       <c r="I105" s="94"/>
@@ -5961,19 +5961,19 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" s="73" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="B106" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C106" s="97" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>465</v>
+        <v>515</v>
       </c>
       <c r="E106" s="39" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="F106" s="93"/>
       <c r="G106" s="96" t="s">
@@ -5983,7 +5983,7 @@
       <c r="I106" s="94"/>
       <c r="J106" s="95"/>
       <c r="K106" s="98" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="L106" s="95" t="s">
         <v>19</v>
@@ -5992,23 +5992,23 @@
     </row>
     <row r="107" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A107" s="73" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="B107" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C107" s="97" t="s">
+        <v>449</v>
+      </c>
+      <c r="D107" s="40" t="s">
+        <v>453</v>
+      </c>
+      <c r="E107" s="39" t="s">
         <v>462</v>
-      </c>
-      <c r="D107" s="40" t="s">
-        <v>467</v>
-      </c>
-      <c r="E107" s="39" t="s">
-        <v>477</v>
       </c>
       <c r="F107" s="93"/>
       <c r="G107" s="96" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H107" s="94"/>
       <c r="I107" s="94"/>
@@ -6023,23 +6023,23 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="B108" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C108" s="97" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="E108" s="39" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="F108" s="93"/>
       <c r="G108" s="96" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H108" s="94"/>
       <c r="I108" s="94"/>
@@ -6054,19 +6054,19 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="73" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="B109" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C109" s="97" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D109" s="40" t="s">
-        <v>470</v>
+        <v>516</v>
       </c>
       <c r="E109" s="39" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="F109" s="93"/>
       <c r="G109" s="96" t="s">
@@ -6076,7 +6076,7 @@
       <c r="I109" s="94"/>
       <c r="J109" s="95"/>
       <c r="K109" s="98" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="L109" s="95" t="s">
         <v>19</v>
@@ -6085,23 +6085,23 @@
     </row>
     <row r="110" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="63" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="B110" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C110" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D110" s="40" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="E110" s="39" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="F110" s="101"/>
       <c r="G110" s="104" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H110" s="102"/>
       <c r="I110" s="102"/>
@@ -6116,19 +6116,19 @@
     </row>
     <row r="111" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="63" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="B111" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C111" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="E111" s="39" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="F111" s="101"/>
       <c r="G111" s="104" t="s">
@@ -6138,7 +6138,7 @@
       <c r="I111" s="102"/>
       <c r="J111" s="103"/>
       <c r="K111" s="106" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="L111" s="103" t="s">
         <v>19</v>
@@ -6147,23 +6147,23 @@
     </row>
     <row r="112" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="63" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="B112" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C112" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="E112" s="39" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="F112" s="101"/>
       <c r="G112" s="104" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H112" s="102"/>
       <c r="I112" s="102"/>
@@ -6178,19 +6178,19 @@
     </row>
     <row r="113" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="63" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="B113" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C113" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>485</v>
+        <v>518</v>
       </c>
       <c r="E113" s="39" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="F113" s="101"/>
       <c r="G113" s="104" t="s">
@@ -6200,7 +6200,7 @@
       <c r="I113" s="102"/>
       <c r="J113" s="103"/>
       <c r="K113" s="106" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="L113" s="103" t="s">
         <v>19</v>
@@ -6209,19 +6209,19 @@
     </row>
     <row r="114" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="63" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B114" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C114" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="E114" s="39" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="F114" s="101"/>
       <c r="G114" s="104" t="s">
@@ -6231,7 +6231,7 @@
       <c r="I114" s="102"/>
       <c r="J114" s="103"/>
       <c r="K114" s="106" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="L114" s="103" t="s">
         <v>19</v>
@@ -6240,23 +6240,23 @@
     </row>
     <row r="115" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="63" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B115" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C115" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="E115" s="39" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="F115" s="101"/>
       <c r="G115" s="104" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H115" s="102"/>
       <c r="I115" s="102"/>
@@ -6271,19 +6271,19 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" s="63" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B116" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C116" s="105" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>490</v>
+        <v>519</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="F116" s="101"/>
       <c r="G116" s="104" t="s">
@@ -6293,7 +6293,7 @@
       <c r="I116" s="102"/>
       <c r="J116" s="103"/>
       <c r="K116" s="106" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="L116" s="103" t="s">
         <v>19</v>
@@ -6302,28 +6302,28 @@
     </row>
     <row r="117" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A117" s="99" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B117" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="C117" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D117" s="110" t="s">
+        <v>312</v>
+      </c>
+      <c r="E117" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="F117" s="49" t="s">
+        <v>314</v>
+      </c>
+      <c r="G117" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C117" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="D117" s="110" t="s">
-        <v>319</v>
-      </c>
-      <c r="E117" s="111" t="s">
-        <v>320</v>
-      </c>
-      <c r="F117" s="49" t="s">
-        <v>321</v>
-      </c>
-      <c r="G117" s="50" t="s">
-        <v>90</v>
-      </c>
       <c r="H117" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I117" s="51"/>
       <c r="J117" s="52"/>
@@ -6337,25 +6337,25 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" s="99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B118" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D118" s="110" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E118" s="111" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F118" s="49" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G118" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H118" s="51"/>
       <c r="I118" s="51"/>
@@ -6370,25 +6370,25 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" s="99" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="B119" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C119" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D119" s="110" t="s">
         <v>318</v>
       </c>
-      <c r="D119" s="110" t="s">
-        <v>325</v>
-      </c>
       <c r="E119" s="111" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F119" s="49" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="G119" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H119" s="51"/>
       <c r="I119" s="51"/>
@@ -6403,25 +6403,25 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" s="99" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="B120" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D120" s="110" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E120" s="111" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F120" s="49" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G120" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H120" s="51"/>
       <c r="I120" s="51"/>
@@ -6436,23 +6436,23 @@
     </row>
     <row r="121" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A121" s="99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B121" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D121" s="110" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="E121" s="111" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F121" s="49"/>
       <c r="G121" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H121" s="51"/>
       <c r="I121" s="51"/>
@@ -6467,23 +6467,23 @@
     </row>
     <row r="122" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A122" s="99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B122" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D122" s="110" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E122" s="111" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F122" s="49"/>
       <c r="G122" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H122" s="51"/>
       <c r="I122" s="51"/>
@@ -6498,23 +6498,23 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" s="99" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B123" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D123" s="110" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E123" s="111" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F123" s="49"/>
       <c r="G123" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H123" s="51"/>
       <c r="I123" s="51"/>
@@ -6529,23 +6529,23 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" s="99" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="B124" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D124" s="110" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E124" s="111" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F124" s="49"/>
       <c r="G124" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H124" s="51"/>
       <c r="I124" s="51"/>
@@ -6560,23 +6560,23 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" s="99" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="B125" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D125" s="110" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E125" s="111" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F125" s="49"/>
       <c r="G125" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H125" s="51"/>
       <c r="I125" s="51"/>
@@ -6591,26 +6591,26 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" s="99" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="B126" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D126" s="110" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E126" s="111" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F126" s="49"/>
       <c r="G126" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H126" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I126" s="51"/>
       <c r="J126" s="52"/>
@@ -6624,23 +6624,23 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" s="99" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="B127" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D127" s="110" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E127" s="111" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F127" s="49"/>
       <c r="G127" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H127" s="51"/>
       <c r="I127" s="51"/>
@@ -6655,26 +6655,26 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" s="99" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="B128" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D128" s="110" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E128" s="111" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="F128" s="49"/>
       <c r="G128" s="54" t="s">
         <v>30</v>
       </c>
       <c r="H128" s="51" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="I128" s="51"/>
       <c r="J128" s="52"/>
@@ -6688,19 +6688,19 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="99" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="B129" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D129" s="110" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E129" s="111" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="F129" s="49"/>
       <c r="G129" s="50" t="s">
@@ -6719,19 +6719,19 @@
     </row>
     <row r="130" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A130" s="99" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="B130" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D130" s="110" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E130" s="111" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="F130" s="49"/>
       <c r="G130" s="50" t="s">
@@ -6750,26 +6750,26 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="99" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="B131" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D131" s="110" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E131" s="111" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="F131" s="49"/>
       <c r="G131" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H131" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I131" s="51"/>
       <c r="J131" s="52"/>
@@ -6783,19 +6783,19 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="99" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B132" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D132" s="110" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E132" s="111" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F132" s="49"/>
       <c r="G132" s="50" t="s">
@@ -6814,19 +6814,19 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="99" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="B133" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D133" s="110" t="s">
-        <v>359</v>
+        <v>520</v>
       </c>
       <c r="E133" s="111" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F133" s="49"/>
       <c r="G133" s="50" t="s">
@@ -6836,7 +6836,7 @@
       <c r="I133" s="51"/>
       <c r="J133" s="52"/>
       <c r="K133" s="53" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="L133" s="52" t="s">
         <v>19</v>
@@ -6845,19 +6845,19 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="99" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="B134" s="100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D134" s="110" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E134" s="111" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="F134" s="49"/>
       <c r="G134" s="50" t="s">
@@ -6876,28 +6876,28 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="99" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="B135" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D135" s="110" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E135" s="111" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="F135" s="49" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="G135" s="50" t="s">
         <v>32</v>
       </c>
       <c r="H135" s="51" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="I135" s="51"/>
       <c r="J135" s="52"/>
@@ -6911,25 +6911,25 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="99" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="B136" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D136" s="110" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="E136" s="111" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="F136" s="49" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G136" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H136" s="51"/>
       <c r="I136" s="51"/>
@@ -6944,25 +6944,25 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="99" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B137" s="100" t="s">
+        <v>355</v>
+      </c>
+      <c r="C137" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="D137" s="110" t="s">
         <v>363</v>
       </c>
-      <c r="C137" s="48" t="s">
+      <c r="E137" s="111" t="s">
         <v>364</v>
       </c>
-      <c r="D137" s="110" t="s">
-        <v>371</v>
-      </c>
-      <c r="E137" s="111" t="s">
-        <v>372</v>
-      </c>
       <c r="F137" s="49" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G137" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H137" s="51"/>
       <c r="I137" s="51"/>
@@ -6977,25 +6977,25 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="99" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="B138" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D138" s="110" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E138" s="111" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F138" s="49" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G138" s="54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H138" s="51"/>
       <c r="I138" s="51"/>
@@ -7010,19 +7010,19 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="99" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="B139" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D139" s="110" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="E139" s="111" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="F139" s="49"/>
       <c r="G139" s="50" t="s">
@@ -7041,22 +7041,22 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="99" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="B140" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D140" s="110" t="s">
-        <v>379</v>
+        <v>521</v>
       </c>
       <c r="E140" s="111" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="F140" s="49" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="G140" s="50" t="s">
         <v>27</v>
@@ -7065,7 +7065,7 @@
       <c r="I140" s="51"/>
       <c r="J140" s="52"/>
       <c r="K140" s="53" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="L140" s="52" t="s">
         <v>19</v>
@@ -7074,26 +7074,26 @@
     </row>
     <row r="141" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A141" s="99" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="B141" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D141" s="110" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
       <c r="E141" s="111" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="F141" s="49"/>
       <c r="G141" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H141" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I141" s="51"/>
       <c r="J141" s="52"/>
@@ -7107,26 +7107,26 @@
     </row>
     <row r="142" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A142" s="99" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="B142" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D142" s="110" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="E142" s="111" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="F142" s="49"/>
       <c r="G142" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H142" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I142" s="51"/>
       <c r="J142" s="52"/>
@@ -7140,26 +7140,26 @@
     </row>
     <row r="143" spans="1:13" s="92" customFormat="1" ht="51" x14ac:dyDescent="0.35">
       <c r="A143" s="99" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="B143" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C143" s="48" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D143" s="110" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="E143" s="111" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="F143" s="49"/>
       <c r="G143" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H143" s="51" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="I143" s="51"/>
       <c r="J143" s="52"/>
@@ -7173,19 +7173,19 @@
     </row>
     <row r="144" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A144" s="99" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="B144" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C144" s="48" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D144" s="110" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E144" s="111" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="F144" s="49"/>
       <c r="G144" s="50" t="s">
@@ -7204,22 +7204,22 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" s="99" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="B145" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C145" s="48" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D145" s="110" t="s">
-        <v>385</v>
+        <v>522</v>
       </c>
       <c r="E145" s="111" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="F145" s="49" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="G145" s="50" t="s">
         <v>27</v>
@@ -7228,7 +7228,7 @@
       <c r="I145" s="51"/>
       <c r="J145" s="52"/>
       <c r="K145" s="53" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="L145" s="52" t="s">
         <v>19</v>
@@ -7237,19 +7237,19 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" s="99" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="B146" s="100" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C146" s="48" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D146" s="110" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E146" s="111" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F146" s="49"/>
       <c r="G146" s="50" t="s">
@@ -7268,19 +7268,19 @@
     </row>
     <row r="147" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A147" s="109" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
       <c r="B147" s="108" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C147" s="48" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D147" s="110" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="E147" s="111" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="F147" s="49"/>
       <c r="G147" s="50" t="s">

</xml_diff>